<commit_message>
Niño me pago :D
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="121">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -186,12 +186,6 @@
   </si>
   <si>
     <t xml:space="preserve">                I N G R E S O S</t>
-  </si>
-  <si>
-    <t>Sra. Lety</t>
-  </si>
-  <si>
-    <t>Ingles (13-16 feb)</t>
   </si>
   <si>
     <t>Día</t>
@@ -384,6 +378,15 @@
   </si>
   <si>
     <t>Post Melisa</t>
+  </si>
+  <si>
+    <t>Inicio</t>
+  </si>
+  <si>
+    <t>Pastel :D</t>
+  </si>
+  <si>
+    <t>Beca :D</t>
   </si>
 </sst>
 </file>
@@ -1086,8 +1089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1111,7 @@
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.25">
       <c r="B1" s="56" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C1" s="57">
         <v>42955</v>
@@ -1118,7 +1121,7 @@
       <c r="T1" s="47"/>
       <c r="U1" s="47"/>
       <c r="V1" s="47" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="W1" s="47"/>
       <c r="X1" s="47"/>
@@ -1177,98 +1180,98 @@
         <v>11</v>
       </c>
       <c r="T2" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="U2" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="V2" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="W2" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="U2" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="V2" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="W2" s="42" t="s">
+      <c r="X2" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z2" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA2" s="46" t="s">
         <v>58</v>
-      </c>
-      <c r="X2" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y2" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z2" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA2" s="46" t="s">
-        <v>60</v>
       </c>
       <c r="AB2" s="65" t="s">
         <v>10</v>
       </c>
       <c r="AC2" s="38" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AD2" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE2" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF2" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="AE2" s="36" t="s">
+      <c r="AG2" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="AF2" s="36" t="s">
+      <c r="AH2" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="AG2" s="36" t="s">
+      <c r="AI2" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="AH2" s="36" t="s">
+      <c r="AJ2" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="AI2" s="36" t="s">
+      <c r="AK2" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="AJ2" s="36" t="s">
+      <c r="AL2" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="AK2" s="36" t="s">
+      <c r="AM2" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="AL2" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="AM2" s="36" t="s">
-        <v>70</v>
-      </c>
       <c r="AN2" s="71" t="s">
+        <v>101</v>
+      </c>
+      <c r="AO2" s="72" t="s">
+        <v>102</v>
+      </c>
+      <c r="AP2" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="AO2" s="72" t="s">
+      <c r="AQ2" s="72" t="s">
         <v>104</v>
       </c>
-      <c r="AP2" s="72" t="s">
+      <c r="AR2" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="AQ2" s="72" t="s">
+      <c r="AS2" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="AR2" s="72" t="s">
+      <c r="AT2" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="AS2" s="72" t="s">
+      <c r="AU2" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="AT2" s="72" t="s">
+      <c r="AV2" s="72" t="s">
         <v>109</v>
-      </c>
-      <c r="AU2" s="73" t="s">
-        <v>110</v>
-      </c>
-      <c r="AV2" s="72" t="s">
-        <v>111</v>
       </c>
       <c r="AX2" s="8"/>
       <c r="AY2" s="74" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="AZ2" s="74" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="BA2" s="8"/>
     </row>
@@ -1280,7 +1283,7 @@
       </c>
       <c r="L3" s="27">
         <f>(SUM(C2,(E11:E500),(K11:K501)))-(SUM((D11:D500),(C11:C500)))</f>
-        <v>13000</v>
+        <v>13600</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -1288,10 +1291,10 @@
         <v>42955</v>
       </c>
       <c r="T3" s="51" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="U3" s="52" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="V3" s="44">
         <f>(SUM(W3,X3))-Z3</f>
@@ -1311,7 +1314,7 @@
         <v>50</v>
       </c>
       <c r="AB3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AN3">
         <f t="shared" ref="AN3:AN66" si="1">SUM(AO3,AV3,AU3)</f>
@@ -1357,7 +1360,7 @@
         <v>42956</v>
       </c>
       <c r="T4" s="51" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="U4" s="52"/>
       <c r="V4" s="44">
@@ -1384,7 +1387,7 @@
       </c>
       <c r="AX4" s="62"/>
       <c r="AY4" s="62" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="AZ4" s="62">
         <f>(SUM((AO3:AO519)))-(SUM((AS3:AS519)))</f>
@@ -1413,7 +1416,7 @@
         <v>42957</v>
       </c>
       <c r="T5" s="51" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="U5" s="52"/>
       <c r="V5" s="44">
@@ -1452,7 +1455,8 @@
         <v>9</v>
       </c>
       <c r="L6" s="55">
-        <v>250</v>
+        <f>(SUM(Q11:Q300))-(SUM(E11:E200))</f>
+        <v>1050</v>
       </c>
       <c r="M6" s="32"/>
       <c r="N6" s="32"/>
@@ -1460,7 +1464,7 @@
         <v>42958</v>
       </c>
       <c r="T6" s="51" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="U6" s="76"/>
       <c r="V6" s="44">
@@ -1502,7 +1506,7 @@
         <v>42959</v>
       </c>
       <c r="T7" s="51" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="U7" s="52"/>
       <c r="V7" s="44">
@@ -1533,7 +1537,7 @@
         <v>42960</v>
       </c>
       <c r="T8" s="51" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="U8" s="52"/>
       <c r="V8" s="44">
@@ -1578,7 +1582,7 @@
       </c>
       <c r="L9" s="15">
         <f>SUM(L11:L501)</f>
-        <v>20800</v>
+        <v>20200</v>
       </c>
       <c r="N9" s="35" t="s">
         <v>53</v>
@@ -1590,7 +1594,7 @@
         <v>42961</v>
       </c>
       <c r="T9" s="51" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="U9" s="52"/>
       <c r="V9" s="44">
@@ -1667,7 +1671,7 @@
         <v>42962</v>
       </c>
       <c r="T10" s="51" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="U10" s="52"/>
       <c r="V10" s="44">
@@ -1714,23 +1718,19 @@
         <f t="shared" ref="L11:L75" si="5">J11-K11</f>
         <v>5000</v>
       </c>
-      <c r="N11" s="39">
-        <v>42782</v>
-      </c>
+      <c r="N11" s="39"/>
       <c r="O11" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="P11" s="38" t="s">
-        <v>55</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="P11" s="38"/>
       <c r="Q11" s="40">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="S11" s="50">
         <v>42963</v>
       </c>
       <c r="T11" s="51" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="U11" s="52"/>
       <c r="V11" s="44">
@@ -1774,15 +1774,23 @@
         <f t="shared" si="5"/>
         <v>2500</v>
       </c>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="40"/>
+      <c r="N12" s="39">
+        <v>42956</v>
+      </c>
+      <c r="O12" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="P12" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q12" s="40">
+        <v>600</v>
+      </c>
       <c r="S12" s="50">
         <v>42964</v>
       </c>
       <c r="T12" s="51" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="U12" s="52"/>
       <c r="V12" s="44">
@@ -1829,17 +1837,25 @@
       </c>
       <c r="M13">
         <f>SUM((L13:L22),L33)</f>
-        <v>4660</v>
-      </c>
-      <c r="N13" s="38"/>
-      <c r="O13" s="38"/>
-      <c r="P13" s="38"/>
-      <c r="Q13" s="40"/>
+        <v>4860</v>
+      </c>
+      <c r="N13" s="39">
+        <v>42956</v>
+      </c>
+      <c r="O13" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="P13" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q13" s="40">
+        <v>200</v>
+      </c>
       <c r="S13" s="50">
         <v>42965</v>
       </c>
       <c r="T13" s="51" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="U13" s="52"/>
       <c r="V13" s="44">
@@ -1893,7 +1909,7 @@
         <v>42966</v>
       </c>
       <c r="T14" s="51" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="U14" s="52"/>
       <c r="V14" s="44">
@@ -1928,15 +1944,15 @@
         <v>24</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J15" s="24">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="K15" s="23"/>
       <c r="L15" s="21">
         <f t="shared" si="5"/>
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="N15" s="38"/>
       <c r="O15" s="38"/>
@@ -1946,7 +1962,7 @@
         <v>42967</v>
       </c>
       <c r="T15" s="51" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="U15" s="76"/>
       <c r="V15" s="44">
@@ -2000,7 +2016,7 @@
         <v>42968</v>
       </c>
       <c r="T16" s="51" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="U16" s="52"/>
       <c r="V16" s="44">
@@ -2054,7 +2070,7 @@
         <v>42969</v>
       </c>
       <c r="T17" s="51" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="U17" s="52"/>
       <c r="V17" s="44">
@@ -2109,7 +2125,7 @@
         <v>42970</v>
       </c>
       <c r="T18" s="51" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="U18" s="52"/>
       <c r="V18" s="80">
@@ -2162,7 +2178,7 @@
         <v>42971</v>
       </c>
       <c r="T19" s="51" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="U19" s="52"/>
       <c r="V19" s="44">
@@ -2217,7 +2233,7 @@
         <v>42972</v>
       </c>
       <c r="T20" s="51" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="U20" s="52"/>
       <c r="V20" s="44">
@@ -2272,7 +2288,7 @@
         <v>42973</v>
       </c>
       <c r="T21" s="51" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="U21" s="52"/>
       <c r="V21" s="44">
@@ -2304,9 +2320,7 @@
       <c r="C22" s="13"/>
       <c r="D22" s="12"/>
       <c r="E22" s="14"/>
-      <c r="G22" s="62" t="s">
-        <v>31</v>
-      </c>
+      <c r="G22" s="19"/>
       <c r="H22" s="19" t="s">
         <v>24</v>
       </c>
@@ -2329,7 +2343,7 @@
         <v>42974</v>
       </c>
       <c r="T22" s="51" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="U22" s="52"/>
       <c r="V22" s="44">
@@ -2360,7 +2374,7 @@
       <c r="D23" s="12"/>
       <c r="E23" s="14"/>
       <c r="G23" s="62" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H23" s="62" t="s">
         <v>26</v>
@@ -2385,7 +2399,7 @@
         <v>42975</v>
       </c>
       <c r="T23" s="51" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="U23" s="52"/>
       <c r="V23" s="44">
@@ -2416,8 +2430,8 @@
       <c r="C24" s="13"/>
       <c r="D24" s="12"/>
       <c r="E24" s="14"/>
-      <c r="G24" s="69" t="s">
-        <v>30</v>
+      <c r="G24" s="62" t="s">
+        <v>32</v>
       </c>
       <c r="H24" s="62" t="s">
         <v>27</v>
@@ -2442,7 +2456,7 @@
         <v>42976</v>
       </c>
       <c r="T24" s="51" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="U24" s="52"/>
       <c r="V24" s="44">
@@ -2474,8 +2488,8 @@
       <c r="C25" s="13"/>
       <c r="D25" s="12"/>
       <c r="E25" s="14"/>
-      <c r="G25" s="62" t="s">
-        <v>33</v>
+      <c r="G25" s="69" t="s">
+        <v>30</v>
       </c>
       <c r="H25" s="62" t="s">
         <v>29</v>
@@ -2499,7 +2513,7 @@
         <v>42977</v>
       </c>
       <c r="T25" s="51" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="U25" s="52"/>
       <c r="V25" s="44">
@@ -2531,7 +2545,7 @@
       <c r="D26" s="12"/>
       <c r="E26" s="14"/>
       <c r="G26" s="62" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="H26" s="62" t="s">
         <v>29</v>
@@ -2554,7 +2568,7 @@
         <v>42978</v>
       </c>
       <c r="T26" s="51" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="U26" s="52"/>
       <c r="V26" s="44">
@@ -2617,14 +2631,14 @@
       <c r="C27" s="13"/>
       <c r="D27" s="12"/>
       <c r="E27" s="14"/>
-      <c r="G27" s="61">
-        <v>42789</v>
+      <c r="G27" s="62" t="s">
+        <v>75</v>
       </c>
       <c r="H27" s="62" t="s">
         <v>28</v>
       </c>
       <c r="I27" s="62" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J27" s="64">
         <v>80</v>
@@ -2691,13 +2705,13 @@
       <c r="D28" s="12"/>
       <c r="E28" s="14"/>
       <c r="G28" s="61">
-        <v>42794</v>
+        <v>42789</v>
       </c>
       <c r="H28" s="62" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I28" s="62" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J28" s="64">
         <v>100</v>
@@ -2762,14 +2776,14 @@
       <c r="C29" s="13"/>
       <c r="D29" s="12"/>
       <c r="E29" s="14"/>
-      <c r="G29" s="66">
-        <v>42802</v>
+      <c r="G29" s="61">
+        <v>42794</v>
       </c>
       <c r="H29" s="62" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I29" s="63" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J29" s="64">
         <v>10</v>
@@ -2841,10 +2855,10 @@
         <v>42802</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J30" s="24">
         <v>140</v>
@@ -2911,12 +2925,14 @@
       <c r="C31" s="13"/>
       <c r="D31" s="12"/>
       <c r="E31" s="14"/>
-      <c r="G31" s="62"/>
+      <c r="G31" s="66">
+        <v>42802</v>
+      </c>
       <c r="H31" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="I31" s="19" t="s">
         <v>83</v>
-      </c>
-      <c r="I31" s="19" t="s">
-        <v>85</v>
       </c>
       <c r="J31" s="24">
         <v>200</v>
@@ -2984,12 +3000,12 @@
       <c r="C32" s="13"/>
       <c r="D32" s="12"/>
       <c r="E32" s="14"/>
-      <c r="G32" s="19"/>
+      <c r="G32" s="62"/>
       <c r="H32" s="62" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I32" s="62" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J32" s="64">
         <v>160</v>
@@ -3062,7 +3078,7 @@
         <v>24</v>
       </c>
       <c r="I33" s="19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J33" s="24">
         <v>300</v>
@@ -3130,10 +3146,10 @@
       <c r="E34" s="14"/>
       <c r="G34" s="19"/>
       <c r="H34" s="19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I34" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J34" s="24">
         <v>1000</v>
@@ -3201,10 +3217,10 @@
       <c r="E35" s="14"/>
       <c r="G35" s="19"/>
       <c r="H35" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I35" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J35" s="24">
         <v>100</v>
@@ -3270,20 +3286,19 @@
       <c r="C36" s="13"/>
       <c r="D36" s="12"/>
       <c r="E36" s="14"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="I36" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="J36" s="24">
+      <c r="G36" s="62"/>
+      <c r="H36" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="I36" s="62" t="s">
+        <v>91</v>
+      </c>
+      <c r="J36" s="64">
         <v>200</v>
       </c>
-      <c r="K36" s="23"/>
-      <c r="L36" s="21">
-        <f t="shared" si="5"/>
-        <v>200</v>
+      <c r="K36" s="67"/>
+      <c r="L36" s="68">
+        <v>0</v>
       </c>
       <c r="N36" s="38"/>
       <c r="O36" s="38"/>
@@ -3343,18 +3358,19 @@
       <c r="E37" s="14"/>
       <c r="G37" s="19"/>
       <c r="H37" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I37" s="19" t="s">
         <v>94</v>
-      </c>
-      <c r="I37" s="19" t="s">
-        <v>96</v>
       </c>
       <c r="J37" s="24">
         <v>1800</v>
       </c>
-      <c r="K37" s="23"/>
+      <c r="K37" s="23">
+        <v>600</v>
+      </c>
       <c r="L37" s="21">
-        <f t="shared" si="5"/>
-        <v>1800</v>
+        <v>1200</v>
       </c>
       <c r="N37" s="38"/>
       <c r="O37" s="38"/>
@@ -3414,10 +3430,10 @@
       <c r="E38" s="14"/>
       <c r="G38" s="19"/>
       <c r="H38" s="19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I38" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J38" s="24">
         <v>2200</v>
@@ -3485,10 +3501,10 @@
       <c r="E39" s="14"/>
       <c r="G39" s="19"/>
       <c r="H39" s="19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I39" s="19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J39" s="24">
         <v>3000</v>

</xml_diff>

<commit_message>
Gastos Cafe Jarocho Sol
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="132">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -416,7 +416,10 @@
     <t>Tacos</t>
   </si>
   <si>
-    <t>Chocolates</t>
+    <t>Jueves super social (Juancho, Edgar, Laura, Sol y Ele)</t>
+  </si>
+  <si>
+    <t>Chocolates, Café Jarocho y Panque</t>
   </si>
 </sst>
 </file>
@@ -1161,7 +1164,7 @@
   <dimension ref="A1:BB963"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,7 +1432,7 @@
       </c>
       <c r="N4" s="89">
         <f>SUM(L3,L9,N7)</f>
-        <v>35312</v>
+        <v>35261.5</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -1510,10 +1513,12 @@
       <c r="U5" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="V5" s="51"/>
+      <c r="V5" s="51" t="s">
+        <v>130</v>
+      </c>
       <c r="W5" s="43">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>-48.5</v>
       </c>
       <c r="X5" s="52">
         <v>70</v>
@@ -1521,7 +1526,7 @@
       <c r="Y5" s="52"/>
       <c r="AA5" s="53">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>118.5</v>
       </c>
       <c r="AB5">
         <v>50</v>
@@ -1530,25 +1535,34 @@
         <v>129</v>
       </c>
       <c r="AD5" s="59" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AE5" s="59">
         <v>12</v>
       </c>
+      <c r="AF5">
+        <v>20.5</v>
+      </c>
+      <c r="AG5">
+        <v>14</v>
+      </c>
       <c r="AO5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="AT5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AU5">
+        <v>2</v>
+      </c>
       <c r="AV5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AW5" s="83">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AY5" s="61"/>
       <c r="AZ5" s="61"/>
@@ -1563,7 +1577,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>452</v>
+        <v>401.5</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -1618,7 +1632,7 @@
       </c>
       <c r="N7" s="88">
         <f>SUM(P7,L6)</f>
-        <v>4852</v>
+        <v>4801.5</v>
       </c>
       <c r="O7" s="85"/>
       <c r="P7" s="84">

</xml_diff>

<commit_message>
Mañana perdida en el banco
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="150">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -468,6 +468,12 @@
   </si>
   <si>
     <t>Maiz; Chocolate</t>
+  </si>
+  <si>
+    <t>Deposito y BancaNet</t>
+  </si>
+  <si>
+    <t>BancaNEt</t>
   </si>
 </sst>
 </file>
@@ -1211,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,7 +1285,7 @@
         <v>17</v>
       </c>
       <c r="C2" s="58">
-        <v>13000</v>
+        <v>12667</v>
       </c>
       <c r="D2" s="55"/>
       <c r="I2" s="6" t="s">
@@ -1406,7 +1412,7 @@
       </c>
       <c r="L3" s="26">
         <f>(SUM(C2,(E11:E500)))-(SUM((D11:D500),(C11:C500)))</f>
-        <v>13000</v>
+        <v>17667</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -1480,7 +1486,7 @@
       </c>
       <c r="N4" s="89">
         <f>SUM(L3,L9,N7)</f>
-        <v>34935.5</v>
+        <v>34660</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -1528,7 +1534,7 @@
       </c>
       <c r="BA4" s="61">
         <f>(SUM((AP3:AP519)))-(SUM((AT3:AT519)))</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="BB4" s="61"/>
     </row>
@@ -1625,7 +1631,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>75.5</v>
+        <v>133</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -1701,12 +1707,12 @@
       </c>
       <c r="N7" s="88">
         <f>SUM(P7,L6)</f>
-        <v>5475.5</v>
+        <v>533</v>
       </c>
       <c r="O7" s="85"/>
       <c r="P7" s="84">
         <f>(SUM(R11:R499))-(SUM(E11:E500))</f>
-        <v>5400</v>
+        <v>400</v>
       </c>
       <c r="Q7" s="59"/>
       <c r="R7" s="59"/>
@@ -1999,8 +2005,15 @@
       </c>
     </row>
     <row r="11" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="E11" s="40"/>
+      <c r="A11" s="33">
+        <v>42964</v>
+      </c>
+      <c r="B11" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" s="83">
+        <v>5000</v>
+      </c>
       <c r="G11" s="18" t="s">
         <v>22</v>
       </c>
@@ -2067,9 +2080,12 @@
         <f t="shared" si="1"/>
         <v>12.5</v>
       </c>
+      <c r="AS11">
+        <v>1</v>
+      </c>
       <c r="AT11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AV11">
         <f t="shared" si="4"/>
@@ -2116,20 +2132,24 @@
       <c r="U12" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="V12" s="51"/>
+      <c r="V12" s="51" t="s">
+        <v>149</v>
+      </c>
       <c r="W12" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X12" s="52"/>
+        <v>57.5</v>
+      </c>
+      <c r="X12" s="52">
+        <v>70</v>
+      </c>
       <c r="Y12" s="76"/>
       <c r="AA12" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="AO12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="AT12">
         <f t="shared" si="2"/>
@@ -2138,6 +2158,9 @@
       <c r="AV12">
         <f t="shared" si="4"/>
         <v>0</v>
+      </c>
+      <c r="AW12">
+        <v>12.5</v>
       </c>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Viernes en la mañanaiwi
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -1248,8 +1248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="N4" s="88">
         <f>SUM(L3,L9,N7)</f>
-        <v>34707</v>
+        <v>34753.5</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -1662,7 +1662,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>180</v>
+        <v>226.5</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -1738,7 +1738,7 @@
       </c>
       <c r="N7" s="87">
         <f>SUM(P7,L6)</f>
-        <v>580</v>
+        <v>626.5</v>
       </c>
       <c r="O7" s="84"/>
       <c r="P7" s="83">
@@ -2167,8 +2167,8 @@
         <v>149</v>
       </c>
       <c r="W12" s="43">
-        <f t="shared" si="3"/>
-        <v>104.5</v>
+        <f>(SUM(X12,Y12))-AA12</f>
+        <v>93.5</v>
       </c>
       <c r="X12" s="52">
         <v>70</v>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="AA12" s="53">
         <f t="shared" si="0"/>
-        <v>92.5</v>
+        <v>103.5</v>
       </c>
       <c r="AB12">
         <v>70</v>
@@ -2197,18 +2197,21 @@
       </c>
       <c r="AO12">
         <f t="shared" si="1"/>
-        <v>12.5</v>
+        <v>23.5</v>
       </c>
       <c r="AT12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AU12">
+        <v>1</v>
+      </c>
       <c r="AV12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AW12">
-        <v>12.5</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.25">
@@ -2260,18 +2263,20 @@
       </c>
       <c r="V13" s="51"/>
       <c r="W13" s="43">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X13" s="52"/>
+        <f>(SUM(X13,Y13))-AA13</f>
+        <v>57.5</v>
+      </c>
+      <c r="X13" s="52">
+        <v>70</v>
+      </c>
       <c r="Y13" s="52"/>
       <c r="AA13" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="AO13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="AT13">
         <f t="shared" si="2"/>
@@ -2281,6 +2286,9 @@
       <c r="AV13">
         <f t="shared" si="4"/>
         <v>0</v>
+      </c>
+      <c r="AW13">
+        <v>12.5</v>
       </c>
     </row>
     <row r="14" spans="1:54" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cuentas del Fin de Semana
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="161">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -484,6 +484,30 @@
   <si>
     <t>Maíz</t>
   </si>
+  <si>
+    <t>Gnomo</t>
+  </si>
+  <si>
+    <t>Juancho-Piel Morena</t>
+  </si>
+  <si>
+    <t>Helados y Nachos</t>
+  </si>
+  <si>
+    <t>Retiro pa Audifonos Centro</t>
+  </si>
+  <si>
+    <t>Inundacion Jaime</t>
+  </si>
+  <si>
+    <t>Café Juancho</t>
+  </si>
+  <si>
+    <t>Tarjeta, PoetistaInterrumpidoMetro, Audifonos y Gomitas</t>
+  </si>
+  <si>
+    <t>Jaime Cargador Atlalilco</t>
+  </si>
 </sst>
 </file>
 
@@ -795,7 +819,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -908,7 +932,6 @@
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1248,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,7 +1338,7 @@
       <c r="B2" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="93">
+      <c r="C2" s="92">
         <v>12667</v>
       </c>
       <c r="D2" s="55"/>
@@ -1443,7 +1466,7 @@
       </c>
       <c r="L3" s="26">
         <f>(SUM(C2,(E11:E500)))-(SUM((D11:D500),(C11:C500)))</f>
-        <v>17667</v>
+        <v>17367</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -1512,12 +1535,12 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="30"/>
-      <c r="M4" s="86" t="s">
+      <c r="M4" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="88">
+      <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>34753.5</v>
+        <v>34351.5</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -1646,7 +1669,7 @@
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="AW5" s="82">
+      <c r="AW5" s="81">
         <v>12</v>
       </c>
       <c r="AY5" s="60"/>
@@ -1662,12 +1685,12 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>226.5</v>
+        <v>124.5</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
-      <c r="O6" s="84"/>
-      <c r="P6" s="84" t="s">
+      <c r="O6" s="83"/>
+      <c r="P6" s="83" t="s">
         <v>117</v>
       </c>
       <c r="Q6" s="58"/>
@@ -1678,7 +1701,7 @@
       <c r="U6" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="V6" s="81" t="s">
+      <c r="V6" s="80" t="s">
         <v>132</v>
       </c>
       <c r="W6" s="43">
@@ -1696,7 +1719,7 @@
       <c r="AB6">
         <v>0</v>
       </c>
-      <c r="AC6" s="82" t="s">
+      <c r="AC6" s="81" t="s">
         <v>133</v>
       </c>
       <c r="AD6" t="s">
@@ -1733,15 +1756,15 @@
       <c r="J7" s="31"/>
       <c r="K7" s="31"/>
       <c r="L7" s="31"/>
-      <c r="M7" s="85" t="s">
+      <c r="M7" s="84" t="s">
         <v>118</v>
       </c>
-      <c r="N7" s="87">
+      <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>626.5</v>
-      </c>
-      <c r="O7" s="84"/>
-      <c r="P7" s="83">
+        <v>524.5</v>
+      </c>
+      <c r="O7" s="83"/>
+      <c r="P7" s="82">
         <f>(SUM(R11:R499))-(SUM(E11:E500))</f>
         <v>400</v>
       </c>
@@ -1771,7 +1794,7 @@
       <c r="AB7">
         <v>170</v>
       </c>
-      <c r="AC7" s="82" t="s">
+      <c r="AC7" s="81" t="s">
         <v>136</v>
       </c>
       <c r="AD7" t="s">
@@ -1816,7 +1839,7 @@
       <c r="X8" s="52">
         <v>250</v>
       </c>
-      <c r="Y8" s="75"/>
+      <c r="Y8" s="74"/>
       <c r="AA8" s="53">
         <f t="shared" si="0"/>
         <v>258</v>
@@ -1824,7 +1847,7 @@
       <c r="AB8">
         <v>0</v>
       </c>
-      <c r="AC8" s="82" t="s">
+      <c r="AC8" s="81" t="s">
         <v>139</v>
       </c>
       <c r="AD8" t="s">
@@ -1910,7 +1933,7 @@
       <c r="AB9">
         <v>50</v>
       </c>
-      <c r="AC9" s="82" t="s">
+      <c r="AC9" s="81" t="s">
         <v>141</v>
       </c>
       <c r="AD9" t="s">
@@ -1985,7 +2008,7 @@
       <c r="Q10" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="R10" s="89" t="s">
+      <c r="R10" s="88" t="s">
         <v>124</v>
       </c>
       <c r="T10" s="49">
@@ -2012,7 +2035,7 @@
       <c r="AB10">
         <v>60</v>
       </c>
-      <c r="AC10" s="82" t="s">
+      <c r="AC10" s="81" t="s">
         <v>116</v>
       </c>
       <c r="AI10" s="18"/>
@@ -2042,7 +2065,7 @@
       <c r="B11" t="s">
         <v>148</v>
       </c>
-      <c r="E11" s="82">
+      <c r="E11" s="81">
         <v>5000</v>
       </c>
       <c r="G11" s="18" t="s">
@@ -2095,7 +2118,7 @@
       <c r="AB11">
         <v>50</v>
       </c>
-      <c r="AC11" s="82" t="s">
+      <c r="AC11" s="81" t="s">
         <v>129</v>
       </c>
       <c r="AD11" t="s">
@@ -2127,6 +2150,15 @@
       </c>
     </row>
     <row r="12" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A12" s="33">
+        <v>42966</v>
+      </c>
+      <c r="B12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12">
+        <v>300</v>
+      </c>
       <c r="G12" s="18" t="s">
         <v>30</v>
       </c>
@@ -2173,7 +2205,7 @@
       <c r="X12" s="52">
         <v>70</v>
       </c>
-      <c r="Y12" s="92">
+      <c r="Y12" s="91">
         <v>127</v>
       </c>
       <c r="Z12" t="s">
@@ -2186,7 +2218,7 @@
       <c r="AB12">
         <v>70</v>
       </c>
-      <c r="AC12" s="82" t="s">
+      <c r="AC12" s="81" t="s">
         <v>150</v>
       </c>
       <c r="AD12" t="s">
@@ -2233,7 +2265,7 @@
         <f t="shared" si="5"/>
         <v>1100</v>
       </c>
-      <c r="M13" s="90">
+      <c r="M13" s="89">
         <f>SUM((L13:L23))</f>
         <v>5120</v>
       </c>
@@ -2246,7 +2278,7 @@
       <c r="P13" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="Q13" s="91">
+      <c r="Q13" s="90">
         <v>3800</v>
       </c>
       <c r="R13" s="39">
@@ -2261,10 +2293,12 @@
       <c r="U13" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="V13" s="51"/>
+      <c r="V13" s="51" t="s">
+        <v>157</v>
+      </c>
       <c r="W13" s="43">
         <f>(SUM(X13,Y13))-AA13</f>
-        <v>57.5</v>
+        <v>-161.5</v>
       </c>
       <c r="X13" s="52">
         <v>70</v>
@@ -2272,20 +2306,40 @@
       <c r="Y13" s="52"/>
       <c r="AA13" s="53">
         <f t="shared" si="0"/>
-        <v>12.5</v>
+        <v>231.5</v>
+      </c>
+      <c r="AB13">
+        <v>150</v>
+      </c>
+      <c r="AC13" s="81" t="s">
+        <v>153</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>155</v>
+      </c>
+      <c r="AE13">
+        <v>19</v>
+      </c>
+      <c r="AF13">
+        <v>19</v>
+      </c>
+      <c r="AG13">
+        <v>16</v>
       </c>
       <c r="AO13">
         <f t="shared" si="1"/>
-        <v>12.5</v>
+        <v>27.5</v>
       </c>
       <c r="AT13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AU13" s="76"/>
+      <c r="AU13" s="75">
+        <v>3</v>
+      </c>
       <c r="AV13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AW13">
         <v>12.5</v>
@@ -2331,28 +2385,62 @@
       <c r="U14" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="V14" s="51"/>
+      <c r="V14" s="51" t="s">
+        <v>158</v>
+      </c>
       <c r="W14" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-173</v>
       </c>
       <c r="X14" s="52"/>
-      <c r="Y14" s="52"/>
+      <c r="Y14" s="52">
+        <v>250</v>
+      </c>
       <c r="AA14" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>423</v>
+      </c>
+      <c r="AB14">
+        <v>200</v>
+      </c>
+      <c r="AC14" s="81" t="s">
+        <v>154</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>159</v>
+      </c>
+      <c r="AE14">
+        <v>10</v>
+      </c>
+      <c r="AF14">
+        <v>160</v>
+      </c>
+      <c r="AG14">
+        <v>20</v>
+      </c>
+      <c r="AH14">
+        <v>4</v>
       </c>
       <c r="AO14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="AP14">
+        <v>20</v>
+      </c>
+      <c r="AS14">
+        <v>4</v>
       </c>
       <c r="AT14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AV14">
         <f t="shared" si="4"/>
         <v>0</v>
+      </c>
+      <c r="AW14">
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.25">
@@ -2393,29 +2481,37 @@
       <c r="U15" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="V15" s="74"/>
+      <c r="V15" s="80" t="s">
+        <v>160</v>
+      </c>
       <c r="W15" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="X15" s="52"/>
       <c r="Y15" s="52"/>
       <c r="AA15" s="53">
         <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="AB15">
         <v>0</v>
       </c>
       <c r="AF15" s="18"/>
       <c r="AO15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AT15">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AU15">
+        <v>2</v>
+      </c>
       <c r="AV15">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:54" x14ac:dyDescent="0.25">
@@ -2455,7 +2551,7 @@
       </c>
       <c r="X16" s="52"/>
       <c r="Y16" s="52"/>
-      <c r="AA16" s="77">
+      <c r="AA16" s="76">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2509,7 +2605,7 @@
         <v>0</v>
       </c>
       <c r="X17" s="52"/>
-      <c r="Y17" s="75"/>
+      <c r="Y17" s="74"/>
       <c r="AA17" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2560,7 +2656,7 @@
         <v>96</v>
       </c>
       <c r="V18" s="51"/>
-      <c r="W18" s="78">
+      <c r="W18" s="77">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2731,7 +2827,7 @@
         <v>0</v>
       </c>
       <c r="X21" s="52"/>
-      <c r="Y21" s="79"/>
+      <c r="Y21" s="78"/>
       <c r="AA21" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2786,8 +2882,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X22" s="75"/>
-      <c r="Y22" s="75"/>
+      <c r="X22" s="74"/>
+      <c r="Y22" s="74"/>
       <c r="AA22" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2904,7 +3000,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AF24" s="80"/>
+      <c r="AF24" s="79"/>
       <c r="AO24">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2963,7 +3059,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AH25" s="80"/>
+      <c r="AH25" s="79"/>
       <c r="AO25">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3241,7 +3337,7 @@
       <c r="T29" s="49"/>
       <c r="U29" s="50"/>
       <c r="V29" s="51"/>
-      <c r="W29" s="78">
+      <c r="W29" s="77">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3361,7 +3457,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AP30" s="80"/>
+      <c r="AP30" s="79"/>
     </row>
     <row r="31" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C31" s="13"/>
@@ -3478,7 +3574,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB32" s="80"/>
+      <c r="AB32" s="79"/>
       <c r="AE32">
         <v>0</v>
       </c>
@@ -4301,7 +4397,7 @@
       <c r="R44" s="39"/>
       <c r="T44" s="49"/>
       <c r="U44" s="50"/>
-      <c r="V44" s="81"/>
+      <c r="V44" s="80"/>
       <c r="W44" s="43">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4312,7 +4408,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AC44" s="82"/>
+      <c r="AC44" s="81"/>
       <c r="AE44">
         <v>0</v>
       </c>
@@ -4381,7 +4477,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AC45" s="82"/>
+      <c r="AC45" s="81"/>
       <c r="AE45">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Gastos de inicio de semana
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="163">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -507,6 +507,12 @@
   </si>
   <si>
     <t>Jaime Cargador Atlalilco</t>
+  </si>
+  <si>
+    <t>Camila!</t>
+  </si>
+  <si>
+    <t>Chocolate; Café</t>
   </si>
 </sst>
 </file>
@@ -1271,8 +1277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1540,7 +1546,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>34351.5</v>
+        <v>34345.5</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -1588,7 +1594,7 @@
       </c>
       <c r="BA4" s="60">
         <f>(SUM((AP3:AP519)))-(SUM((AT3:AT519)))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="BB4" s="60"/>
     </row>
@@ -1685,7 +1691,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>124.5</v>
+        <v>118.5</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -1761,7 +1767,7 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>524.5</v>
+        <v>518.5</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
@@ -2544,28 +2550,61 @@
       <c r="U16" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="V16" s="51"/>
+      <c r="V16" s="51" t="s">
+        <v>161</v>
+      </c>
       <c r="W16" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X16" s="52"/>
+        <v>-6</v>
+      </c>
+      <c r="X16" s="52">
+        <v>120</v>
+      </c>
       <c r="Y16" s="52"/>
       <c r="AA16" s="76">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AE16" s="18"/>
+        <v>126</v>
+      </c>
+      <c r="AB16">
+        <v>60</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>162</v>
+      </c>
+      <c r="AE16" s="18">
+        <v>6</v>
+      </c>
+      <c r="AF16">
+        <v>30</v>
+      </c>
       <c r="AO16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="AP16">
+        <v>30</v>
+      </c>
+      <c r="AQ16">
+        <v>2</v>
+      </c>
+      <c r="AS16">
+        <v>1</v>
       </c>
       <c r="AT16">
         <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="AU16">
         <v>0</v>
       </c>
       <c r="AV16">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AW16">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Gastos Martes 22 agosto
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="165">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -513,6 +513,12 @@
   </si>
   <si>
     <t>Chocolate; Café</t>
+  </si>
+  <si>
+    <t>PruebaE</t>
+  </si>
+  <si>
+    <t>Prueba E</t>
   </si>
 </sst>
 </file>
@@ -1277,8 +1283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="BB17" sqref="BB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1546,7 +1552,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>34345.5</v>
+        <v>34277</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -1691,7 +1697,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>118.5</v>
+        <v>50</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -1767,7 +1773,7 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>518.5</v>
+        <v>450</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
@@ -2638,22 +2644,37 @@
       <c r="U17" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="V17" s="51"/>
+      <c r="V17" s="51" t="s">
+        <v>164</v>
+      </c>
       <c r="W17" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X17" s="52"/>
+        <v>-68.5</v>
+      </c>
+      <c r="X17" s="52">
+        <v>70</v>
+      </c>
       <c r="Y17" s="74"/>
       <c r="AA17" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AD17" s="40"/>
+        <v>138.5</v>
+      </c>
+      <c r="AB17">
+        <v>50</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>150</v>
+      </c>
+      <c r="AD17" s="81" t="s">
+        <v>163</v>
+      </c>
+      <c r="AE17">
+        <v>76</v>
+      </c>
       <c r="AL17" s="40"/>
       <c r="AO17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="AT17">
         <f>(AQ17*8)+(AS17*5)</f>
@@ -2662,6 +2683,9 @@
       <c r="AV17">
         <f t="shared" si="4"/>
         <v>0</v>
+      </c>
+      <c r="AW17">
+        <v>12.5</v>
       </c>
     </row>
     <row r="18" spans="3:54" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cuentas salida con Edgar
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="169">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -524,10 +524,13 @@
     <t>Edgar</t>
   </si>
   <si>
-    <t>Cheetos</t>
+    <t>Pa salir con Edgar</t>
   </si>
   <si>
-    <t>Pa salir con Edgar</t>
+    <t>Croissant</t>
+  </si>
+  <si>
+    <t>Cheetos, Malteada Oreo</t>
   </si>
 </sst>
 </file>
@@ -1292,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="O14" workbookViewId="0">
+      <selection activeCell="Y36" sqref="Y36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,7 +1564,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>34326.5</v>
+        <v>34205.5</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -1706,7 +1709,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>299.5</v>
+        <v>178.5</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -1782,7 +1785,7 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>499.5</v>
+        <v>378.5</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
@@ -2557,7 +2560,7 @@
       <c r="N16" s="37"/>
       <c r="O16" s="37"/>
       <c r="P16" s="37" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q16" s="39"/>
       <c r="R16" s="39">
@@ -2736,7 +2739,7 @@
       </c>
       <c r="W18" s="77">
         <f t="shared" si="3"/>
-        <v>49.5</v>
+        <v>-71.5</v>
       </c>
       <c r="X18" s="52">
         <v>70</v>
@@ -2744,28 +2747,40 @@
       <c r="Y18" s="52"/>
       <c r="AA18" s="53">
         <f t="shared" si="0"/>
-        <v>20.5</v>
+        <v>141.5</v>
+      </c>
+      <c r="AB18">
+        <v>45</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>167</v>
       </c>
       <c r="AD18" s="81" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="AE18">
         <v>8</v>
       </c>
+      <c r="AF18">
+        <v>50</v>
+      </c>
       <c r="AO18">
         <f t="shared" si="1"/>
-        <v>12.5</v>
+        <v>38.5</v>
       </c>
       <c r="AT18">
         <f>(AQ18*8)+(AS18*5)</f>
         <v>0</v>
       </c>
+      <c r="AU18">
+        <v>4</v>
+      </c>
       <c r="AV18">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AW18">
-        <v>12.5</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="19" spans="3:54" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Gastos dia del cafe de Juancho
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Tesis_AdrianaFelCha\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="171">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -531,6 +531,12 @@
   </si>
   <si>
     <t>Cheetos, Malteada Oreo</t>
+  </si>
+  <si>
+    <t>Ingles Maraton</t>
+  </si>
+  <si>
+    <t>Copias, Tamborcito</t>
   </si>
 </sst>
 </file>
@@ -1295,8 +1301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O14" workbookViewId="0">
-      <selection activeCell="Y36" sqref="Y36"/>
+    <sheetView tabSelected="1" topLeftCell="AM2" workbookViewId="0">
+      <selection activeCell="AS20" sqref="AS20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,7 +1570,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>34205.5</v>
+        <v>34164.5</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -1612,7 +1618,7 @@
       </c>
       <c r="BA4" s="60">
         <f>(SUM((AP3:AP519)))-(SUM((AT3:AT519)))</f>
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="BB4" s="60"/>
     </row>
@@ -1709,7 +1715,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>178.5</v>
+        <v>137.5</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -1785,7 +1791,7 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>378.5</v>
+        <v>337.5</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
@@ -2813,25 +2819,55 @@
       <c r="U19" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="V19" s="51"/>
+      <c r="V19" s="51" t="s">
+        <v>169</v>
+      </c>
       <c r="W19" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X19" s="52"/>
+        <v>-41</v>
+      </c>
+      <c r="X19" s="52">
+        <v>70</v>
+      </c>
       <c r="Y19" s="52"/>
       <c r="AA19" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>111</v>
+      </c>
+      <c r="AB19">
+        <v>68</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>158</v>
+      </c>
+      <c r="AD19" s="81" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF19">
+        <v>11</v>
+      </c>
+      <c r="AG19">
+        <v>2</v>
       </c>
       <c r="AO19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AP19" s="40"/>
+        <v>30</v>
+      </c>
+      <c r="AP19" s="40">
+        <v>30</v>
+      </c>
+      <c r="AQ19">
+        <v>2</v>
+      </c>
+      <c r="AS19">
+        <v>1</v>
+      </c>
       <c r="AT19" s="5">
         <f>(AQ19*8)+(AS19*5)</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="AV19">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
Me cai en una coladeraaaaa
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="186">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -567,6 +567,21 @@
   </si>
   <si>
     <t>Ginecologa SARI</t>
+  </si>
+  <si>
+    <t>Mariscos - Caldo</t>
+  </si>
+  <si>
+    <t>Revision Tesis Jaime</t>
+  </si>
+  <si>
+    <t>Coladera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Casa </t>
+  </si>
+  <si>
+    <t>Chocolate, Maíz</t>
   </si>
 </sst>
 </file>
@@ -1342,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AA23" sqref="AA23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,7 +1626,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>34059</v>
+        <v>34042.5</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -1659,7 +1674,7 @@
       </c>
       <c r="BA4" s="60">
         <f>(SUM((AP3:AP519)))-(SUM((AT3:AT519)))</f>
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="BB4" s="60"/>
     </row>
@@ -1756,7 +1771,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>232</v>
+        <v>215.5</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -1832,7 +1847,7 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>232</v>
+        <v>215.5</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
@@ -3123,16 +3138,26 @@
       <c r="U22" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="V22" s="51"/>
+      <c r="V22" s="51" t="s">
+        <v>182</v>
+      </c>
       <c r="W22" s="43">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X22" s="74"/>
+      <c r="X22" s="74">
+        <v>0</v>
+      </c>
       <c r="Y22" s="74"/>
       <c r="AA22" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="AB22">
+        <v>0</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>184</v>
       </c>
       <c r="AO22">
         <f t="shared" si="1"/>
@@ -3177,29 +3202,56 @@
       <c r="U23" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="V23" s="51"/>
+      <c r="V23" s="51" t="s">
+        <v>183</v>
+      </c>
       <c r="W23" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X23" s="52"/>
+        <v>-16.5</v>
+      </c>
+      <c r="X23" s="52">
+        <v>130</v>
+      </c>
       <c r="Y23" s="52"/>
       <c r="AA23" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AF23" s="40"/>
+        <v>146.5</v>
+      </c>
+      <c r="AB23">
+        <v>70</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>181</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>185</v>
+      </c>
+      <c r="AE23">
+        <v>10</v>
+      </c>
+      <c r="AF23" s="40">
+        <v>4</v>
+      </c>
       <c r="AO23" s="40">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>62.5</v>
+      </c>
+      <c r="AP23">
+        <v>50</v>
+      </c>
+      <c r="AS23">
+        <v>2</v>
       </c>
       <c r="AT23">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AV23">
         <f t="shared" si="4"/>
         <v>0</v>
+      </c>
+      <c r="AW23">
+        <v>12.5</v>
       </c>
     </row>
     <row r="24" spans="3:54" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finanzas miercoles pre comida
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="189">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -586,6 +585,12 @@
   </si>
   <si>
     <t>Azucar</t>
+  </si>
+  <si>
+    <t>Café Ale</t>
+  </si>
+  <si>
+    <t>Sol instrumento</t>
   </si>
 </sst>
 </file>
@@ -1362,7 +1367,7 @@
   <dimension ref="A1:BB963"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AC24" sqref="AC24"/>
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,7 +1635,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>34066</v>
+        <v>34073.5</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -1678,7 +1683,7 @@
       </c>
       <c r="BA4" s="60">
         <f>(SUM((AP3:AP519)))-(SUM((AT3:AT519)))</f>
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="BB4" s="60"/>
     </row>
@@ -1775,7 +1780,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>239</v>
+        <v>246.5</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -1851,7 +1856,7 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>239</v>
+        <v>246.5</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
@@ -3291,7 +3296,9 @@
       <c r="U24" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="V24" s="51"/>
+      <c r="V24" s="51" t="s">
+        <v>188</v>
+      </c>
       <c r="W24" s="43">
         <f t="shared" si="3"/>
         <v>23.5</v>
@@ -3322,9 +3329,12 @@
         <v>12.5</v>
       </c>
       <c r="AQ24" s="40"/>
+      <c r="AS24">
+        <v>2</v>
+      </c>
       <c r="AT24">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AV24">
         <f t="shared" si="4"/>
@@ -3367,21 +3377,31 @@
       <c r="U25" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="V25" s="51"/>
+      <c r="V25" s="51" t="s">
+        <v>187</v>
+      </c>
       <c r="W25" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X25" s="52"/>
+        <v>7.5</v>
+      </c>
+      <c r="X25" s="52">
+        <v>30</v>
+      </c>
       <c r="Y25" s="52"/>
       <c r="AA25" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>22.5</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>152</v>
+      </c>
+      <c r="AE25">
+        <v>10</v>
       </c>
       <c r="AH25" s="79"/>
       <c r="AO25">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="AT25">
         <f t="shared" si="6"/>
@@ -3390,6 +3410,9 @@
       <c r="AV25">
         <f t="shared" si="4"/>
         <v>0</v>
+      </c>
+      <c r="AW25">
+        <v>12.5</v>
       </c>
     </row>
     <row r="26" spans="3:54" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Completando el registro de la semana Sin Tesis
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="213">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -660,6 +660,9 @@
   </si>
   <si>
     <t>Copias</t>
+  </si>
+  <si>
+    <t>Netflix</t>
   </si>
 </sst>
 </file>
@@ -1451,8 +1454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T19" workbookViewId="0">
-      <selection activeCell="AD30" sqref="AD30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,7 +1649,7 @@
       </c>
       <c r="L3" s="26">
         <f>(SUM(C2,(E11:E500)))-(SUM((D11:D500),(C11:C500)))</f>
-        <v>16888.45</v>
+        <v>16881.259999999998</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -1720,7 +1723,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>34070</v>
+        <v>33698.06</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -1865,7 +1868,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>552</v>
+        <v>712.80000000000018</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -1941,12 +1944,12 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>552</v>
+        <v>342.80000000000018</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
         <f>(SUM(R11:R499))-(SUM(E11:E500))</f>
-        <v>0</v>
+        <v>-370</v>
       </c>
       <c r="Q7" s="58"/>
       <c r="R7" s="58"/>
@@ -2080,7 +2083,7 @@
       </c>
       <c r="L9" s="15">
         <f>SUM(L11:L501)</f>
-        <v>16629.55</v>
+        <v>16474</v>
       </c>
       <c r="N9" s="34" t="s">
         <v>51</v>
@@ -2542,7 +2545,7 @@
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="12">
-        <v>209</v>
+        <v>211.44</v>
       </c>
       <c r="E14" s="14"/>
       <c r="G14" s="18"/>
@@ -2640,9 +2643,15 @@
       </c>
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="C15" s="13"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="14"/>
+      <c r="A15" s="33">
+        <v>42983</v>
+      </c>
+      <c r="B15" t="s">
+        <v>212</v>
+      </c>
+      <c r="C15">
+        <v>160.80000000000001</v>
+      </c>
       <c r="G15" s="18"/>
       <c r="H15" s="18" t="s">
         <v>24</v>
@@ -2711,9 +2720,17 @@
       </c>
     </row>
     <row r="16" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="C16" s="13"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="14"/>
+      <c r="A16" s="93">
+        <v>42987</v>
+      </c>
+      <c r="B16" s="94" t="s">
+        <v>176</v>
+      </c>
+      <c r="C16" s="94"/>
+      <c r="D16" s="94">
+        <v>213.95</v>
+      </c>
+      <c r="E16" s="94"/>
       <c r="G16" s="18"/>
       <c r="H16" s="18" t="s">
         <v>24</v>
@@ -2802,10 +2819,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:54" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A17" s="33">
+        <v>42987</v>
+      </c>
       <c r="C17" s="13"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="14"/>
+      <c r="E17" s="14">
+        <v>370</v>
+      </c>
       <c r="G17" s="18"/>
       <c r="H17" s="18" t="s">
         <v>24</v>
@@ -2884,7 +2906,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="18" spans="3:54" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:54" x14ac:dyDescent="0.25">
       <c r="C18" s="13"/>
       <c r="D18" s="12"/>
       <c r="E18" s="14"/>
@@ -2969,7 +2991,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="19" spans="3:54" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:54" x14ac:dyDescent="0.25">
       <c r="C19" s="13"/>
       <c r="D19" s="12"/>
       <c r="E19" s="14"/>
@@ -3066,7 +3088,7 @@
       </c>
       <c r="BB19" s="40"/>
     </row>
-    <row r="20" spans="3:54" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" x14ac:dyDescent="0.25">
       <c r="C20" s="13"/>
       <c r="D20" s="12"/>
       <c r="E20" s="14"/>
@@ -3149,7 +3171,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="21" spans="3:54" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:54" x14ac:dyDescent="0.25">
       <c r="C21" s="13"/>
       <c r="D21" s="12"/>
       <c r="E21" s="14"/>
@@ -3226,7 +3248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="3:54" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:54" x14ac:dyDescent="0.25">
       <c r="C22" s="13"/>
       <c r="D22" s="12"/>
       <c r="E22" s="14"/>
@@ -3290,7 +3312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:54" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:54" x14ac:dyDescent="0.25">
       <c r="C23" s="13"/>
       <c r="D23" s="12"/>
       <c r="E23" s="14"/>
@@ -3372,7 +3394,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="24" spans="3:54" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:54" x14ac:dyDescent="0.25">
       <c r="C24" s="13"/>
       <c r="D24" s="12"/>
       <c r="E24" s="14"/>
@@ -3453,7 +3475,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="25" spans="3:54" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:54" x14ac:dyDescent="0.25">
       <c r="C25" s="13"/>
       <c r="D25" s="12"/>
       <c r="E25" s="14"/>
@@ -3533,7 +3555,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="26" spans="3:54" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:54" x14ac:dyDescent="0.25">
       <c r="C26" s="13"/>
       <c r="D26" s="12"/>
       <c r="E26" s="14"/>
@@ -3638,7 +3660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="3:54" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:54" x14ac:dyDescent="0.25">
       <c r="C27" s="13"/>
       <c r="D27" s="12"/>
       <c r="E27" s="14"/>
@@ -3739,7 +3761,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="28" spans="3:54" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:54" x14ac:dyDescent="0.25">
       <c r="C28" s="13"/>
       <c r="D28" s="12"/>
       <c r="E28" s="14"/>
@@ -3837,7 +3859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="3:54" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:54" x14ac:dyDescent="0.25">
       <c r="C29" s="13"/>
       <c r="D29" s="12"/>
       <c r="E29" s="14"/>
@@ -3943,7 +3965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="3:54" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:54" x14ac:dyDescent="0.25">
       <c r="C30" s="13"/>
       <c r="D30" s="12"/>
       <c r="E30" s="14"/>
@@ -4053,7 +4075,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="3:54" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:54" x14ac:dyDescent="0.25">
       <c r="C31" s="13"/>
       <c r="D31" s="12"/>
       <c r="E31" s="14"/>
@@ -4159,7 +4181,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="3:54" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:54" x14ac:dyDescent="0.25">
       <c r="C32" s="13"/>
       <c r="D32" s="12"/>
       <c r="E32" s="14"/>
@@ -4845,10 +4867,11 @@
       <c r="J39" s="23">
         <v>269.55</v>
       </c>
-      <c r="K39" s="22"/>
+      <c r="K39" s="22">
+        <v>270</v>
+      </c>
       <c r="L39" s="20">
-        <f t="shared" si="7"/>
-        <v>269.55</v>
+        <v>0</v>
       </c>
       <c r="N39" s="37"/>
       <c r="O39" s="37"/>
@@ -4917,14 +4940,24 @@
       <c r="C40" s="13"/>
       <c r="D40" s="12"/>
       <c r="E40" s="14"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="23"/>
-      <c r="K40" s="22"/>
+      <c r="G40" s="64">
+        <v>42987</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I40" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="J40" s="23">
+        <v>214</v>
+      </c>
+      <c r="K40" s="22">
+        <v>100</v>
+      </c>
       <c r="L40" s="20">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="N40" s="37"/>
       <c r="O40" s="37"/>
@@ -16699,7 +16732,7 @@
         <v>0</v>
       </c>
       <c r="AV197">
-        <f t="shared" ref="AV196:AV259" si="24">AU197*5</f>
+        <f t="shared" ref="AV197:AV259" si="24">AU197*5</f>
         <v>0</v>
       </c>
     </row>
@@ -19729,7 +19762,7 @@
         <v>0</v>
       </c>
       <c r="AT238">
-        <f t="shared" ref="AT213:AT276" si="27">(AQ238*6)+(AR238*8)+(AS238*5)</f>
+        <f t="shared" ref="AT238:AT276" si="27">(AQ238*6)+(AR238*8)+(AS238*5)</f>
         <v>0</v>
       </c>
       <c r="AV238">

</xml_diff>

<commit_message>
Gastos lunes y prestamo Juancho
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="218">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -664,12 +664,27 @@
   <si>
     <t>Netflix</t>
   </si>
+  <si>
+    <t>Prestamo Juancho</t>
+  </si>
+  <si>
+    <t>Pa' reparar su lap</t>
+  </si>
+  <si>
+    <t>Papá Tomas</t>
+  </si>
+  <si>
+    <t>Videollamada Uri</t>
+  </si>
+  <si>
+    <t>Papá pagando Ubers</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -795,6 +810,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="8" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -994,7 +1017,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1158,6 +1181,7 @@
     <xf numFmtId="0" fontId="17" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1455,7 +1479,7 @@
   <dimension ref="A1:BB963"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1649,7 +1673,7 @@
       </c>
       <c r="L3" s="26">
         <f>(SUM(C2,(E11:E500)))-(SUM((D11:D500),(C11:C500)))</f>
-        <v>16881.259999999998</v>
+        <v>15881.26</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -1723,7 +1747,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>33698.06</v>
+        <v>34805.560000000005</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -1868,7 +1892,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>712.80000000000018</v>
+        <v>1820.3000000000002</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -1944,7 +1968,7 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>342.80000000000018</v>
+        <v>1450.3000000000002</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
@@ -2083,7 +2107,7 @@
       </c>
       <c r="L9" s="15">
         <f>SUM(L11:L501)</f>
-        <v>16474</v>
+        <v>17474</v>
       </c>
       <c r="N9" s="34" t="s">
         <v>51</v>
@@ -2823,7 +2847,10 @@
       <c r="A17" s="33">
         <v>42987</v>
       </c>
-      <c r="C17" s="13"/>
+      <c r="B17" t="s">
+        <v>217</v>
+      </c>
+      <c r="C17" s="99"/>
       <c r="D17" s="12"/>
       <c r="E17" s="14">
         <v>370</v>
@@ -2907,7 +2934,15 @@
       </c>
     </row>
     <row r="18" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="C18" s="13"/>
+      <c r="A18" s="33">
+        <v>42989</v>
+      </c>
+      <c r="B18" t="s">
+        <v>213</v>
+      </c>
+      <c r="C18" s="13">
+        <v>1000</v>
+      </c>
       <c r="D18" s="12"/>
       <c r="E18" s="14"/>
       <c r="G18" s="18"/>
@@ -4283,7 +4318,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="3:50" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C33" s="13"/>
       <c r="D33" s="12"/>
       <c r="E33" s="14"/>
@@ -4393,7 +4428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="3:50" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C34" s="13"/>
       <c r="D34" s="12"/>
       <c r="E34" s="14"/>
@@ -4493,7 +4528,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="3:50" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C35" s="13"/>
       <c r="D35" s="12"/>
       <c r="E35" s="14"/>
@@ -4600,7 +4635,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="3:50" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C36" s="13"/>
       <c r="D36" s="12"/>
       <c r="E36" s="14"/>
@@ -4629,7 +4664,9 @@
       <c r="U36" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="V36" s="51"/>
+      <c r="V36" s="51" t="s">
+        <v>215</v>
+      </c>
       <c r="W36" s="43">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4683,7 +4720,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:50" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A37" s="40"/>
       <c r="C37" s="13"/>
       <c r="D37" s="12"/>
       <c r="E37" s="14"/>
@@ -4712,17 +4750,26 @@
       <c r="T37" s="49">
         <v>42989</v>
       </c>
-      <c r="U37" s="50"/>
-      <c r="V37" s="51"/>
+      <c r="U37" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="V37" s="51" t="s">
+        <v>216</v>
+      </c>
       <c r="W37" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X37" s="52"/>
+        <v>107.5</v>
+      </c>
+      <c r="X37" s="52">
+        <v>120</v>
+      </c>
       <c r="Y37" s="52"/>
       <c r="AA37" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12.5</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>141</v>
       </c>
       <c r="AE37">
         <v>0</v>
@@ -4756,7 +4803,7 @@
       </c>
       <c r="AO37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="AT37">
         <f t="shared" si="6"/>
@@ -4766,8 +4813,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="3:50" x14ac:dyDescent="0.25">
+      <c r="AW37">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C38" s="13"/>
       <c r="D38" s="12"/>
       <c r="E38" s="14"/>
@@ -4851,7 +4901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:50" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C39" s="13"/>
       <c r="D39" s="12"/>
       <c r="E39" s="14"/>
@@ -4936,7 +4986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:50" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C40" s="13"/>
       <c r="D40" s="12"/>
       <c r="E40" s="14"/>
@@ -5022,18 +5072,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="3:50" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C41" s="13"/>
       <c r="D41" s="12"/>
       <c r="E41" s="14"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="23"/>
+      <c r="G41" s="64">
+        <v>42989</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="I41" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="J41" s="23">
+        <v>1000</v>
+      </c>
       <c r="K41" s="22"/>
       <c r="L41" s="20">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="N41" s="37"/>
       <c r="O41" s="37"/>
@@ -5098,7 +5156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="3:50" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C42" s="13"/>
       <c r="D42" s="12"/>
       <c r="E42" s="14"/>
@@ -5174,7 +5232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:50" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C43" s="13"/>
       <c r="D43" s="12"/>
       <c r="E43" s="14"/>
@@ -5251,7 +5309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="3:50" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C44" s="13"/>
       <c r="D44" s="12"/>
       <c r="E44" s="14"/>
@@ -5330,7 +5388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:50" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C45" s="13"/>
       <c r="D45" s="12"/>
       <c r="E45" s="14"/>
@@ -5408,7 +5466,7 @@
       </c>
       <c r="AX45" s="40"/>
     </row>
-    <row r="46" spans="3:50" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C46" s="13"/>
       <c r="D46" s="12"/>
       <c r="E46" s="14"/>
@@ -5484,7 +5542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="3:50" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C47" s="13"/>
       <c r="D47" s="12"/>
       <c r="E47" s="14"/>
@@ -5560,7 +5618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:50" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C48" s="13"/>
       <c r="D48" s="12"/>
       <c r="E48" s="14"/>

</xml_diff>

<commit_message>
Ajustando cuentas - Faltan 130 pesos
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="225">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -688,6 +688,18 @@
   <si>
     <t>Emiliano 1</t>
   </si>
+  <si>
+    <t>Sra. Julia</t>
+  </si>
+  <si>
+    <t>Ingles Emiliano</t>
+  </si>
+  <si>
+    <t>Copas y Señor Metro</t>
+  </si>
+  <si>
+    <t>Guardando</t>
+  </si>
 </sst>
 </file>
 
@@ -832,7 +844,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="31">
+  <fills count="30">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1004,12 +1016,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1187,10 +1193,10 @@
     <xf numFmtId="0" fontId="6" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1487,9 +1493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V37" sqref="V37"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1756,7 +1760,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>35193.060000000005</v>
+        <v>35083.560000000005</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -1901,7 +1905,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>1837.8000000000002</v>
+        <v>1228.3000000000002</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -1977,12 +1981,12 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>1837.8000000000002</v>
+        <v>1728.3000000000002</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
         <f>(SUM(R11:R499))-(SUM(E11:E500))</f>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="Q7" s="58"/>
       <c r="R7" s="58"/>
@@ -2859,7 +2863,7 @@
       <c r="B17" t="s">
         <v>217</v>
       </c>
-      <c r="C17" s="99"/>
+      <c r="C17" s="98"/>
       <c r="D17" s="12"/>
       <c r="E17" s="14">
         <v>370</v>
@@ -3321,10 +3325,18 @@
         <f t="shared" si="5"/>
         <v>100</v>
       </c>
-      <c r="N22" s="38"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="37"/>
-      <c r="Q22" s="39"/>
+      <c r="N22" s="38">
+        <v>42989</v>
+      </c>
+      <c r="O22" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="P22" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q22" s="39">
+        <v>100</v>
+      </c>
       <c r="R22" s="39"/>
       <c r="T22" s="49">
         <v>42974</v>
@@ -3385,11 +3397,18 @@
         <f t="shared" si="5"/>
         <v>300</v>
       </c>
-      <c r="N23" s="37"/>
+      <c r="N23" s="38">
+        <v>42990</v>
+      </c>
       <c r="O23" s="37"/>
-      <c r="P23" s="37"/>
+      <c r="P23" s="37" t="s">
+        <v>224</v>
+      </c>
       <c r="Q23" s="39"/>
-      <c r="R23" s="39"/>
+      <c r="R23" s="39">
+        <v>500</v>
+      </c>
+      <c r="S23" s="81"/>
       <c r="T23" s="49">
         <v>42975</v>
       </c>
@@ -3949,17 +3968,12 @@
       </c>
       <c r="W29" s="77">
         <f t="shared" si="3"/>
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="X29" s="52">
         <v>0</v>
       </c>
-      <c r="Y29" s="98">
-        <v>130</v>
-      </c>
-      <c r="Z29" t="s">
-        <v>151</v>
-      </c>
+      <c r="Y29" s="99"/>
       <c r="AA29" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4879,7 +4893,7 @@
       </c>
       <c r="W38" s="43">
         <f t="shared" si="3"/>
-        <v>67.5</v>
+        <v>-12</v>
       </c>
       <c r="X38" s="52">
         <v>80</v>
@@ -4887,13 +4901,22 @@
       <c r="Y38" s="52"/>
       <c r="AA38" s="53">
         <f t="shared" si="0"/>
-        <v>12.5</v>
+        <v>92</v>
+      </c>
+      <c r="AB38">
+        <v>70</v>
+      </c>
+      <c r="AC38" t="s">
+        <v>150</v>
+      </c>
+      <c r="AD38" t="s">
+        <v>223</v>
       </c>
       <c r="AE38">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="AF38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG38">
         <v>0</v>

</xml_diff>

<commit_message>
Gastos domingo y lunes
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="235">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -720,6 +720,15 @@
   </si>
   <si>
     <t>Sushi</t>
+  </si>
+  <si>
+    <t>Estudios</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>Dia Libre Jaime</t>
   </si>
 </sst>
 </file>
@@ -1523,8 +1532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="AM16" workbookViewId="0">
+      <selection activeCell="AP20" sqref="AP20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1792,7 +1801,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>34004.82</v>
+        <v>34112.32</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -1937,7 +1946,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>150</v>
+        <v>757.5</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -2013,12 +2022,12 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>650</v>
+        <v>757.5</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
         <f>(SUM(R11:R499))-(SUM(E11:E500))</f>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="58"/>
       <c r="R7" s="58"/>
@@ -3521,11 +3530,17 @@
       <c r="L24" s="66">
         <v>0</v>
       </c>
-      <c r="N24" s="37"/>
+      <c r="N24" s="38">
+        <v>42996</v>
+      </c>
       <c r="O24" s="37"/>
-      <c r="P24" s="37"/>
+      <c r="P24" s="37" t="s">
+        <v>232</v>
+      </c>
       <c r="Q24" s="39"/>
-      <c r="R24" s="39"/>
+      <c r="R24" s="39">
+        <v>-500</v>
+      </c>
       <c r="T24" s="49">
         <v>42976</v>
       </c>
@@ -5419,12 +5434,16 @@
       <c r="U43" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="V43" s="51"/>
+      <c r="V43" s="51" t="s">
+        <v>233</v>
+      </c>
       <c r="W43" s="43">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X43" s="52"/>
+      <c r="X43" s="52">
+        <v>0</v>
+      </c>
       <c r="Y43" s="52"/>
       <c r="AA43" s="53">
         <f t="shared" si="0"/>
@@ -5498,16 +5517,20 @@
       <c r="U44" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="V44" s="80"/>
+      <c r="V44" s="80" t="s">
+        <v>234</v>
+      </c>
       <c r="W44" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X44" s="52"/>
+        <v>107.5</v>
+      </c>
+      <c r="X44" s="52">
+        <v>120</v>
+      </c>
       <c r="Y44" s="52"/>
       <c r="AA44" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="AC44" s="81"/>
       <c r="AE44">
@@ -5542,7 +5565,7 @@
       </c>
       <c r="AO44">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="AP44" s="12"/>
       <c r="AQ44" s="12"/>
@@ -5553,6 +5576,9 @@
       <c r="AV44">
         <f t="shared" si="4"/>
         <v>0</v>
+      </c>
+      <c r="AW44">
+        <v>12.5</v>
       </c>
     </row>
     <row r="45" spans="1:50" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cuentas de la semana sin UNAM
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="255">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -737,10 +737,58 @@
     <t>Cervezas;Bubulubus; Estudios</t>
   </si>
   <si>
-    <t>Emiliano y Sra Letty</t>
+    <t xml:space="preserve">Mamá - Desayuno tía </t>
   </si>
   <si>
-    <t xml:space="preserve">Mamá - Desayuno tía </t>
+    <t>Sra Julia</t>
+  </si>
+  <si>
+    <t>Pago desayuno</t>
+  </si>
+  <si>
+    <t>Temblor</t>
+  </si>
+  <si>
+    <t>Post Temblor</t>
+  </si>
+  <si>
+    <t>La palma</t>
+  </si>
+  <si>
+    <t>Caldo mamá</t>
+  </si>
+  <si>
+    <t>Medicinas;Limosnero</t>
+  </si>
+  <si>
+    <t>Sanborns Jaime</t>
+  </si>
+  <si>
+    <t>Clases Inglés</t>
+  </si>
+  <si>
+    <t>Capacitacion fallida Fac</t>
+  </si>
+  <si>
+    <t>Copias; mamá Taxi</t>
+  </si>
+  <si>
+    <t>Bubulubu</t>
+  </si>
+  <si>
+    <t>Buffette China</t>
+  </si>
+  <si>
+    <t>Regreso al lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Propina Café Beto;Agua </t>
+  </si>
+  <si>
+    <t>Majo</t>
+  </si>
+  <si>
+    <t>MaskDeMasque</t>
   </si>
 </sst>
 </file>
@@ -1544,8 +1592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1739,7 +1787,7 @@
       </c>
       <c r="L3" s="26">
         <f>(SUM(C2,(E11:E500)))-(SUM((D11:D500),(C11:C500)))</f>
-        <v>15880.82</v>
+        <v>15765.82</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -1813,7 +1861,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>33687.32</v>
+        <v>34261.82</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -1958,7 +2006,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>132.5</v>
+        <v>22</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -2034,12 +2082,12 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>132.5</v>
+        <v>1022</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
         <f>(SUM(R11:R499))-(SUM(E11:E500))</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="Q7" s="58"/>
       <c r="R7" s="58"/>
@@ -2173,7 +2221,7 @@
       </c>
       <c r="L9" s="15">
         <f>SUM(L11:L501)</f>
-        <v>17674</v>
+        <v>17474</v>
       </c>
       <c r="N9" s="34" t="s">
         <v>51</v>
@@ -3093,8 +3141,16 @@
       </c>
     </row>
     <row r="19" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A19" s="33">
+        <v>43001</v>
+      </c>
+      <c r="B19" t="s">
+        <v>245</v>
+      </c>
       <c r="C19" s="13"/>
-      <c r="D19" s="12"/>
+      <c r="D19" s="12">
+        <v>115</v>
+      </c>
       <c r="E19" s="14"/>
       <c r="G19" s="18"/>
       <c r="H19" s="18" t="s">
@@ -3629,10 +3685,18 @@
       <c r="L25" s="66">
         <v>0</v>
       </c>
-      <c r="N25" s="37"/>
-      <c r="O25" s="37"/>
-      <c r="P25" s="37"/>
-      <c r="Q25" s="39"/>
+      <c r="N25" s="38">
+        <v>42998</v>
+      </c>
+      <c r="O25" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="P25" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q25" s="39">
+        <v>200</v>
+      </c>
       <c r="R25" s="39"/>
       <c r="T25" s="49">
         <v>42977</v>
@@ -3708,11 +3772,21 @@
       <c r="L26" s="66">
         <v>0</v>
       </c>
-      <c r="N26" s="37"/>
-      <c r="O26" s="37"/>
-      <c r="P26" s="37"/>
-      <c r="Q26" s="39"/>
-      <c r="R26" s="39"/>
+      <c r="N26" s="38">
+        <v>42998</v>
+      </c>
+      <c r="O26" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="P26" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q26" s="39">
+        <v>200</v>
+      </c>
+      <c r="R26" s="39">
+        <v>200</v>
+      </c>
       <c r="T26" s="49">
         <v>42978</v>
       </c>
@@ -3812,10 +3886,16 @@
       <c r="L27" s="66">
         <v>0</v>
       </c>
-      <c r="N27" s="37"/>
-      <c r="O27" s="37"/>
+      <c r="N27" s="38">
+        <v>43000</v>
+      </c>
+      <c r="O27" s="37" t="s">
+        <v>170</v>
+      </c>
       <c r="P27" s="37"/>
-      <c r="Q27" s="39"/>
+      <c r="Q27" s="39">
+        <v>650</v>
+      </c>
       <c r="R27" s="39"/>
       <c r="T27" s="49">
         <v>42979</v>
@@ -3913,10 +3993,16 @@
       <c r="L28" s="66">
         <v>0</v>
       </c>
-      <c r="N28" s="37"/>
-      <c r="O28" s="37"/>
+      <c r="N28" s="38">
+        <v>43000</v>
+      </c>
+      <c r="O28" s="37" t="s">
+        <v>238</v>
+      </c>
       <c r="P28" s="37"/>
-      <c r="Q28" s="39"/>
+      <c r="Q28" s="39">
+        <v>60</v>
+      </c>
       <c r="R28" s="39"/>
       <c r="T28" s="49">
         <v>42980</v>
@@ -4011,11 +4097,15 @@
       <c r="L29" s="66">
         <v>0</v>
       </c>
-      <c r="N29" s="37"/>
+      <c r="N29" s="38">
+        <v>43003</v>
+      </c>
       <c r="O29" s="37"/>
       <c r="P29" s="37"/>
       <c r="Q29" s="39"/>
-      <c r="R29" s="39"/>
+      <c r="R29" s="39">
+        <v>800</v>
+      </c>
       <c r="T29" s="49">
         <v>42981</v>
       </c>
@@ -5027,22 +5117,22 @@
       <c r="C39" s="13"/>
       <c r="D39" s="12"/>
       <c r="E39" s="14"/>
-      <c r="G39" s="64">
+      <c r="G39" s="59">
         <v>42973</v>
       </c>
-      <c r="H39" s="18" t="s">
+      <c r="H39" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="I39" s="18" t="s">
+      <c r="I39" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="J39" s="23">
+      <c r="J39" s="62">
         <v>269.55</v>
       </c>
-      <c r="K39" s="22">
+      <c r="K39" s="65">
         <v>270</v>
       </c>
-      <c r="L39" s="20">
+      <c r="L39" s="66">
         <v>0</v>
       </c>
       <c r="N39" s="37"/>
@@ -5335,22 +5425,24 @@
       <c r="C42" s="13"/>
       <c r="D42" s="12"/>
       <c r="E42" s="14"/>
-      <c r="G42" s="64">
+      <c r="G42" s="59">
         <v>42997</v>
       </c>
-      <c r="H42" s="18" t="s">
+      <c r="H42" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="I42" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="J42" s="23">
+      <c r="I42" s="60" t="s">
+        <v>237</v>
+      </c>
+      <c r="J42" s="62">
         <v>200</v>
       </c>
-      <c r="K42" s="22"/>
-      <c r="L42" s="20">
+      <c r="K42" s="65">
+        <v>200</v>
+      </c>
+      <c r="L42" s="66">
         <f t="shared" si="7"/>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="N42" s="37"/>
       <c r="O42" s="37"/>
@@ -5639,11 +5731,11 @@
         <v>91</v>
       </c>
       <c r="V45" s="51" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="W45" s="43">
         <f t="shared" si="3"/>
-        <v>-110</v>
+        <v>-199</v>
       </c>
       <c r="X45" s="52">
         <v>80</v>
@@ -5653,9 +5745,14 @@
       </c>
       <c r="AA45" s="53">
         <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="AC45" s="81"/>
+        <v>289</v>
+      </c>
+      <c r="AB45">
+        <v>70</v>
+      </c>
+      <c r="AC45" s="81" t="s">
+        <v>242</v>
+      </c>
       <c r="AE45" s="12">
         <v>200</v>
       </c>
@@ -5688,7 +5785,7 @@
       </c>
       <c r="AO45">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AT45">
         <f t="shared" si="6"/>
@@ -5697,6 +5794,9 @@
       <c r="AV45">
         <f t="shared" si="4"/>
         <v>0</v>
+      </c>
+      <c r="AW45">
+        <v>19</v>
       </c>
       <c r="AX45" s="40"/>
     </row>
@@ -5724,22 +5824,35 @@
       <c r="U46" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="V46" s="51"/>
+      <c r="V46" s="51" t="s">
+        <v>241</v>
+      </c>
       <c r="W46" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X46" s="52"/>
+        <v>-131</v>
+      </c>
+      <c r="X46" s="52">
+        <v>80</v>
+      </c>
       <c r="Y46" s="52"/>
       <c r="AA46" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>211</v>
+      </c>
+      <c r="AB46">
+        <v>0</v>
+      </c>
+      <c r="AC46" s="81" t="s">
+        <v>243</v>
+      </c>
+      <c r="AD46" t="s">
+        <v>244</v>
       </c>
       <c r="AE46">
-        <v>0</v>
+        <v>204</v>
       </c>
       <c r="AF46">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AG46">
         <v>0</v>
@@ -5767,7 +5880,7 @@
       </c>
       <c r="AO46">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT46">
         <f t="shared" si="6"/>
@@ -5776,6 +5889,9 @@
       <c r="AV46">
         <f t="shared" si="4"/>
         <v>0</v>
+      </c>
+      <c r="AW46">
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:50" x14ac:dyDescent="0.25">
@@ -5802,22 +5918,32 @@
       <c r="U47" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="V47" s="51"/>
+      <c r="V47" s="51" t="s">
+        <v>246</v>
+      </c>
       <c r="W47" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X47" s="52"/>
+        <v>13</v>
+      </c>
+      <c r="X47" s="52">
+        <v>50</v>
+      </c>
       <c r="Y47" s="52"/>
       <c r="AA47" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="AB47">
+        <v>0</v>
+      </c>
+      <c r="AD47" t="s">
+        <v>248</v>
       </c>
       <c r="AE47">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AF47">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AG47">
         <v>0</v>
@@ -5880,19 +6006,32 @@
       <c r="U48" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="V48" s="51"/>
+      <c r="V48" s="51" t="s">
+        <v>247</v>
+      </c>
       <c r="W48" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X48" s="52"/>
+        <v>-7.5</v>
+      </c>
+      <c r="X48" s="52">
+        <v>80</v>
+      </c>
       <c r="Y48" s="52"/>
       <c r="AA48" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>87.5</v>
+      </c>
+      <c r="AB48">
+        <v>70</v>
+      </c>
+      <c r="AC48" t="s">
+        <v>153</v>
+      </c>
+      <c r="AD48" t="s">
+        <v>249</v>
       </c>
       <c r="AE48">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AF48">
         <v>0</v>
@@ -5923,7 +6062,7 @@
       </c>
       <c r="AO48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="AT48">
         <f t="shared" si="6"/>
@@ -5933,8 +6072,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="3:48" x14ac:dyDescent="0.25">
+      <c r="AW48">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="49" spans="3:49" x14ac:dyDescent="0.25">
       <c r="C49" s="13"/>
       <c r="D49" s="12"/>
       <c r="E49" s="14"/>
@@ -5958,16 +6100,26 @@
       <c r="U49" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="V49" s="51"/>
+      <c r="V49" s="51" t="s">
+        <v>253</v>
+      </c>
       <c r="W49" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X49" s="52"/>
+        <v>-6.5</v>
+      </c>
+      <c r="X49" s="52">
+        <v>120</v>
+      </c>
       <c r="Y49" s="52"/>
       <c r="AA49" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>126.5</v>
+      </c>
+      <c r="AB49">
+        <v>120</v>
+      </c>
+      <c r="AC49" t="s">
+        <v>250</v>
       </c>
       <c r="AE49">
         <v>0</v>
@@ -6001,7 +6153,7 @@
       </c>
       <c r="AO49">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="AT49">
         <f t="shared" si="6"/>
@@ -6011,8 +6163,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="3:48" x14ac:dyDescent="0.25">
+      <c r="AW49">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="50" spans="3:49" x14ac:dyDescent="0.25">
       <c r="C50" s="13"/>
       <c r="D50" s="12"/>
       <c r="E50" s="14"/>
@@ -6036,7 +6191,9 @@
       <c r="U50" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="V50" s="51"/>
+      <c r="V50" s="51" t="s">
+        <v>254</v>
+      </c>
       <c r="W50" s="43">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -6090,7 +6247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:49" x14ac:dyDescent="0.25">
       <c r="C51" s="13"/>
       <c r="D51" s="12"/>
       <c r="E51" s="14"/>
@@ -6111,23 +6268,38 @@
       <c r="T51" s="49">
         <v>43003</v>
       </c>
-      <c r="U51" s="50"/>
-      <c r="V51" s="51"/>
+      <c r="U51" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="V51" s="51" t="s">
+        <v>251</v>
+      </c>
       <c r="W51" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X51" s="52"/>
+        <v>0.5</v>
+      </c>
+      <c r="X51" s="52">
+        <v>120</v>
+      </c>
       <c r="Y51" s="52"/>
       <c r="AA51" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>119.5</v>
+      </c>
+      <c r="AB51">
+        <v>70</v>
+      </c>
+      <c r="AC51" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD51" t="s">
+        <v>252</v>
       </c>
       <c r="AE51">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AF51">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AG51">
         <v>0</v>
@@ -6155,7 +6327,7 @@
       </c>
       <c r="AO51">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="AT51">
         <f t="shared" si="6"/>
@@ -6165,8 +6337,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="3:48" x14ac:dyDescent="0.25">
+      <c r="AW51">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="52" spans="3:49" x14ac:dyDescent="0.25">
       <c r="C52" s="13"/>
       <c r="D52" s="12"/>
       <c r="E52" s="14"/>
@@ -6187,7 +6362,9 @@
       <c r="T52" s="49">
         <v>43004</v>
       </c>
-      <c r="U52" s="50"/>
+      <c r="U52" s="50" t="s">
+        <v>91</v>
+      </c>
       <c r="V52" s="51"/>
       <c r="W52" s="43">
         <f t="shared" si="3"/>
@@ -6242,7 +6419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:49" x14ac:dyDescent="0.25">
       <c r="C53" s="13"/>
       <c r="D53" s="12"/>
       <c r="E53" s="14"/>
@@ -6263,7 +6440,9 @@
       <c r="T53" s="49">
         <v>43005</v>
       </c>
-      <c r="U53" s="50"/>
+      <c r="U53" s="50" t="s">
+        <v>96</v>
+      </c>
       <c r="V53" s="51"/>
       <c r="W53" s="43">
         <f t="shared" si="3"/>
@@ -6318,7 +6497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:49" x14ac:dyDescent="0.25">
       <c r="C54" s="13"/>
       <c r="D54" s="12"/>
       <c r="E54" s="14"/>
@@ -6339,7 +6518,9 @@
       <c r="T54" s="49">
         <v>43006</v>
       </c>
-      <c r="U54" s="50"/>
+      <c r="U54" s="50" t="s">
+        <v>55</v>
+      </c>
       <c r="V54" s="51"/>
       <c r="W54" s="43">
         <f t="shared" si="3"/>
@@ -6394,7 +6575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:49" x14ac:dyDescent="0.25">
       <c r="C55" s="13"/>
       <c r="D55" s="12"/>
       <c r="E55" s="14"/>
@@ -6415,7 +6596,9 @@
       <c r="T55" s="49">
         <v>43007</v>
       </c>
-      <c r="U55" s="50"/>
+      <c r="U55" s="50" t="s">
+        <v>92</v>
+      </c>
       <c r="V55" s="51"/>
       <c r="W55" s="43">
         <f t="shared" si="3"/>
@@ -6470,7 +6653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:49" x14ac:dyDescent="0.25">
       <c r="C56" s="13"/>
       <c r="D56" s="12"/>
       <c r="E56" s="14"/>
@@ -6491,7 +6674,9 @@
       <c r="T56" s="49">
         <v>43008</v>
       </c>
-      <c r="U56" s="50"/>
+      <c r="U56" s="50" t="s">
+        <v>93</v>
+      </c>
       <c r="V56" s="51"/>
       <c r="W56" s="43">
         <f t="shared" si="3"/>
@@ -6546,7 +6731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:49" x14ac:dyDescent="0.25">
       <c r="C57" s="13"/>
       <c r="D57" s="12"/>
       <c r="E57" s="14"/>
@@ -6567,7 +6752,9 @@
       <c r="T57" s="49">
         <v>43009</v>
       </c>
-      <c r="U57" s="50"/>
+      <c r="U57" s="50" t="s">
+        <v>94</v>
+      </c>
       <c r="V57" s="51"/>
       <c r="W57" s="43">
         <f t="shared" si="3"/>
@@ -6622,7 +6809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:49" x14ac:dyDescent="0.25">
       <c r="C58" s="13"/>
       <c r="D58" s="12"/>
       <c r="E58" s="14"/>
@@ -6698,7 +6885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:49" x14ac:dyDescent="0.25">
       <c r="C59" s="13"/>
       <c r="D59" s="12"/>
       <c r="E59" s="14"/>
@@ -6774,7 +6961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:49" x14ac:dyDescent="0.25">
       <c r="C60" s="13"/>
       <c r="D60" s="12"/>
       <c r="E60" s="14"/>
@@ -6850,7 +7037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:49" x14ac:dyDescent="0.25">
       <c r="C61" s="13"/>
       <c r="D61" s="12"/>
       <c r="E61" s="14"/>
@@ -6926,7 +7113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:49" x14ac:dyDescent="0.25">
       <c r="C62" s="13"/>
       <c r="D62" s="12"/>
       <c r="E62" s="14"/>
@@ -7002,7 +7189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:49" x14ac:dyDescent="0.25">
       <c r="C63" s="13"/>
       <c r="D63" s="12"/>
       <c r="E63" s="14"/>
@@ -7078,7 +7265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:49" x14ac:dyDescent="0.25">
       <c r="C64" s="13"/>
       <c r="D64" s="12"/>
       <c r="E64" s="14"/>

</xml_diff>

<commit_message>
Gastos y ganancias del Jueves
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="264">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -799,6 +799,24 @@
   <si>
     <t>Celular para su papá</t>
   </si>
+  <si>
+    <t>Prestamo Ale</t>
+  </si>
+  <si>
+    <t>Chocolates, Café Toks y Prestamo Ale</t>
+  </si>
+  <si>
+    <t>Ingles tarde</t>
+  </si>
+  <si>
+    <t>Copias y Tamborsito; Cambio del billete de la sra Letty</t>
+  </si>
+  <si>
+    <t>Pago Uber</t>
+  </si>
+  <si>
+    <t>Tennis</t>
+  </si>
 </sst>
 </file>
 
@@ -1137,7 +1155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1305,6 +1323,9 @@
     <xf numFmtId="0" fontId="7" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1313,8 +1334,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF33CC33"/>
       <color rgb="FFCCFFCC"/>
-      <color rgb="FF33CC33"/>
       <color rgb="FFCFCFCF"/>
       <color rgb="FFFF9797"/>
       <color rgb="FFF6F7C9"/>
@@ -1602,7 +1623,7 @@
   <dimension ref="A1:BB963"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1796,7 +1817,7 @@
       </c>
       <c r="L3" s="26">
         <f>(SUM(C2,(E11:E500)))-(SUM((D11:D500),(C11:C500)))</f>
-        <v>15765.82</v>
+        <v>11277.82</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -1870,7 +1891,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>34464.82</v>
+        <v>35225.82</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -2015,7 +2036,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>225</v>
+        <v>100</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -2091,12 +2112,12 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>1225</v>
+        <v>1600</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
         <f>(SUM(R11:R499))-(SUM(E11:E500))</f>
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="Q7" s="58"/>
       <c r="R7" s="58"/>
@@ -2230,7 +2251,7 @@
       </c>
       <c r="L9" s="15">
         <f>SUM(L11:L501)</f>
-        <v>17474</v>
+        <v>22348</v>
       </c>
       <c r="N9" s="34" t="s">
         <v>51</v>
@@ -2499,12 +2520,12 @@
         <v>43</v>
       </c>
       <c r="J12" s="23">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="K12" s="22"/>
       <c r="L12" s="20">
         <f t="shared" si="5"/>
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="N12" s="38">
         <v>42956</v>
@@ -3255,7 +3276,15 @@
       <c r="BB19" s="40"/>
     </row>
     <row r="20" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="C20" s="13"/>
+      <c r="A20" s="33">
+        <v>43005</v>
+      </c>
+      <c r="B20" t="s">
+        <v>258</v>
+      </c>
+      <c r="C20" s="13">
+        <v>3200</v>
+      </c>
       <c r="D20" s="12"/>
       <c r="E20" s="14"/>
       <c r="G20" s="18"/>
@@ -3338,8 +3367,16 @@
       </c>
     </row>
     <row r="21" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A21" s="33">
+        <v>43006</v>
+      </c>
+      <c r="B21" t="s">
+        <v>263</v>
+      </c>
       <c r="C21" s="13"/>
-      <c r="D21" s="12"/>
+      <c r="D21" s="12">
+        <v>1288</v>
+      </c>
       <c r="E21" s="14"/>
       <c r="G21" s="18"/>
       <c r="H21" s="18" t="s">
@@ -4212,7 +4249,7 @@
         <v>0</v>
       </c>
       <c r="N30" s="38">
-        <v>43005</v>
+        <v>43004</v>
       </c>
       <c r="O30" s="37" t="s">
         <v>238</v>
@@ -4328,11 +4365,19 @@
         <f>J31-K31</f>
         <v>140</v>
       </c>
-      <c r="N31" s="37"/>
-      <c r="O31" s="37"/>
+      <c r="N31" s="38">
+        <v>43006</v>
+      </c>
+      <c r="O31" s="37" t="s">
+        <v>170</v>
+      </c>
       <c r="P31" s="37"/>
-      <c r="Q31" s="39"/>
-      <c r="R31" s="39"/>
+      <c r="Q31" s="39">
+        <v>500</v>
+      </c>
+      <c r="R31" s="39">
+        <v>500</v>
+      </c>
       <c r="T31" s="49">
         <v>42983</v>
       </c>
@@ -4434,10 +4479,18 @@
         <f>J32-K32</f>
         <v>200</v>
       </c>
-      <c r="N32" s="37"/>
-      <c r="O32" s="37"/>
-      <c r="P32" s="37"/>
-      <c r="Q32" s="39"/>
+      <c r="N32" s="38">
+        <v>43006</v>
+      </c>
+      <c r="O32" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="P32" s="37" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q32" s="39">
+        <v>100</v>
+      </c>
       <c r="R32" s="39"/>
       <c r="T32" s="49">
         <v>42984</v>
@@ -5238,24 +5291,24 @@
       <c r="C40" s="13"/>
       <c r="D40" s="12"/>
       <c r="E40" s="14"/>
-      <c r="G40" s="64">
+      <c r="G40" s="59">
         <v>42987</v>
       </c>
-      <c r="H40" s="18" t="s">
+      <c r="H40" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="I40" s="18" t="s">
+      <c r="I40" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="J40" s="23">
+      <c r="J40" s="62">
         <v>214</v>
       </c>
-      <c r="K40" s="22">
-        <v>100</v>
-      </c>
-      <c r="L40" s="20">
+      <c r="K40" s="65">
+        <v>214</v>
+      </c>
+      <c r="L40" s="66">
         <f t="shared" si="7"/>
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="N40" s="37"/>
       <c r="O40" s="37"/>
@@ -5550,11 +5603,13 @@
       <c r="I43" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="J43" s="23"/>
+      <c r="J43" s="23">
+        <v>3200</v>
+      </c>
       <c r="K43" s="22"/>
       <c r="L43" s="20">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3200</v>
       </c>
       <c r="N43" s="37"/>
       <c r="O43" s="37"/>
@@ -5630,14 +5685,22 @@
       <c r="C44" s="13"/>
       <c r="D44" s="12"/>
       <c r="E44" s="14"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="23"/>
+      <c r="G44" s="64">
+        <v>43006</v>
+      </c>
+      <c r="H44" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I44" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="J44" s="23">
+        <v>1288</v>
+      </c>
       <c r="K44" s="22"/>
       <c r="L44" s="20">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1288</v>
       </c>
       <c r="N44" s="37"/>
       <c r="O44" s="37"/>
@@ -6480,18 +6543,22 @@
       <c r="U53" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="V53" s="51"/>
+      <c r="V53" s="51" t="s">
+        <v>23</v>
+      </c>
       <c r="W53" s="43">
         <f t="shared" si="3"/>
-        <v>-0.5</v>
+        <v>-3370.5</v>
       </c>
       <c r="X53" s="52">
         <v>80</v>
       </c>
-      <c r="Y53" s="52"/>
+      <c r="Y53" s="52">
+        <v>80</v>
+      </c>
       <c r="AA53" s="53">
         <f t="shared" si="0"/>
-        <v>80.5</v>
+        <v>3530.5</v>
       </c>
       <c r="AB53">
         <v>60</v>
@@ -6500,16 +6567,16 @@
         <v>116</v>
       </c>
       <c r="AD53" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="AE53">
         <v>8</v>
       </c>
       <c r="AF53">
-        <v>0</v>
-      </c>
-      <c r="AG53">
-        <v>0</v>
+        <v>250</v>
+      </c>
+      <c r="AG53" s="12">
+        <v>3200</v>
       </c>
       <c r="AH53">
         <v>0</v>
@@ -6572,22 +6639,34 @@
       <c r="U54" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="V54" s="51"/>
+      <c r="V54" s="51" t="s">
+        <v>260</v>
+      </c>
       <c r="W54" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X54" s="52"/>
-      <c r="Y54" s="52"/>
+        <v>-55</v>
+      </c>
+      <c r="X54" s="52">
+        <v>80</v>
+      </c>
+      <c r="Y54" s="101">
+        <v>21.5</v>
+      </c>
       <c r="AA54" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>156.5</v>
+      </c>
+      <c r="AB54">
+        <v>0</v>
+      </c>
+      <c r="AD54" t="s">
+        <v>261</v>
       </c>
       <c r="AE54">
-        <v>0</v>
+        <v>21.5</v>
       </c>
       <c r="AF54">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="AG54">
         <v>0</v>

</xml_diff>

<commit_message>
Gastos fin de semana
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="305">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -880,6 +880,66 @@
   <si>
     <t>No Javs</t>
   </si>
+  <si>
+    <t>TacosJaime; Chocolate</t>
+  </si>
+  <si>
+    <t>Papá pagando tennis :D</t>
+  </si>
+  <si>
+    <t>PAPIME</t>
+  </si>
+  <si>
+    <t>SINCA inscripcion</t>
+  </si>
+  <si>
+    <t>Pagando tennis</t>
+  </si>
+  <si>
+    <t>Sra Letty &amp; Julia</t>
+  </si>
+  <si>
+    <t>Bistecates</t>
+  </si>
+  <si>
+    <t>Chelas, SINCA</t>
+  </si>
+  <si>
+    <t>Agua;Copias</t>
+  </si>
+  <si>
+    <t>Estrenando ESO :D</t>
+  </si>
+  <si>
+    <t>Clases Ingles Tardeeeeee</t>
+  </si>
+  <si>
+    <t>Netflix  (Sept,2016-Oct,2017)</t>
+  </si>
+  <si>
+    <t>Oct,2017</t>
+  </si>
+  <si>
+    <t>BladeRunner Original</t>
+  </si>
+  <si>
+    <t>Sukiya</t>
+  </si>
+  <si>
+    <t>Snickers; Chela; Tarjeta; Nutrisa</t>
+  </si>
+  <si>
+    <t>Mampa</t>
+  </si>
+  <si>
+    <t>Mama</t>
+  </si>
+  <si>
+    <t>Dahlia Iris PW</t>
+  </si>
+  <si>
+    <t>Pagando Uber</t>
+  </si>
 </sst>
 </file>
 
@@ -1688,8 +1748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1883,7 +1943,7 @@
       </c>
       <c r="L3" s="26">
         <f>(SUM(C2,(E11:E500)))-(SUM((D11:D500),(C11:C500)))</f>
-        <v>9688.82</v>
+        <v>10619.23</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -1957,7 +2017,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>34185.32</v>
+        <v>35360.229999999996</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -2005,7 +2065,7 @@
       </c>
       <c r="BA4" s="60">
         <f>(SUM((AP3:AP519)))-(SUM((AT3:AT519)))</f>
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="BB4" s="60"/>
     </row>
@@ -2102,7 +2162,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>48.5</v>
+        <v>241</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -2178,7 +2238,7 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>2048.5</v>
+        <v>2241</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
@@ -2317,7 +2377,7 @@
       </c>
       <c r="L9" s="15">
         <f>SUM(L11:L501)</f>
-        <v>22448</v>
+        <v>22500</v>
       </c>
       <c r="N9" s="34" t="s">
         <v>51</v>
@@ -3800,9 +3860,17 @@
       </c>
     </row>
     <row r="25" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A25" s="33">
+        <v>43015</v>
+      </c>
+      <c r="B25" t="s">
+        <v>286</v>
+      </c>
       <c r="C25" s="13"/>
       <c r="D25" s="12"/>
-      <c r="E25" s="14"/>
+      <c r="E25" s="14">
+        <v>1288</v>
+      </c>
       <c r="G25" s="60" t="s">
         <v>32</v>
       </c>
@@ -3888,8 +3956,16 @@
       </c>
     </row>
     <row r="26" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A26" s="33">
+        <v>43013</v>
+      </c>
+      <c r="B26" t="s">
+        <v>212</v>
+      </c>
       <c r="C26" s="13"/>
-      <c r="D26" s="12"/>
+      <c r="D26" s="12">
+        <v>160.9</v>
+      </c>
       <c r="E26" s="14"/>
       <c r="G26" s="67" t="s">
         <v>30</v>
@@ -4003,8 +4079,16 @@
       </c>
     </row>
     <row r="27" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A27" s="33">
+        <v>43016</v>
+      </c>
+      <c r="B27" t="s">
+        <v>176</v>
+      </c>
       <c r="C27" s="13"/>
-      <c r="D27" s="12"/>
+      <c r="D27" s="12">
+        <v>196.69</v>
+      </c>
       <c r="E27" s="14"/>
       <c r="G27" s="60" t="s">
         <v>33</v>
@@ -5015,11 +5099,21 @@
       <c r="L36" s="66">
         <v>0</v>
       </c>
-      <c r="N36" s="37"/>
-      <c r="O36" s="37"/>
-      <c r="P36" s="37"/>
-      <c r="Q36" s="39"/>
-      <c r="R36" s="39"/>
+      <c r="N36" s="38">
+        <v>43015</v>
+      </c>
+      <c r="O36" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="P36" s="37" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q36" s="39">
+        <v>1288</v>
+      </c>
+      <c r="R36" s="39">
+        <v>1288</v>
+      </c>
       <c r="T36" s="49">
         <v>42988</v>
       </c>
@@ -5104,10 +5198,16 @@
         <f>J37-K37</f>
         <v>1200</v>
       </c>
-      <c r="N37" s="37"/>
-      <c r="O37" s="37"/>
+      <c r="N37" s="38">
+        <v>43012</v>
+      </c>
+      <c r="O37" s="37" t="s">
+        <v>290</v>
+      </c>
       <c r="P37" s="37"/>
-      <c r="Q37" s="39"/>
+      <c r="Q37" s="39">
+        <v>350</v>
+      </c>
       <c r="R37" s="39"/>
       <c r="T37" s="49">
         <v>42989</v>
@@ -5206,10 +5306,18 @@
         <f t="shared" ref="L38:L84" si="7">J38-K38</f>
         <v>1200</v>
       </c>
-      <c r="N38" s="37"/>
-      <c r="O38" s="37"/>
-      <c r="P38" s="37"/>
-      <c r="Q38" s="39"/>
+      <c r="N38" s="38">
+        <v>43016</v>
+      </c>
+      <c r="O38" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="P38" s="37" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q38" s="39">
+        <v>200</v>
+      </c>
       <c r="R38" s="39"/>
       <c r="T38" s="49">
         <v>42990</v>
@@ -5797,22 +5905,24 @@
       <c r="C44" s="13"/>
       <c r="D44" s="12"/>
       <c r="E44" s="14"/>
-      <c r="G44" s="64">
+      <c r="G44" s="59">
         <v>43006</v>
       </c>
-      <c r="H44" s="18" t="s">
+      <c r="H44" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="I44" s="18" t="s">
+      <c r="I44" s="60" t="s">
         <v>263</v>
       </c>
-      <c r="J44" s="23">
+      <c r="J44" s="62">
         <v>1288</v>
       </c>
-      <c r="K44" s="22"/>
-      <c r="L44" s="20">
+      <c r="K44" s="65">
+        <v>1288</v>
+      </c>
+      <c r="L44" s="66">
         <f t="shared" si="7"/>
-        <v>1288</v>
+        <v>0</v>
       </c>
       <c r="N44" s="37"/>
       <c r="O44" s="37"/>
@@ -6008,14 +6118,22 @@
       <c r="C46" s="13"/>
       <c r="D46" s="12"/>
       <c r="E46" s="14"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="23"/>
+      <c r="G46" s="64">
+        <v>43014</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="I46" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="J46" s="23">
+        <v>300</v>
+      </c>
       <c r="K46" s="22"/>
       <c r="L46" s="20">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="N46" s="37"/>
       <c r="O46" s="37"/>
@@ -6102,14 +6220,22 @@
       <c r="C47" s="13"/>
       <c r="D47" s="12"/>
       <c r="E47" s="14"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="23"/>
+      <c r="G47" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="H47" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I47" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="J47" s="23">
+        <v>1040</v>
+      </c>
       <c r="K47" s="22"/>
       <c r="L47" s="20">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1040</v>
       </c>
       <c r="N47" s="37"/>
       <c r="O47" s="37"/>
@@ -6190,11 +6316,21 @@
       <c r="C48" s="13"/>
       <c r="D48" s="12"/>
       <c r="E48" s="14"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="23"/>
-      <c r="K48" s="22"/>
+      <c r="G48" s="64">
+        <v>43016</v>
+      </c>
+      <c r="H48" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="I48" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="J48" s="23">
+        <v>200</v>
+      </c>
+      <c r="K48" s="22">
+        <v>200</v>
+      </c>
       <c r="L48" s="20">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -6764,13 +6900,13 @@
       </c>
       <c r="W54" s="43">
         <f t="shared" si="3"/>
-        <v>-55</v>
+        <v>-45</v>
       </c>
       <c r="X54" s="52">
         <v>80</v>
       </c>
       <c r="Y54" s="101">
-        <v>21.5</v>
+        <v>31.5</v>
       </c>
       <c r="AA54" s="53">
         <f t="shared" si="0"/>
@@ -7285,9 +7421,12 @@
         <f t="shared" si="1"/>
         <v>17.5</v>
       </c>
+      <c r="AQ59">
+        <v>2</v>
+      </c>
       <c r="AT59">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AU59">
         <v>1</v>
@@ -7329,7 +7468,7 @@
       </c>
       <c r="W60" s="43">
         <f t="shared" si="3"/>
-        <v>64</v>
+        <v>-30</v>
       </c>
       <c r="X60" s="52">
         <v>80</v>
@@ -7337,13 +7476,22 @@
       <c r="Y60" s="52"/>
       <c r="AA60" s="53">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>110</v>
+      </c>
+      <c r="AB60">
+        <v>60</v>
+      </c>
+      <c r="AC60" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD60" t="s">
+        <v>285</v>
       </c>
       <c r="AE60">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="AF60">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG60">
         <v>0</v>
@@ -7406,23 +7554,32 @@
       <c r="T61" s="49">
         <v>43013</v>
       </c>
-      <c r="U61" s="50"/>
-      <c r="V61" s="51"/>
+      <c r="U61" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="V61" s="51" t="s">
+        <v>295</v>
+      </c>
       <c r="W61" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X61" s="52"/>
+        <v>40</v>
+      </c>
+      <c r="X61" s="52">
+        <v>80</v>
+      </c>
       <c r="Y61" s="52"/>
       <c r="AA61" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="AD61" t="s">
+        <v>293</v>
       </c>
       <c r="AE61">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AF61">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AG61">
         <v>0</v>
@@ -7450,15 +7607,21 @@
       </c>
       <c r="AO61">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="AQ61">
+        <v>2</v>
       </c>
       <c r="AT61">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="AU61">
+        <v>3</v>
       </c>
       <c r="AV61">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="62" spans="3:49" x14ac:dyDescent="0.25">
@@ -7482,23 +7645,38 @@
       <c r="T62" s="49">
         <v>43014</v>
       </c>
-      <c r="U62" s="50"/>
-      <c r="V62" s="51"/>
+      <c r="U62" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="V62" s="51" t="s">
+        <v>294</v>
+      </c>
       <c r="W62" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X62" s="52"/>
+        <v>-333.5</v>
+      </c>
+      <c r="X62" s="52">
+        <v>80</v>
+      </c>
       <c r="Y62" s="52"/>
       <c r="AA62" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>413.5</v>
+      </c>
+      <c r="AB62">
+        <v>70</v>
+      </c>
+      <c r="AC62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AD62" t="s">
+        <v>292</v>
       </c>
       <c r="AE62">
-        <v>0</v>
-      </c>
-      <c r="AF62">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="AF62" s="12">
+        <v>300</v>
       </c>
       <c r="AG62">
         <v>0</v>
@@ -7526,15 +7704,21 @@
       </c>
       <c r="AO62">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23.5</v>
       </c>
       <c r="AT62">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="AU62">
+        <v>1</v>
+      </c>
       <c r="AV62">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="AW62">
+        <v>18.5</v>
       </c>
     </row>
     <row r="63" spans="3:49" x14ac:dyDescent="0.25">
@@ -7558,29 +7742,44 @@
       <c r="T63" s="49">
         <v>43015</v>
       </c>
-      <c r="U63" s="50"/>
-      <c r="V63" s="51"/>
+      <c r="U63" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="V63" s="51" t="s">
+        <v>298</v>
+      </c>
       <c r="W63" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X63" s="52"/>
+        <v>20</v>
+      </c>
+      <c r="X63" s="52">
+        <v>200</v>
+      </c>
       <c r="Y63" s="52"/>
       <c r="AA63" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>180</v>
+      </c>
+      <c r="AB63">
+        <v>100</v>
+      </c>
+      <c r="AC63" t="s">
+        <v>299</v>
+      </c>
+      <c r="AD63" t="s">
+        <v>300</v>
       </c>
       <c r="AE63">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AF63">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AG63">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AH63">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AI63">
         <v>0</v>
@@ -7634,8 +7833,12 @@
       <c r="T64" s="49">
         <v>43016</v>
       </c>
-      <c r="U64" s="50"/>
-      <c r="V64" s="51"/>
+      <c r="U64" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="V64" s="51" t="s">
+        <v>303</v>
+      </c>
       <c r="W64" s="43">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -7710,7 +7913,9 @@
       <c r="T65" s="49">
         <v>43017</v>
       </c>
-      <c r="U65" s="50"/>
+      <c r="U65" s="50" t="s">
+        <v>95</v>
+      </c>
       <c r="V65" s="51"/>
       <c r="W65" s="43">
         <f t="shared" si="3"/>
@@ -7786,7 +7991,9 @@
       <c r="T66" s="49">
         <v>43018</v>
       </c>
-      <c r="U66" s="50"/>
+      <c r="U66" s="50" t="s">
+        <v>91</v>
+      </c>
       <c r="V66" s="51"/>
       <c r="W66" s="43">
         <f t="shared" si="3"/>
@@ -7862,7 +8069,9 @@
       <c r="T67" s="49">
         <v>43019</v>
       </c>
-      <c r="U67" s="50"/>
+      <c r="U67" s="50" t="s">
+        <v>96</v>
+      </c>
       <c r="V67" s="51"/>
       <c r="W67" s="43">
         <f t="shared" si="3"/>
@@ -7938,7 +8147,9 @@
       <c r="T68" s="49">
         <v>43020</v>
       </c>
-      <c r="U68" s="50"/>
+      <c r="U68" s="50" t="s">
+        <v>55</v>
+      </c>
       <c r="V68" s="51"/>
       <c r="W68" s="43">
         <f t="shared" ref="W68:W131" si="10">(SUM(X68,Y68))-AA68</f>
@@ -8014,7 +8225,9 @@
       <c r="T69" s="49">
         <v>43021</v>
       </c>
-      <c r="U69" s="50"/>
+      <c r="U69" s="50" t="s">
+        <v>92</v>
+      </c>
       <c r="V69" s="51"/>
       <c r="W69" s="43">
         <f t="shared" si="10"/>
@@ -8090,7 +8303,9 @@
       <c r="T70" s="49">
         <v>43022</v>
       </c>
-      <c r="U70" s="50"/>
+      <c r="U70" s="50" t="s">
+        <v>93</v>
+      </c>
       <c r="V70" s="51"/>
       <c r="W70" s="43">
         <f t="shared" si="10"/>
@@ -8166,7 +8381,9 @@
       <c r="T71" s="49">
         <v>43023</v>
       </c>
-      <c r="U71" s="50"/>
+      <c r="U71" s="50" t="s">
+        <v>94</v>
+      </c>
       <c r="V71" s="51"/>
       <c r="W71" s="43">
         <f t="shared" si="10"/>
@@ -8242,7 +8459,9 @@
       <c r="T72" s="49">
         <v>43024</v>
       </c>
-      <c r="U72" s="50"/>
+      <c r="U72" s="50" t="s">
+        <v>95</v>
+      </c>
       <c r="V72" s="51"/>
       <c r="W72" s="43">
         <f t="shared" si="10"/>
@@ -8318,7 +8537,9 @@
       <c r="T73" s="49">
         <v>43025</v>
       </c>
-      <c r="U73" s="50"/>
+      <c r="U73" s="50" t="s">
+        <v>91</v>
+      </c>
       <c r="V73" s="51"/>
       <c r="W73" s="43">
         <f t="shared" si="10"/>
@@ -8394,7 +8615,9 @@
       <c r="T74" s="49">
         <v>43026</v>
       </c>
-      <c r="U74" s="50"/>
+      <c r="U74" s="50" t="s">
+        <v>96</v>
+      </c>
       <c r="V74" s="51"/>
       <c r="W74" s="43">
         <f t="shared" si="10"/>
@@ -8470,7 +8693,9 @@
       <c r="T75" s="49">
         <v>43027</v>
       </c>
-      <c r="U75" s="50"/>
+      <c r="U75" s="50" t="s">
+        <v>55</v>
+      </c>
       <c r="V75" s="51"/>
       <c r="W75" s="43">
         <f t="shared" si="10"/>
@@ -8546,7 +8771,9 @@
       <c r="T76" s="49">
         <v>43028</v>
       </c>
-      <c r="U76" s="50"/>
+      <c r="U76" s="50" t="s">
+        <v>92</v>
+      </c>
       <c r="V76" s="51"/>
       <c r="W76" s="43">
         <f t="shared" si="10"/>
@@ -8622,7 +8849,9 @@
       <c r="T77" s="49">
         <v>43029</v>
       </c>
-      <c r="U77" s="50"/>
+      <c r="U77" s="50" t="s">
+        <v>93</v>
+      </c>
       <c r="V77" s="51"/>
       <c r="W77" s="43">
         <f t="shared" si="10"/>
@@ -8698,7 +8927,9 @@
       <c r="T78" s="49">
         <v>43030</v>
       </c>
-      <c r="U78" s="50"/>
+      <c r="U78" s="50" t="s">
+        <v>94</v>
+      </c>
       <c r="V78" s="51"/>
       <c r="W78" s="43">
         <f t="shared" si="10"/>
@@ -9303,7 +9534,9 @@
       <c r="P86" s="37"/>
       <c r="Q86" s="39"/>
       <c r="R86" s="39"/>
-      <c r="T86" s="50"/>
+      <c r="T86" s="49">
+        <v>43038</v>
+      </c>
       <c r="U86" s="50"/>
       <c r="V86" s="51"/>
       <c r="W86" s="43">
@@ -9377,7 +9610,9 @@
       <c r="P87" s="37"/>
       <c r="Q87" s="39"/>
       <c r="R87" s="39"/>
-      <c r="T87" s="50"/>
+      <c r="T87" s="49">
+        <v>43039</v>
+      </c>
       <c r="U87" s="50"/>
       <c r="V87" s="51"/>
       <c r="W87" s="43">
@@ -9451,7 +9686,9 @@
       <c r="P88" s="37"/>
       <c r="Q88" s="39"/>
       <c r="R88" s="39"/>
-      <c r="T88" s="50"/>
+      <c r="T88" s="49">
+        <v>43040</v>
+      </c>
       <c r="U88" s="50"/>
       <c r="V88" s="51"/>
       <c r="W88" s="43">
@@ -9525,7 +9762,9 @@
       <c r="P89" s="37"/>
       <c r="Q89" s="39"/>
       <c r="R89" s="39"/>
-      <c r="T89" s="50"/>
+      <c r="T89" s="49">
+        <v>43041</v>
+      </c>
       <c r="U89" s="50"/>
       <c r="V89" s="51"/>
       <c r="W89" s="43">
@@ -9599,7 +9838,9 @@
       <c r="P90" s="37"/>
       <c r="Q90" s="39"/>
       <c r="R90" s="39"/>
-      <c r="T90" s="50"/>
+      <c r="T90" s="49">
+        <v>43042</v>
+      </c>
       <c r="U90" s="50"/>
       <c r="V90" s="51"/>
       <c r="W90" s="43">
@@ -9673,7 +9914,9 @@
       <c r="P91" s="37"/>
       <c r="Q91" s="39"/>
       <c r="R91" s="39"/>
-      <c r="T91" s="50"/>
+      <c r="T91" s="49">
+        <v>43043</v>
+      </c>
       <c r="U91" s="50"/>
       <c r="V91" s="51"/>
       <c r="W91" s="43">
@@ -9747,7 +9990,9 @@
       <c r="P92" s="37"/>
       <c r="Q92" s="39"/>
       <c r="R92" s="39"/>
-      <c r="T92" s="50"/>
+      <c r="T92" s="49">
+        <v>43044</v>
+      </c>
       <c r="U92" s="50"/>
       <c r="V92" s="51"/>
       <c r="W92" s="43">
@@ -9821,7 +10066,9 @@
       <c r="P93" s="37"/>
       <c r="Q93" s="39"/>
       <c r="R93" s="39"/>
-      <c r="T93" s="50"/>
+      <c r="T93" s="49">
+        <v>43045</v>
+      </c>
       <c r="U93" s="50"/>
       <c r="V93" s="51"/>
       <c r="W93" s="43">
@@ -9895,7 +10142,9 @@
       <c r="P94" s="37"/>
       <c r="Q94" s="39"/>
       <c r="R94" s="39"/>
-      <c r="T94" s="50"/>
+      <c r="T94" s="49">
+        <v>43046</v>
+      </c>
       <c r="U94" s="50"/>
       <c r="V94" s="51"/>
       <c r="W94" s="43">
@@ -9969,7 +10218,9 @@
       <c r="P95" s="37"/>
       <c r="Q95" s="39"/>
       <c r="R95" s="39"/>
-      <c r="T95" s="50"/>
+      <c r="T95" s="49">
+        <v>43047</v>
+      </c>
       <c r="U95" s="50"/>
       <c r="V95" s="51"/>
       <c r="W95" s="43">
@@ -10043,7 +10294,9 @@
       <c r="P96" s="37"/>
       <c r="Q96" s="39"/>
       <c r="R96" s="39"/>
-      <c r="T96" s="50"/>
+      <c r="T96" s="49">
+        <v>43048</v>
+      </c>
       <c r="U96" s="50"/>
       <c r="V96" s="51"/>
       <c r="W96" s="43">
@@ -10117,7 +10370,9 @@
       <c r="P97" s="37"/>
       <c r="Q97" s="39"/>
       <c r="R97" s="39"/>
-      <c r="T97" s="50"/>
+      <c r="T97" s="49">
+        <v>43049</v>
+      </c>
       <c r="U97" s="50"/>
       <c r="V97" s="51"/>
       <c r="W97" s="43">
@@ -10191,7 +10446,9 @@
       <c r="P98" s="37"/>
       <c r="Q98" s="39"/>
       <c r="R98" s="39"/>
-      <c r="T98" s="50"/>
+      <c r="T98" s="49">
+        <v>43050</v>
+      </c>
       <c r="U98" s="50"/>
       <c r="V98" s="51"/>
       <c r="W98" s="43">
@@ -10265,7 +10522,9 @@
       <c r="P99" s="37"/>
       <c r="Q99" s="39"/>
       <c r="R99" s="39"/>
-      <c r="T99" s="50"/>
+      <c r="T99" s="49">
+        <v>43051</v>
+      </c>
       <c r="U99" s="50"/>
       <c r="V99" s="51"/>
       <c r="W99" s="43">
@@ -10339,7 +10598,9 @@
       <c r="P100" s="37"/>
       <c r="Q100" s="39"/>
       <c r="R100" s="39"/>
-      <c r="T100" s="50"/>
+      <c r="T100" s="49">
+        <v>43052</v>
+      </c>
       <c r="U100" s="50"/>
       <c r="V100" s="51"/>
       <c r="W100" s="43">
@@ -10413,7 +10674,9 @@
       <c r="P101" s="37"/>
       <c r="Q101" s="39"/>
       <c r="R101" s="39"/>
-      <c r="T101" s="50"/>
+      <c r="T101" s="49">
+        <v>43053</v>
+      </c>
       <c r="U101" s="50"/>
       <c r="V101" s="51"/>
       <c r="W101" s="43">
@@ -10487,7 +10750,9 @@
       <c r="P102" s="37"/>
       <c r="Q102" s="39"/>
       <c r="R102" s="39"/>
-      <c r="T102" s="50"/>
+      <c r="T102" s="49">
+        <v>43054</v>
+      </c>
       <c r="U102" s="50"/>
       <c r="V102" s="51"/>
       <c r="W102" s="43">
@@ -10561,7 +10826,9 @@
       <c r="P103" s="37"/>
       <c r="Q103" s="39"/>
       <c r="R103" s="39"/>
-      <c r="T103" s="50"/>
+      <c r="T103" s="49">
+        <v>43055</v>
+      </c>
       <c r="U103" s="50"/>
       <c r="V103" s="51"/>
       <c r="W103" s="43">
@@ -10635,7 +10902,9 @@
       <c r="P104" s="37"/>
       <c r="Q104" s="39"/>
       <c r="R104" s="39"/>
-      <c r="T104" s="50"/>
+      <c r="T104" s="49">
+        <v>43056</v>
+      </c>
       <c r="U104" s="50"/>
       <c r="V104" s="51"/>
       <c r="W104" s="43">
@@ -10709,7 +10978,9 @@
       <c r="P105" s="37"/>
       <c r="Q105" s="39"/>
       <c r="R105" s="39"/>
-      <c r="T105" s="50"/>
+      <c r="T105" s="49">
+        <v>43057</v>
+      </c>
       <c r="U105" s="50"/>
       <c r="V105" s="51"/>
       <c r="W105" s="43">
@@ -10783,7 +11054,9 @@
       <c r="P106" s="37"/>
       <c r="Q106" s="39"/>
       <c r="R106" s="39"/>
-      <c r="T106" s="50"/>
+      <c r="T106" s="49">
+        <v>43058</v>
+      </c>
       <c r="U106" s="50"/>
       <c r="V106" s="51"/>
       <c r="W106" s="43">
@@ -10857,7 +11130,9 @@
       <c r="P107" s="37"/>
       <c r="Q107" s="39"/>
       <c r="R107" s="39"/>
-      <c r="T107" s="50"/>
+      <c r="T107" s="49">
+        <v>43059</v>
+      </c>
       <c r="U107" s="50"/>
       <c r="V107" s="51"/>
       <c r="W107" s="43">
@@ -10931,7 +11206,9 @@
       <c r="P108" s="37"/>
       <c r="Q108" s="39"/>
       <c r="R108" s="39"/>
-      <c r="T108" s="50"/>
+      <c r="T108" s="49">
+        <v>43060</v>
+      </c>
       <c r="U108" s="50"/>
       <c r="V108" s="51"/>
       <c r="W108" s="43">
@@ -11005,7 +11282,9 @@
       <c r="P109" s="37"/>
       <c r="Q109" s="39"/>
       <c r="R109" s="39"/>
-      <c r="T109" s="50"/>
+      <c r="T109" s="49">
+        <v>43061</v>
+      </c>
       <c r="U109" s="50"/>
       <c r="V109" s="51"/>
       <c r="W109" s="43">
@@ -11079,7 +11358,9 @@
       <c r="P110" s="37"/>
       <c r="Q110" s="39"/>
       <c r="R110" s="39"/>
-      <c r="T110" s="50"/>
+      <c r="T110" s="49">
+        <v>43062</v>
+      </c>
       <c r="U110" s="50"/>
       <c r="V110" s="51"/>
       <c r="W110" s="43">
@@ -11153,7 +11434,9 @@
       <c r="P111" s="37"/>
       <c r="Q111" s="39"/>
       <c r="R111" s="39"/>
-      <c r="T111" s="50"/>
+      <c r="T111" s="49">
+        <v>43063</v>
+      </c>
       <c r="U111" s="50"/>
       <c r="V111" s="51"/>
       <c r="W111" s="43">
@@ -11227,7 +11510,9 @@
       <c r="P112" s="37"/>
       <c r="Q112" s="39"/>
       <c r="R112" s="39"/>
-      <c r="T112" s="50"/>
+      <c r="T112" s="49">
+        <v>43064</v>
+      </c>
       <c r="U112" s="50"/>
       <c r="V112" s="51"/>
       <c r="W112" s="43">
@@ -11301,7 +11586,9 @@
       <c r="P113" s="37"/>
       <c r="Q113" s="39"/>
       <c r="R113" s="39"/>
-      <c r="T113" s="50"/>
+      <c r="T113" s="49">
+        <v>43065</v>
+      </c>
       <c r="U113" s="50"/>
       <c r="V113" s="51"/>
       <c r="W113" s="43">
@@ -11375,7 +11662,9 @@
       <c r="P114" s="37"/>
       <c r="Q114" s="39"/>
       <c r="R114" s="39"/>
-      <c r="T114" s="50"/>
+      <c r="T114" s="49">
+        <v>43066</v>
+      </c>
       <c r="U114" s="50"/>
       <c r="V114" s="51"/>
       <c r="W114" s="43">
@@ -11449,7 +11738,9 @@
       <c r="P115" s="37"/>
       <c r="Q115" s="39"/>
       <c r="R115" s="39"/>
-      <c r="T115" s="50"/>
+      <c r="T115" s="49">
+        <v>43067</v>
+      </c>
       <c r="U115" s="50"/>
       <c r="V115" s="51"/>
       <c r="W115" s="43">
@@ -11523,7 +11814,9 @@
       <c r="P116" s="37"/>
       <c r="Q116" s="39"/>
       <c r="R116" s="39"/>
-      <c r="T116" s="50"/>
+      <c r="T116" s="49">
+        <v>43068</v>
+      </c>
       <c r="U116" s="50"/>
       <c r="V116" s="51"/>
       <c r="W116" s="43">
@@ -11597,7 +11890,9 @@
       <c r="P117" s="37"/>
       <c r="Q117" s="39"/>
       <c r="R117" s="39"/>
-      <c r="T117" s="50"/>
+      <c r="T117" s="49">
+        <v>43069</v>
+      </c>
       <c r="U117" s="50"/>
       <c r="V117" s="51"/>
       <c r="W117" s="43">
@@ -11671,7 +11966,9 @@
       <c r="P118" s="37"/>
       <c r="Q118" s="39"/>
       <c r="R118" s="39"/>
-      <c r="T118" s="50"/>
+      <c r="T118" s="49">
+        <v>43070</v>
+      </c>
       <c r="U118" s="50"/>
       <c r="V118" s="51"/>
       <c r="W118" s="43">
@@ -11745,7 +12042,9 @@
       <c r="P119" s="37"/>
       <c r="Q119" s="39"/>
       <c r="R119" s="39"/>
-      <c r="T119" s="50"/>
+      <c r="T119" s="49">
+        <v>43071</v>
+      </c>
       <c r="U119" s="50"/>
       <c r="V119" s="51"/>
       <c r="W119" s="43">
@@ -11819,7 +12118,9 @@
       <c r="P120" s="37"/>
       <c r="Q120" s="39"/>
       <c r="R120" s="39"/>
-      <c r="T120" s="50"/>
+      <c r="T120" s="49">
+        <v>43072</v>
+      </c>
       <c r="U120" s="50"/>
       <c r="V120" s="51"/>
       <c r="W120" s="43">
@@ -11893,7 +12194,9 @@
       <c r="P121" s="37"/>
       <c r="Q121" s="39"/>
       <c r="R121" s="39"/>
-      <c r="T121" s="50"/>
+      <c r="T121" s="49">
+        <v>43073</v>
+      </c>
       <c r="U121" s="50"/>
       <c r="V121" s="51"/>
       <c r="W121" s="43">
@@ -11967,7 +12270,9 @@
       <c r="P122" s="37"/>
       <c r="Q122" s="39"/>
       <c r="R122" s="39"/>
-      <c r="T122" s="50"/>
+      <c r="T122" s="49">
+        <v>43074</v>
+      </c>
       <c r="U122" s="50"/>
       <c r="V122" s="51"/>
       <c r="W122" s="43">
@@ -12041,7 +12346,9 @@
       <c r="P123" s="37"/>
       <c r="Q123" s="39"/>
       <c r="R123" s="39"/>
-      <c r="T123" s="50"/>
+      <c r="T123" s="49">
+        <v>43075</v>
+      </c>
       <c r="U123" s="50"/>
       <c r="V123" s="51"/>
       <c r="W123" s="43">
@@ -12115,7 +12422,9 @@
       <c r="P124" s="37"/>
       <c r="Q124" s="39"/>
       <c r="R124" s="39"/>
-      <c r="T124" s="50"/>
+      <c r="T124" s="49">
+        <v>43076</v>
+      </c>
       <c r="U124" s="50"/>
       <c r="V124" s="51"/>
       <c r="W124" s="43">
@@ -12189,7 +12498,9 @@
       <c r="P125" s="37"/>
       <c r="Q125" s="39"/>
       <c r="R125" s="39"/>
-      <c r="T125" s="50"/>
+      <c r="T125" s="49">
+        <v>43077</v>
+      </c>
       <c r="U125" s="50"/>
       <c r="V125" s="51"/>
       <c r="W125" s="43">
@@ -12263,7 +12574,9 @@
       <c r="P126" s="37"/>
       <c r="Q126" s="39"/>
       <c r="R126" s="39"/>
-      <c r="T126" s="50"/>
+      <c r="T126" s="49">
+        <v>43078</v>
+      </c>
       <c r="U126" s="50"/>
       <c r="V126" s="51"/>
       <c r="W126" s="43">
@@ -12337,7 +12650,9 @@
       <c r="P127" s="37"/>
       <c r="Q127" s="39"/>
       <c r="R127" s="39"/>
-      <c r="T127" s="50"/>
+      <c r="T127" s="49">
+        <v>43079</v>
+      </c>
       <c r="U127" s="50"/>
       <c r="V127" s="51"/>
       <c r="W127" s="43">
@@ -12411,7 +12726,9 @@
       <c r="P128" s="37"/>
       <c r="Q128" s="39"/>
       <c r="R128" s="39"/>
-      <c r="T128" s="50"/>
+      <c r="T128" s="49">
+        <v>43080</v>
+      </c>
       <c r="U128" s="50"/>
       <c r="V128" s="51"/>
       <c r="W128" s="43">
@@ -12485,7 +12802,9 @@
       <c r="P129" s="37"/>
       <c r="Q129" s="39"/>
       <c r="R129" s="39"/>
-      <c r="T129" s="50"/>
+      <c r="T129" s="49">
+        <v>43081</v>
+      </c>
       <c r="U129" s="50"/>
       <c r="V129" s="51"/>
       <c r="W129" s="43">
@@ -12559,7 +12878,9 @@
       <c r="P130" s="37"/>
       <c r="Q130" s="39"/>
       <c r="R130" s="39"/>
-      <c r="T130" s="50"/>
+      <c r="T130" s="49">
+        <v>43082</v>
+      </c>
       <c r="U130" s="50"/>
       <c r="V130" s="51"/>
       <c r="W130" s="43">
@@ -12633,7 +12954,9 @@
       <c r="P131" s="37"/>
       <c r="Q131" s="39"/>
       <c r="R131" s="39"/>
-      <c r="T131" s="50"/>
+      <c r="T131" s="49">
+        <v>43083</v>
+      </c>
       <c r="U131" s="50"/>
       <c r="V131" s="51"/>
       <c r="W131" s="43">
@@ -12707,7 +13030,9 @@
       <c r="P132" s="37"/>
       <c r="Q132" s="39"/>
       <c r="R132" s="39"/>
-      <c r="T132" s="50"/>
+      <c r="T132" s="49">
+        <v>43084</v>
+      </c>
       <c r="U132" s="50"/>
       <c r="V132" s="51"/>
       <c r="W132" s="43">
@@ -12781,7 +13106,9 @@
       <c r="P133" s="37"/>
       <c r="Q133" s="39"/>
       <c r="R133" s="39"/>
-      <c r="T133" s="50"/>
+      <c r="T133" s="49">
+        <v>43085</v>
+      </c>
       <c r="U133" s="50"/>
       <c r="V133" s="51"/>
       <c r="W133" s="43">
@@ -12855,7 +13182,9 @@
       <c r="P134" s="37"/>
       <c r="Q134" s="39"/>
       <c r="R134" s="39"/>
-      <c r="T134" s="50"/>
+      <c r="T134" s="49">
+        <v>43086</v>
+      </c>
       <c r="U134" s="50"/>
       <c r="V134" s="51"/>
       <c r="W134" s="43">
@@ -12929,7 +13258,9 @@
       <c r="P135" s="37"/>
       <c r="Q135" s="39"/>
       <c r="R135" s="39"/>
-      <c r="T135" s="50"/>
+      <c r="T135" s="49">
+        <v>43087</v>
+      </c>
       <c r="U135" s="50"/>
       <c r="V135" s="51"/>
       <c r="W135" s="43">
@@ -13003,7 +13334,9 @@
       <c r="P136" s="37"/>
       <c r="Q136" s="39"/>
       <c r="R136" s="39"/>
-      <c r="T136" s="50"/>
+      <c r="T136" s="49">
+        <v>43088</v>
+      </c>
       <c r="U136" s="50"/>
       <c r="V136" s="51"/>
       <c r="W136" s="43">
@@ -13077,7 +13410,9 @@
       <c r="P137" s="37"/>
       <c r="Q137" s="39"/>
       <c r="R137" s="39"/>
-      <c r="T137" s="50"/>
+      <c r="T137" s="49">
+        <v>43089</v>
+      </c>
       <c r="U137" s="50"/>
       <c r="V137" s="51"/>
       <c r="W137" s="43">
@@ -13151,7 +13486,9 @@
       <c r="P138" s="37"/>
       <c r="Q138" s="39"/>
       <c r="R138" s="39"/>
-      <c r="T138" s="50"/>
+      <c r="T138" s="49">
+        <v>43090</v>
+      </c>
       <c r="U138" s="50"/>
       <c r="V138" s="51"/>
       <c r="W138" s="43">
@@ -13225,7 +13562,9 @@
       <c r="P139" s="37"/>
       <c r="Q139" s="39"/>
       <c r="R139" s="39"/>
-      <c r="T139" s="50"/>
+      <c r="T139" s="49">
+        <v>43091</v>
+      </c>
       <c r="U139" s="50"/>
       <c r="V139" s="51"/>
       <c r="W139" s="43">
@@ -13299,7 +13638,9 @@
       <c r="P140" s="37"/>
       <c r="Q140" s="39"/>
       <c r="R140" s="39"/>
-      <c r="T140" s="50"/>
+      <c r="T140" s="49">
+        <v>43092</v>
+      </c>
       <c r="U140" s="50"/>
       <c r="V140" s="51"/>
       <c r="W140" s="43">
@@ -13373,7 +13714,9 @@
       <c r="P141" s="37"/>
       <c r="Q141" s="39"/>
       <c r="R141" s="39"/>
-      <c r="T141" s="50"/>
+      <c r="T141" s="49">
+        <v>43093</v>
+      </c>
       <c r="U141" s="50"/>
       <c r="V141" s="51"/>
       <c r="W141" s="43">
@@ -13447,7 +13790,9 @@
       <c r="P142" s="37"/>
       <c r="Q142" s="39"/>
       <c r="R142" s="39"/>
-      <c r="T142" s="50"/>
+      <c r="T142" s="49">
+        <v>43094</v>
+      </c>
       <c r="U142" s="50"/>
       <c r="V142" s="51"/>
       <c r="W142" s="43">
@@ -13521,7 +13866,9 @@
       <c r="P143" s="37"/>
       <c r="Q143" s="39"/>
       <c r="R143" s="39"/>
-      <c r="T143" s="50"/>
+      <c r="T143" s="49">
+        <v>43095</v>
+      </c>
       <c r="U143" s="50"/>
       <c r="V143" s="51"/>
       <c r="W143" s="43">
@@ -13595,7 +13942,9 @@
       <c r="P144" s="37"/>
       <c r="Q144" s="39"/>
       <c r="R144" s="39"/>
-      <c r="T144" s="50"/>
+      <c r="T144" s="49">
+        <v>43096</v>
+      </c>
       <c r="U144" s="50"/>
       <c r="V144" s="51"/>
       <c r="W144" s="43">
@@ -13669,7 +14018,9 @@
       <c r="P145" s="37"/>
       <c r="Q145" s="39"/>
       <c r="R145" s="39"/>
-      <c r="T145" s="50"/>
+      <c r="T145" s="49">
+        <v>43097</v>
+      </c>
       <c r="U145" s="50"/>
       <c r="V145" s="51"/>
       <c r="W145" s="43">
@@ -13743,7 +14094,9 @@
       <c r="P146" s="37"/>
       <c r="Q146" s="39"/>
       <c r="R146" s="39"/>
-      <c r="T146" s="50"/>
+      <c r="T146" s="49">
+        <v>43098</v>
+      </c>
       <c r="U146" s="50"/>
       <c r="V146" s="51"/>
       <c r="W146" s="43">
@@ -13817,7 +14170,9 @@
       <c r="P147" s="37"/>
       <c r="Q147" s="39"/>
       <c r="R147" s="39"/>
-      <c r="T147" s="50"/>
+      <c r="T147" s="49">
+        <v>43099</v>
+      </c>
       <c r="U147" s="50"/>
       <c r="V147" s="51"/>
       <c r="W147" s="43">
@@ -13891,7 +14246,9 @@
       <c r="P148" s="37"/>
       <c r="Q148" s="39"/>
       <c r="R148" s="39"/>
-      <c r="T148" s="50"/>
+      <c r="T148" s="49">
+        <v>43100</v>
+      </c>
       <c r="U148" s="50"/>
       <c r="V148" s="51"/>
       <c r="W148" s="43">
@@ -13965,7 +14322,7 @@
       <c r="P149" s="37"/>
       <c r="Q149" s="39"/>
       <c r="R149" s="39"/>
-      <c r="T149" s="50"/>
+      <c r="T149" s="49"/>
       <c r="U149" s="50"/>
       <c r="V149" s="51"/>
       <c r="W149" s="43">
@@ -14039,7 +14396,7 @@
       <c r="P150" s="37"/>
       <c r="Q150" s="39"/>
       <c r="R150" s="39"/>
-      <c r="T150" s="50"/>
+      <c r="T150" s="49"/>
       <c r="U150" s="50"/>
       <c r="V150" s="51"/>
       <c r="W150" s="43">
@@ -14113,7 +14470,7 @@
       <c r="P151" s="37"/>
       <c r="Q151" s="39"/>
       <c r="R151" s="39"/>
-      <c r="T151" s="50"/>
+      <c r="T151" s="49"/>
       <c r="U151" s="50"/>
       <c r="V151" s="51"/>
       <c r="W151" s="43">
@@ -14187,7 +14544,7 @@
       <c r="P152" s="37"/>
       <c r="Q152" s="39"/>
       <c r="R152" s="39"/>
-      <c r="T152" s="50"/>
+      <c r="T152" s="49"/>
       <c r="U152" s="50"/>
       <c r="V152" s="51"/>
       <c r="W152" s="43">
@@ -14261,7 +14618,7 @@
       <c r="P153" s="37"/>
       <c r="Q153" s="39"/>
       <c r="R153" s="39"/>
-      <c r="T153" s="50"/>
+      <c r="T153" s="49"/>
       <c r="U153" s="50"/>
       <c r="V153" s="51"/>
       <c r="W153" s="43">
@@ -14335,7 +14692,7 @@
       <c r="P154" s="37"/>
       <c r="Q154" s="39"/>
       <c r="R154" s="39"/>
-      <c r="T154" s="50"/>
+      <c r="T154" s="49"/>
       <c r="U154" s="50"/>
       <c r="V154" s="51"/>
       <c r="W154" s="43">
@@ -14409,7 +14766,7 @@
       <c r="P155" s="37"/>
       <c r="Q155" s="39"/>
       <c r="R155" s="39"/>
-      <c r="T155" s="50"/>
+      <c r="T155" s="49"/>
       <c r="U155" s="50"/>
       <c r="V155" s="51"/>
       <c r="W155" s="43">
@@ -14483,7 +14840,7 @@
       <c r="P156" s="37"/>
       <c r="Q156" s="39"/>
       <c r="R156" s="39"/>
-      <c r="T156" s="50"/>
+      <c r="T156" s="49"/>
       <c r="U156" s="50"/>
       <c r="V156" s="51"/>
       <c r="W156" s="43">
@@ -14557,7 +14914,7 @@
       <c r="P157" s="37"/>
       <c r="Q157" s="39"/>
       <c r="R157" s="39"/>
-      <c r="T157" s="50"/>
+      <c r="T157" s="49"/>
       <c r="U157" s="50"/>
       <c r="V157" s="51"/>
       <c r="W157" s="43">
@@ -14631,7 +14988,7 @@
       <c r="P158" s="37"/>
       <c r="Q158" s="39"/>
       <c r="R158" s="39"/>
-      <c r="T158" s="50"/>
+      <c r="T158" s="49"/>
       <c r="U158" s="50"/>
       <c r="V158" s="51"/>
       <c r="W158" s="43">
@@ -14705,7 +15062,7 @@
       <c r="P159" s="37"/>
       <c r="Q159" s="39"/>
       <c r="R159" s="39"/>
-      <c r="T159" s="50"/>
+      <c r="T159" s="49"/>
       <c r="U159" s="50"/>
       <c r="V159" s="51"/>
       <c r="W159" s="43">
@@ -14779,7 +15136,7 @@
       <c r="P160" s="37"/>
       <c r="Q160" s="39"/>
       <c r="R160" s="39"/>
-      <c r="T160" s="50"/>
+      <c r="T160" s="49"/>
       <c r="U160" s="50"/>
       <c r="V160" s="51"/>
       <c r="W160" s="43">
@@ -14853,7 +15210,7 @@
       <c r="P161" s="37"/>
       <c r="Q161" s="39"/>
       <c r="R161" s="39"/>
-      <c r="T161" s="50"/>
+      <c r="T161" s="49"/>
       <c r="U161" s="50"/>
       <c r="V161" s="51"/>
       <c r="W161" s="43">
@@ -14927,7 +15284,7 @@
       <c r="P162" s="37"/>
       <c r="Q162" s="39"/>
       <c r="R162" s="39"/>
-      <c r="T162" s="50"/>
+      <c r="T162" s="49"/>
       <c r="U162" s="50"/>
       <c r="V162" s="51"/>
       <c r="W162" s="43">
@@ -15001,7 +15358,7 @@
       <c r="P163" s="37"/>
       <c r="Q163" s="39"/>
       <c r="R163" s="39"/>
-      <c r="T163" s="50"/>
+      <c r="T163" s="49"/>
       <c r="U163" s="50"/>
       <c r="V163" s="51"/>
       <c r="W163" s="43">
@@ -15075,7 +15432,7 @@
       <c r="P164" s="37"/>
       <c r="Q164" s="39"/>
       <c r="R164" s="39"/>
-      <c r="T164" s="50"/>
+      <c r="T164" s="49"/>
       <c r="U164" s="50"/>
       <c r="V164" s="51"/>
       <c r="W164" s="43">
@@ -15149,7 +15506,7 @@
       <c r="P165" s="37"/>
       <c r="Q165" s="39"/>
       <c r="R165" s="39"/>
-      <c r="T165" s="50"/>
+      <c r="T165" s="49"/>
       <c r="U165" s="50"/>
       <c r="V165" s="51"/>
       <c r="W165" s="43">
@@ -15223,7 +15580,7 @@
       <c r="P166" s="37"/>
       <c r="Q166" s="39"/>
       <c r="R166" s="39"/>
-      <c r="T166" s="50"/>
+      <c r="T166" s="49"/>
       <c r="U166" s="50"/>
       <c r="V166" s="51"/>
       <c r="W166" s="43">
@@ -15297,7 +15654,7 @@
       <c r="P167" s="37"/>
       <c r="Q167" s="39"/>
       <c r="R167" s="39"/>
-      <c r="T167" s="50"/>
+      <c r="T167" s="49"/>
       <c r="U167" s="50"/>
       <c r="V167" s="51"/>
       <c r="W167" s="43">
@@ -15371,7 +15728,7 @@
       <c r="P168" s="37"/>
       <c r="Q168" s="39"/>
       <c r="R168" s="39"/>
-      <c r="T168" s="50"/>
+      <c r="T168" s="49"/>
       <c r="U168" s="50"/>
       <c r="V168" s="51"/>
       <c r="W168" s="43">
@@ -15445,7 +15802,7 @@
       <c r="P169" s="37"/>
       <c r="Q169" s="39"/>
       <c r="R169" s="39"/>
-      <c r="T169" s="50"/>
+      <c r="T169" s="49"/>
       <c r="U169" s="50"/>
       <c r="V169" s="51"/>
       <c r="W169" s="43">
@@ -15519,7 +15876,7 @@
       <c r="P170" s="37"/>
       <c r="Q170" s="39"/>
       <c r="R170" s="39"/>
-      <c r="T170" s="50"/>
+      <c r="T170" s="49"/>
       <c r="U170" s="50"/>
       <c r="V170" s="51"/>
       <c r="W170" s="43">
@@ -15593,7 +15950,7 @@
       <c r="P171" s="37"/>
       <c r="Q171" s="39"/>
       <c r="R171" s="39"/>
-      <c r="T171" s="50"/>
+      <c r="T171" s="49"/>
       <c r="U171" s="50"/>
       <c r="V171" s="51"/>
       <c r="W171" s="43">
@@ -15667,7 +16024,7 @@
       <c r="P172" s="37"/>
       <c r="Q172" s="39"/>
       <c r="R172" s="39"/>
-      <c r="T172" s="50"/>
+      <c r="T172" s="49"/>
       <c r="U172" s="50"/>
       <c r="V172" s="51"/>
       <c r="W172" s="43">
@@ -15741,7 +16098,7 @@
       <c r="P173" s="37"/>
       <c r="Q173" s="39"/>
       <c r="R173" s="39"/>
-      <c r="T173" s="50"/>
+      <c r="T173" s="49"/>
       <c r="U173" s="50"/>
       <c r="V173" s="51"/>
       <c r="W173" s="43">
@@ -15815,7 +16172,7 @@
       <c r="P174" s="37"/>
       <c r="Q174" s="39"/>
       <c r="R174" s="39"/>
-      <c r="T174" s="50"/>
+      <c r="T174" s="49"/>
       <c r="U174" s="50"/>
       <c r="V174" s="51"/>
       <c r="W174" s="43">
@@ -15889,7 +16246,7 @@
       <c r="P175" s="37"/>
       <c r="Q175" s="39"/>
       <c r="R175" s="39"/>
-      <c r="T175" s="50"/>
+      <c r="T175" s="49"/>
       <c r="U175" s="50"/>
       <c r="V175" s="51"/>
       <c r="W175" s="43">
@@ -15963,7 +16320,7 @@
       <c r="P176" s="37"/>
       <c r="Q176" s="39"/>
       <c r="R176" s="39"/>
-      <c r="T176" s="50"/>
+      <c r="T176" s="49"/>
       <c r="U176" s="50"/>
       <c r="V176" s="51"/>
       <c r="W176" s="43">
@@ -16037,7 +16394,7 @@
       <c r="P177" s="37"/>
       <c r="Q177" s="39"/>
       <c r="R177" s="39"/>
-      <c r="T177" s="50"/>
+      <c r="T177" s="49"/>
       <c r="U177" s="50"/>
       <c r="V177" s="51"/>
       <c r="W177" s="43">
@@ -16111,7 +16468,7 @@
       <c r="P178" s="37"/>
       <c r="Q178" s="39"/>
       <c r="R178" s="39"/>
-      <c r="T178" s="50"/>
+      <c r="T178" s="49"/>
       <c r="U178" s="50"/>
       <c r="V178" s="51"/>
       <c r="W178" s="43">
@@ -16185,7 +16542,7 @@
       <c r="P179" s="37"/>
       <c r="Q179" s="39"/>
       <c r="R179" s="39"/>
-      <c r="T179" s="50"/>
+      <c r="T179" s="49"/>
       <c r="U179" s="50"/>
       <c r="V179" s="51"/>
       <c r="W179" s="43">
@@ -16259,7 +16616,7 @@
       <c r="P180" s="37"/>
       <c r="Q180" s="39"/>
       <c r="R180" s="39"/>
-      <c r="T180" s="50"/>
+      <c r="T180" s="49"/>
       <c r="U180" s="50"/>
       <c r="V180" s="51"/>
       <c r="W180" s="43">
@@ -16333,7 +16690,7 @@
       <c r="P181" s="37"/>
       <c r="Q181" s="39"/>
       <c r="R181" s="39"/>
-      <c r="T181" s="50"/>
+      <c r="T181" s="49"/>
       <c r="U181" s="50"/>
       <c r="V181" s="51"/>
       <c r="W181" s="43">
@@ -16407,7 +16764,7 @@
       <c r="P182" s="37"/>
       <c r="Q182" s="39"/>
       <c r="R182" s="39"/>
-      <c r="T182" s="50"/>
+      <c r="T182" s="49"/>
       <c r="U182" s="50"/>
       <c r="V182" s="51"/>
       <c r="W182" s="43">
@@ -16481,7 +16838,7 @@
       <c r="P183" s="37"/>
       <c r="Q183" s="39"/>
       <c r="R183" s="39"/>
-      <c r="T183" s="50"/>
+      <c r="T183" s="49"/>
       <c r="U183" s="50"/>
       <c r="V183" s="51"/>
       <c r="W183" s="43">
@@ -16555,7 +16912,7 @@
       <c r="P184" s="37"/>
       <c r="Q184" s="39"/>
       <c r="R184" s="39"/>
-      <c r="T184" s="50"/>
+      <c r="T184" s="49"/>
       <c r="U184" s="50"/>
       <c r="V184" s="51"/>
       <c r="W184" s="43">
@@ -16629,7 +16986,7 @@
       <c r="P185" s="37"/>
       <c r="Q185" s="39"/>
       <c r="R185" s="39"/>
-      <c r="T185" s="50"/>
+      <c r="T185" s="49"/>
       <c r="U185" s="50"/>
       <c r="V185" s="51"/>
       <c r="W185" s="43">
@@ -16703,7 +17060,7 @@
       <c r="P186" s="37"/>
       <c r="Q186" s="39"/>
       <c r="R186" s="39"/>
-      <c r="T186" s="50"/>
+      <c r="T186" s="49"/>
       <c r="U186" s="50"/>
       <c r="V186" s="51"/>
       <c r="W186" s="43">
@@ -16777,7 +17134,7 @@
       <c r="P187" s="37"/>
       <c r="Q187" s="39"/>
       <c r="R187" s="39"/>
-      <c r="T187" s="50"/>
+      <c r="T187" s="49"/>
       <c r="U187" s="50"/>
       <c r="V187" s="51"/>
       <c r="W187" s="43">
@@ -16851,7 +17208,7 @@
       <c r="P188" s="37"/>
       <c r="Q188" s="39"/>
       <c r="R188" s="39"/>
-      <c r="T188" s="50"/>
+      <c r="T188" s="49"/>
       <c r="U188" s="50"/>
       <c r="V188" s="51"/>
       <c r="W188" s="43">
@@ -16925,7 +17282,7 @@
       <c r="P189" s="37"/>
       <c r="Q189" s="39"/>
       <c r="R189" s="39"/>
-      <c r="T189" s="50"/>
+      <c r="T189" s="49"/>
       <c r="U189" s="50"/>
       <c r="V189" s="51"/>
       <c r="W189" s="43">
@@ -16999,7 +17356,7 @@
       <c r="P190" s="37"/>
       <c r="Q190" s="39"/>
       <c r="R190" s="39"/>
-      <c r="T190" s="50"/>
+      <c r="T190" s="49"/>
       <c r="U190" s="50"/>
       <c r="V190" s="51"/>
       <c r="W190" s="43">
@@ -17073,7 +17430,7 @@
       <c r="P191" s="37"/>
       <c r="Q191" s="39"/>
       <c r="R191" s="39"/>
-      <c r="T191" s="50"/>
+      <c r="T191" s="49"/>
       <c r="U191" s="50"/>
       <c r="V191" s="51"/>
       <c r="W191" s="43">
@@ -17147,7 +17504,7 @@
       <c r="P192" s="37"/>
       <c r="Q192" s="39"/>
       <c r="R192" s="39"/>
-      <c r="T192" s="50"/>
+      <c r="T192" s="49"/>
       <c r="U192" s="50"/>
       <c r="V192" s="51"/>
       <c r="W192" s="43">
@@ -17221,7 +17578,7 @@
       <c r="P193" s="37"/>
       <c r="Q193" s="39"/>
       <c r="R193" s="39"/>
-      <c r="T193" s="50"/>
+      <c r="T193" s="49"/>
       <c r="U193" s="50"/>
       <c r="V193" s="51"/>
       <c r="W193" s="43">
@@ -17295,7 +17652,7 @@
       <c r="P194" s="37"/>
       <c r="Q194" s="39"/>
       <c r="R194" s="39"/>
-      <c r="T194" s="50"/>
+      <c r="T194" s="49"/>
       <c r="U194" s="50"/>
       <c r="V194" s="51"/>
       <c r="W194" s="43">
@@ -17369,7 +17726,7 @@
       <c r="P195" s="37"/>
       <c r="Q195" s="39"/>
       <c r="R195" s="39"/>
-      <c r="T195" s="50"/>
+      <c r="T195" s="49"/>
       <c r="U195" s="50"/>
       <c r="V195" s="51"/>
       <c r="W195" s="43">
@@ -17443,7 +17800,7 @@
       <c r="P196" s="37"/>
       <c r="Q196" s="39"/>
       <c r="R196" s="39"/>
-      <c r="T196" s="50"/>
+      <c r="T196" s="49"/>
       <c r="U196" s="50"/>
       <c r="V196" s="51"/>
       <c r="W196" s="43">
@@ -17517,7 +17874,7 @@
       <c r="P197" s="37"/>
       <c r="Q197" s="39"/>
       <c r="R197" s="39"/>
-      <c r="T197" s="50"/>
+      <c r="T197" s="49"/>
       <c r="U197" s="50"/>
       <c r="V197" s="51"/>
       <c r="W197" s="43">
@@ -17591,7 +17948,7 @@
       <c r="P198" s="37"/>
       <c r="Q198" s="39"/>
       <c r="R198" s="39"/>
-      <c r="T198" s="50"/>
+      <c r="T198" s="49"/>
       <c r="U198" s="50"/>
       <c r="V198" s="51"/>
       <c r="W198" s="43">
@@ -17665,7 +18022,7 @@
       <c r="P199" s="37"/>
       <c r="Q199" s="39"/>
       <c r="R199" s="39"/>
-      <c r="T199" s="50"/>
+      <c r="T199" s="49"/>
       <c r="U199" s="50"/>
       <c r="V199" s="51"/>
       <c r="W199" s="43">
@@ -17739,7 +18096,7 @@
       <c r="P200" s="37"/>
       <c r="Q200" s="39"/>
       <c r="R200" s="39"/>
-      <c r="T200" s="50"/>
+      <c r="T200" s="49"/>
       <c r="U200" s="50"/>
       <c r="V200" s="51"/>
       <c r="W200" s="43">
@@ -17813,7 +18170,7 @@
       <c r="P201" s="37"/>
       <c r="Q201" s="39"/>
       <c r="R201" s="39"/>
-      <c r="T201" s="50"/>
+      <c r="T201" s="49"/>
       <c r="U201" s="50"/>
       <c r="V201" s="51"/>
       <c r="W201" s="43">
@@ -17887,7 +18244,7 @@
       <c r="P202" s="37"/>
       <c r="Q202" s="39"/>
       <c r="R202" s="39"/>
-      <c r="T202" s="50"/>
+      <c r="T202" s="49"/>
       <c r="U202" s="50"/>
       <c r="V202" s="51"/>
       <c r="W202" s="43">
@@ -17961,7 +18318,7 @@
       <c r="P203" s="37"/>
       <c r="Q203" s="39"/>
       <c r="R203" s="39"/>
-      <c r="T203" s="50"/>
+      <c r="T203" s="49"/>
       <c r="U203" s="50"/>
       <c r="V203" s="51"/>
       <c r="W203" s="43">
@@ -18035,7 +18392,7 @@
       <c r="P204" s="37"/>
       <c r="Q204" s="39"/>
       <c r="R204" s="39"/>
-      <c r="T204" s="50"/>
+      <c r="T204" s="49"/>
       <c r="U204" s="50"/>
       <c r="V204" s="51"/>
       <c r="W204" s="43">
@@ -18109,7 +18466,7 @@
       <c r="P205" s="37"/>
       <c r="Q205" s="39"/>
       <c r="R205" s="39"/>
-      <c r="T205" s="50"/>
+      <c r="T205" s="49"/>
       <c r="U205" s="50"/>
       <c r="V205" s="51"/>
       <c r="W205" s="43">
@@ -18183,7 +18540,7 @@
       <c r="P206" s="37"/>
       <c r="Q206" s="39"/>
       <c r="R206" s="39"/>
-      <c r="T206" s="50"/>
+      <c r="T206" s="49"/>
       <c r="U206" s="50"/>
       <c r="V206" s="51"/>
       <c r="W206" s="43">
@@ -18257,7 +18614,7 @@
       <c r="P207" s="37"/>
       <c r="Q207" s="39"/>
       <c r="R207" s="39"/>
-      <c r="T207" s="50"/>
+      <c r="T207" s="49"/>
       <c r="U207" s="50"/>
       <c r="V207" s="51"/>
       <c r="W207" s="43">
@@ -18331,7 +18688,7 @@
       <c r="P208" s="37"/>
       <c r="Q208" s="39"/>
       <c r="R208" s="39"/>
-      <c r="T208" s="50"/>
+      <c r="T208" s="49"/>
       <c r="U208" s="50"/>
       <c r="V208" s="51"/>
       <c r="W208" s="43">
@@ -18405,7 +18762,7 @@
       <c r="P209" s="37"/>
       <c r="Q209" s="39"/>
       <c r="R209" s="39"/>
-      <c r="T209" s="50"/>
+      <c r="T209" s="49"/>
       <c r="U209" s="50"/>
       <c r="V209" s="51"/>
       <c r="W209" s="43">
@@ -18479,7 +18836,7 @@
       <c r="P210" s="37"/>
       <c r="Q210" s="39"/>
       <c r="R210" s="39"/>
-      <c r="T210" s="50"/>
+      <c r="T210" s="49"/>
       <c r="U210" s="50"/>
       <c r="V210" s="51"/>
       <c r="W210" s="43">
@@ -18553,7 +18910,7 @@
       <c r="P211" s="37"/>
       <c r="Q211" s="39"/>
       <c r="R211" s="39"/>
-      <c r="T211" s="50"/>
+      <c r="T211" s="49"/>
       <c r="U211" s="50"/>
       <c r="V211" s="51"/>
       <c r="W211" s="43">
@@ -18627,7 +18984,7 @@
       <c r="P212" s="37"/>
       <c r="Q212" s="39"/>
       <c r="R212" s="39"/>
-      <c r="T212" s="50"/>
+      <c r="T212" s="49"/>
       <c r="U212" s="50"/>
       <c r="V212" s="51"/>
       <c r="W212" s="43">
@@ -18701,7 +19058,7 @@
       <c r="P213" s="37"/>
       <c r="Q213" s="39"/>
       <c r="R213" s="39"/>
-      <c r="T213" s="50"/>
+      <c r="T213" s="49"/>
       <c r="U213" s="50"/>
       <c r="V213" s="51"/>
       <c r="W213" s="43">
@@ -18775,7 +19132,7 @@
       <c r="P214" s="37"/>
       <c r="Q214" s="39"/>
       <c r="R214" s="39"/>
-      <c r="T214" s="50"/>
+      <c r="T214" s="49"/>
       <c r="U214" s="50"/>
       <c r="V214" s="51"/>
       <c r="W214" s="43">
@@ -18849,7 +19206,7 @@
       <c r="P215" s="37"/>
       <c r="Q215" s="39"/>
       <c r="R215" s="39"/>
-      <c r="T215" s="50"/>
+      <c r="T215" s="49"/>
       <c r="U215" s="50"/>
       <c r="V215" s="51"/>
       <c r="W215" s="43">
@@ -18923,7 +19280,7 @@
       <c r="P216" s="37"/>
       <c r="Q216" s="39"/>
       <c r="R216" s="39"/>
-      <c r="T216" s="50"/>
+      <c r="T216" s="49"/>
       <c r="U216" s="50"/>
       <c r="V216" s="51"/>
       <c r="W216" s="43">
@@ -18997,7 +19354,7 @@
       <c r="P217" s="37"/>
       <c r="Q217" s="39"/>
       <c r="R217" s="39"/>
-      <c r="T217" s="50"/>
+      <c r="T217" s="49"/>
       <c r="U217" s="50"/>
       <c r="V217" s="51"/>
       <c r="W217" s="43">
@@ -19071,7 +19428,7 @@
       <c r="P218" s="37"/>
       <c r="Q218" s="39"/>
       <c r="R218" s="39"/>
-      <c r="T218" s="50"/>
+      <c r="T218" s="49"/>
       <c r="U218" s="50"/>
       <c r="V218" s="51"/>
       <c r="W218" s="43">
@@ -19145,7 +19502,7 @@
       <c r="P219" s="37"/>
       <c r="Q219" s="39"/>
       <c r="R219" s="39"/>
-      <c r="T219" s="50"/>
+      <c r="T219" s="49"/>
       <c r="U219" s="50"/>
       <c r="V219" s="51"/>
       <c r="W219" s="43">
@@ -19219,7 +19576,7 @@
       <c r="P220" s="37"/>
       <c r="Q220" s="39"/>
       <c r="R220" s="39"/>
-      <c r="T220" s="50"/>
+      <c r="T220" s="49"/>
       <c r="U220" s="50"/>
       <c r="V220" s="51"/>
       <c r="W220" s="43">
@@ -19293,7 +19650,7 @@
       <c r="P221" s="37"/>
       <c r="Q221" s="39"/>
       <c r="R221" s="39"/>
-      <c r="T221" s="50"/>
+      <c r="T221" s="49"/>
       <c r="U221" s="50"/>
       <c r="V221" s="51"/>
       <c r="W221" s="43">
@@ -19367,7 +19724,7 @@
       <c r="P222" s="37"/>
       <c r="Q222" s="39"/>
       <c r="R222" s="39"/>
-      <c r="T222" s="50"/>
+      <c r="T222" s="49"/>
       <c r="U222" s="50"/>
       <c r="V222" s="51"/>
       <c r="W222" s="43">
@@ -19441,7 +19798,7 @@
       <c r="P223" s="37"/>
       <c r="Q223" s="39"/>
       <c r="R223" s="39"/>
-      <c r="T223" s="50"/>
+      <c r="T223" s="49"/>
       <c r="U223" s="50"/>
       <c r="V223" s="51"/>
       <c r="W223" s="43">
@@ -19515,7 +19872,7 @@
       <c r="P224" s="37"/>
       <c r="Q224" s="39"/>
       <c r="R224" s="39"/>
-      <c r="T224" s="50"/>
+      <c r="T224" s="49"/>
       <c r="U224" s="50"/>
       <c r="V224" s="51"/>
       <c r="W224" s="43">
@@ -19589,7 +19946,7 @@
       <c r="P225" s="37"/>
       <c r="Q225" s="39"/>
       <c r="R225" s="39"/>
-      <c r="T225" s="50"/>
+      <c r="T225" s="49"/>
       <c r="U225" s="50"/>
       <c r="V225" s="51"/>
       <c r="W225" s="43">
@@ -19663,7 +20020,7 @@
       <c r="P226" s="37"/>
       <c r="Q226" s="39"/>
       <c r="R226" s="39"/>
-      <c r="T226" s="50"/>
+      <c r="T226" s="49"/>
       <c r="U226" s="50"/>
       <c r="V226" s="51"/>
       <c r="W226" s="43">
@@ -19737,7 +20094,7 @@
       <c r="P227" s="37"/>
       <c r="Q227" s="39"/>
       <c r="R227" s="39"/>
-      <c r="T227" s="50"/>
+      <c r="T227" s="49"/>
       <c r="U227" s="50"/>
       <c r="V227" s="51"/>
       <c r="W227" s="43">
@@ -19811,7 +20168,7 @@
       <c r="P228" s="37"/>
       <c r="Q228" s="39"/>
       <c r="R228" s="39"/>
-      <c r="T228" s="50"/>
+      <c r="T228" s="49"/>
       <c r="U228" s="50"/>
       <c r="V228" s="51"/>
       <c r="W228" s="43">
@@ -19885,7 +20242,7 @@
       <c r="P229" s="37"/>
       <c r="Q229" s="39"/>
       <c r="R229" s="39"/>
-      <c r="T229" s="50"/>
+      <c r="T229" s="49"/>
       <c r="U229" s="50"/>
       <c r="V229" s="51"/>
       <c r="W229" s="43">
@@ -19959,7 +20316,7 @@
       <c r="P230" s="37"/>
       <c r="Q230" s="39"/>
       <c r="R230" s="39"/>
-      <c r="T230" s="50"/>
+      <c r="T230" s="49"/>
       <c r="U230" s="50"/>
       <c r="V230" s="51"/>
       <c r="W230" s="43">
@@ -20033,7 +20390,7 @@
       <c r="P231" s="37"/>
       <c r="Q231" s="39"/>
       <c r="R231" s="39"/>
-      <c r="T231" s="50"/>
+      <c r="T231" s="49"/>
       <c r="U231" s="50"/>
       <c r="V231" s="51"/>
       <c r="W231" s="43">
@@ -20107,7 +20464,7 @@
       <c r="P232" s="37"/>
       <c r="Q232" s="39"/>
       <c r="R232" s="39"/>
-      <c r="T232" s="50"/>
+      <c r="T232" s="49"/>
       <c r="U232" s="50"/>
       <c r="V232" s="51"/>
       <c r="W232" s="43">
@@ -20181,7 +20538,7 @@
       <c r="P233" s="37"/>
       <c r="Q233" s="39"/>
       <c r="R233" s="39"/>
-      <c r="T233" s="50"/>
+      <c r="T233" s="49"/>
       <c r="U233" s="50"/>
       <c r="V233" s="51"/>
       <c r="W233" s="43">
@@ -20255,7 +20612,7 @@
       <c r="P234" s="37"/>
       <c r="Q234" s="39"/>
       <c r="R234" s="39"/>
-      <c r="T234" s="50"/>
+      <c r="T234" s="49"/>
       <c r="U234" s="50"/>
       <c r="V234" s="51"/>
       <c r="W234" s="43">
@@ -20329,7 +20686,7 @@
       <c r="P235" s="37"/>
       <c r="Q235" s="39"/>
       <c r="R235" s="39"/>
-      <c r="T235" s="50"/>
+      <c r="T235" s="49"/>
       <c r="U235" s="50"/>
       <c r="V235" s="51"/>
       <c r="W235" s="43">
@@ -20403,7 +20760,7 @@
       <c r="P236" s="37"/>
       <c r="Q236" s="39"/>
       <c r="R236" s="39"/>
-      <c r="T236" s="50"/>
+      <c r="T236" s="49"/>
       <c r="U236" s="50"/>
       <c r="V236" s="51"/>
       <c r="W236" s="43">
@@ -20477,7 +20834,7 @@
       <c r="P237" s="37"/>
       <c r="Q237" s="39"/>
       <c r="R237" s="39"/>
-      <c r="T237" s="50"/>
+      <c r="T237" s="49"/>
       <c r="U237" s="50"/>
       <c r="V237" s="51"/>
       <c r="W237" s="43">
@@ -20551,7 +20908,7 @@
       <c r="P238" s="37"/>
       <c r="Q238" s="39"/>
       <c r="R238" s="39"/>
-      <c r="T238" s="50"/>
+      <c r="T238" s="49"/>
       <c r="U238" s="50"/>
       <c r="V238" s="51"/>
       <c r="W238" s="43">

</xml_diff>

<commit_message>
Gastos y ganancias martes
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="309">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -943,6 +943,15 @@
   <si>
     <t>Lalo Boletos Devolucion</t>
   </si>
+  <si>
+    <t xml:space="preserve"> Pago Semanal</t>
+  </si>
+  <si>
+    <t>Codigo Arreglado</t>
+  </si>
+  <si>
+    <t>Edgar Alitas</t>
+  </si>
 </sst>
 </file>
 
@@ -1751,8 +1760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2020,7 +2029,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>35459.229999999996</v>
+        <v>35667.729999999996</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -2068,7 +2077,7 @@
       </c>
       <c r="BA4" s="60">
         <f>(SUM((AP3:AP519)))-(SUM((AT3:AT519)))</f>
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="BB4" s="60"/>
     </row>
@@ -2165,7 +2174,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>340</v>
+        <v>448.5</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -2241,12 +2250,12 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>2340</v>
+        <v>2548.5</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
         <f>(SUM(R11:R499))-(SUM(E11:E500))</f>
-        <v>2000</v>
+        <v>2100</v>
       </c>
       <c r="Q7" s="58"/>
       <c r="R7" s="58"/>
@@ -5426,11 +5435,21 @@
       <c r="L39" s="66">
         <v>0</v>
       </c>
-      <c r="N39" s="37"/>
-      <c r="O39" s="37"/>
-      <c r="P39" s="37"/>
-      <c r="Q39" s="39"/>
-      <c r="R39" s="39"/>
+      <c r="N39" s="38">
+        <v>43019</v>
+      </c>
+      <c r="O39" s="37" t="s">
+        <v>278</v>
+      </c>
+      <c r="P39" s="37" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q39" s="39">
+        <v>250</v>
+      </c>
+      <c r="R39" s="39">
+        <v>100</v>
+      </c>
       <c r="T39" s="49">
         <v>42991</v>
       </c>
@@ -8010,10 +8029,12 @@
       <c r="U66" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="V66" s="51"/>
+      <c r="V66" s="51" t="s">
+        <v>307</v>
+      </c>
       <c r="W66" s="43">
         <f t="shared" si="3"/>
-        <v>67.5</v>
+        <v>-54</v>
       </c>
       <c r="X66" s="52">
         <v>80</v>
@@ -8021,10 +8042,19 @@
       <c r="Y66" s="52"/>
       <c r="AA66" s="53">
         <f t="shared" si="0"/>
-        <v>12.5</v>
+        <v>134</v>
+      </c>
+      <c r="AB66">
+        <v>64</v>
+      </c>
+      <c r="AC66" t="s">
+        <v>150</v>
+      </c>
+      <c r="AD66" t="s">
+        <v>211</v>
       </c>
       <c r="AE66">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="AF66">
         <v>0</v>
@@ -8055,11 +8085,20 @@
       </c>
       <c r="AO66">
         <f t="shared" si="1"/>
-        <v>12.5</v>
+        <v>62.5</v>
+      </c>
+      <c r="AP66">
+        <v>50</v>
+      </c>
+      <c r="AQ66">
+        <v>2</v>
+      </c>
+      <c r="AS66">
+        <v>1</v>
       </c>
       <c r="AT66">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AV66">
         <f t="shared" si="4"/>
@@ -8093,12 +8132,16 @@
       <c r="U67" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="V67" s="51"/>
+      <c r="V67" s="51" t="s">
+        <v>308</v>
+      </c>
       <c r="W67" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X67" s="52"/>
+        <v>80</v>
+      </c>
+      <c r="X67" s="52">
+        <v>80</v>
+      </c>
       <c r="Y67" s="52"/>
       <c r="AA67" s="53">
         <f t="shared" ref="AA67:AA130" si="8">SUM(AB67,AE67,AF67,AG67,AH67,AI67,AJ67,AK67,AL67,AM67,AN67,AO67)</f>

</xml_diff>

<commit_message>
Gastos del miercoles por la tarde
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="311">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -950,7 +950,13 @@
     <t>Codigo Arreglado</t>
   </si>
   <si>
-    <t>Edgar Alitas</t>
+    <t>Alitas Edgar&amp;Jaime</t>
+  </si>
+  <si>
+    <t>Alitas JaimeEdgar</t>
+  </si>
+  <si>
+    <t>Solo Emilio</t>
   </si>
 </sst>
 </file>
@@ -1760,8 +1766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2029,7 +2035,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>35667.729999999996</v>
+        <v>35462.729999999996</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -2077,7 +2083,7 @@
       </c>
       <c r="BA4" s="60">
         <f>(SUM((AP3:AP519)))-(SUM((AT3:AT519)))</f>
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="BB4" s="60"/>
     </row>
@@ -2174,7 +2180,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>448.5</v>
+        <v>243.5</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -2250,7 +2256,7 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>2548.5</v>
+        <v>2343.5</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
@@ -8133,11 +8139,11 @@
         <v>96</v>
       </c>
       <c r="V67" s="51" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="W67" s="43">
         <f t="shared" si="3"/>
-        <v>80</v>
+        <v>-192.5</v>
       </c>
       <c r="X67" s="52">
         <v>80</v>
@@ -8145,10 +8151,19 @@
       <c r="Y67" s="52"/>
       <c r="AA67" s="53">
         <f t="shared" ref="AA67:AA130" si="8">SUM(AB67,AE67,AF67,AG67,AH67,AI67,AJ67,AK67,AL67,AM67,AN67,AO67)</f>
-        <v>0</v>
+        <v>272.5</v>
+      </c>
+      <c r="AB67">
+        <v>60</v>
+      </c>
+      <c r="AC67" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD67" t="s">
+        <v>308</v>
       </c>
       <c r="AE67">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="AF67">
         <v>0</v>
@@ -8179,15 +8194,21 @@
       </c>
       <c r="AO67">
         <f t="shared" ref="AO67:AO130" si="9">SUM(AP67,AW67,AV67)</f>
-        <v>0</v>
+        <v>12.5</v>
+      </c>
+      <c r="AS67">
+        <v>1</v>
       </c>
       <c r="AT67">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AV67">
         <f t="shared" si="4"/>
         <v>0</v>
+      </c>
+      <c r="AW67">
+        <v>12.5</v>
       </c>
     </row>
     <row r="68" spans="3:49" x14ac:dyDescent="0.25">
@@ -8214,16 +8235,20 @@
       <c r="U68" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="V68" s="51"/>
+      <c r="V68" s="51" t="s">
+        <v>310</v>
+      </c>
       <c r="W68" s="43">
         <f t="shared" ref="W68:W131" si="10">(SUM(X68,Y68))-AA68</f>
-        <v>0</v>
-      </c>
-      <c r="X68" s="52"/>
+        <v>67.5</v>
+      </c>
+      <c r="X68" s="52">
+        <v>80</v>
+      </c>
       <c r="Y68" s="52"/>
       <c r="AA68" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="AE68">
         <v>0</v>
@@ -8257,15 +8282,24 @@
       </c>
       <c r="AO68">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>12.5</v>
+      </c>
+      <c r="AQ68">
+        <v>2</v>
+      </c>
+      <c r="AS68">
+        <v>1</v>
       </c>
       <c r="AT68">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AV68">
         <f t="shared" ref="AV68:AV131" si="11">AU68*5</f>
         <v>0</v>
+      </c>
+      <c r="AW68">
+        <v>12.5</v>
       </c>
     </row>
     <row r="69" spans="3:49" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finanzas fin de semana
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="318">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -958,6 +958,27 @@
   <si>
     <t>Solo Emilio</t>
   </si>
+  <si>
+    <t>Café Sabado Cine</t>
+  </si>
+  <si>
+    <t>Friki Plaza</t>
+  </si>
+  <si>
+    <t>No estaba el juego</t>
+  </si>
+  <si>
+    <t>Pizzas Jaime</t>
+  </si>
+  <si>
+    <t>BladeRunner 2049</t>
+  </si>
+  <si>
+    <t>Carls Junior</t>
+  </si>
+  <si>
+    <t>Pizzas copilco</t>
+  </si>
 </sst>
 </file>
 
@@ -1766,8 +1787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1961,7 +1982,7 @@
       </c>
       <c r="L3" s="26">
         <f>(SUM(C2,(E11:E500)))-(SUM((D11:D500),(C11:C500)))</f>
-        <v>10619.23</v>
+        <v>10581.23</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -2035,7 +2056,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>35462.729999999996</v>
+        <v>35203.729999999996</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -2180,7 +2201,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>243.5</v>
+        <v>22.5</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -2256,7 +2277,7 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>2343.5</v>
+        <v>2122.5</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
@@ -4212,8 +4233,16 @@
       </c>
     </row>
     <row r="28" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A28" s="33">
+        <v>43022</v>
+      </c>
+      <c r="B28" t="s">
+        <v>311</v>
+      </c>
       <c r="C28" s="13"/>
-      <c r="D28" s="12"/>
+      <c r="D28" s="12">
+        <v>38</v>
+      </c>
       <c r="E28" s="14"/>
       <c r="G28" s="60" t="s">
         <v>73</v>
@@ -5558,11 +5587,17 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="N40" s="37"/>
-      <c r="O40" s="37"/>
+      <c r="N40" s="38">
+        <v>43022</v>
+      </c>
+      <c r="O40" s="37" t="s">
+        <v>312</v>
+      </c>
       <c r="P40" s="37"/>
       <c r="Q40" s="39"/>
-      <c r="R40" s="39"/>
+      <c r="R40" s="39">
+        <v>-2100</v>
+      </c>
       <c r="T40" s="49">
         <v>42992</v>
       </c>
@@ -5651,11 +5686,17 @@
         <f t="shared" si="7"/>
         <v>1000</v>
       </c>
-      <c r="N41" s="37"/>
-      <c r="O41" s="37"/>
+      <c r="N41" s="38">
+        <v>43022</v>
+      </c>
+      <c r="O41" s="37" t="s">
+        <v>313</v>
+      </c>
       <c r="P41" s="37"/>
       <c r="Q41" s="39"/>
-      <c r="R41" s="39"/>
+      <c r="R41" s="39">
+        <v>2100</v>
+      </c>
       <c r="T41" s="49">
         <v>42993</v>
       </c>
@@ -6928,13 +6969,13 @@
       </c>
       <c r="W54" s="43">
         <f t="shared" si="3"/>
-        <v>-45</v>
+        <v>-5</v>
       </c>
       <c r="X54" s="52">
         <v>80</v>
       </c>
       <c r="Y54" s="101">
-        <v>31.5</v>
+        <v>71.5</v>
       </c>
       <c r="AA54" s="53">
         <f t="shared" si="0"/>
@@ -8240,7 +8281,7 @@
       </c>
       <c r="W68" s="43">
         <f t="shared" ref="W68:W131" si="10">(SUM(X68,Y68))-AA68</f>
-        <v>67.5</v>
+        <v>7.5</v>
       </c>
       <c r="X68" s="52">
         <v>80</v>
@@ -8248,10 +8289,19 @@
       <c r="Y68" s="52"/>
       <c r="AA68" s="53">
         <f t="shared" si="8"/>
-        <v>12.5</v>
+        <v>72.5</v>
+      </c>
+      <c r="AB68">
+        <v>50</v>
+      </c>
+      <c r="AC68" t="s">
+        <v>150</v>
+      </c>
+      <c r="AD68" t="s">
+        <v>152</v>
       </c>
       <c r="AE68">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AF68">
         <v>0</v>
@@ -8326,19 +8376,32 @@
       <c r="U69" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="V69" s="51"/>
+      <c r="V69" s="51" t="s">
+        <v>314</v>
+      </c>
       <c r="W69" s="43">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X69" s="52"/>
+        <v>-192.5</v>
+      </c>
+      <c r="X69" s="52">
+        <v>80</v>
+      </c>
       <c r="Y69" s="52"/>
       <c r="AA69" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>272.5</v>
+      </c>
+      <c r="AB69">
+        <v>240</v>
+      </c>
+      <c r="AC69" t="s">
+        <v>317</v>
+      </c>
+      <c r="AD69" t="s">
+        <v>152</v>
       </c>
       <c r="AE69">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AF69">
         <v>0</v>
@@ -8369,15 +8432,21 @@
       </c>
       <c r="AO69">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>22.5</v>
       </c>
       <c r="AT69">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="AU69">
+        <v>2</v>
+      </c>
       <c r="AV69">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="AW69">
+        <v>12.5</v>
       </c>
     </row>
     <row r="70" spans="3:49" x14ac:dyDescent="0.25">
@@ -8404,16 +8473,26 @@
       <c r="U70" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="V70" s="51"/>
+      <c r="V70" s="51" t="s">
+        <v>315</v>
+      </c>
       <c r="W70" s="43">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X70" s="52"/>
+        <v>-8.5</v>
+      </c>
+      <c r="X70" s="52">
+        <v>120</v>
+      </c>
       <c r="Y70" s="52"/>
       <c r="AA70" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>128.5</v>
+      </c>
+      <c r="AB70">
+        <v>100</v>
+      </c>
+      <c r="AC70" t="s">
+        <v>316</v>
       </c>
       <c r="AE70">
         <v>0</v>
@@ -8447,15 +8526,21 @@
       </c>
       <c r="AO70">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>28.5</v>
       </c>
       <c r="AT70">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="AU70">
+        <v>2</v>
+      </c>
       <c r="AV70">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="AW70">
+        <v>18.5</v>
       </c>
     </row>
     <row r="71" spans="3:49" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Gastos hasta el martes
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="321">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -979,6 +979,15 @@
   <si>
     <t>Pizzas copilco</t>
   </si>
+  <si>
+    <t>Plática Pablo Gómez</t>
+  </si>
+  <si>
+    <t>Clases ingles maratónica</t>
+  </si>
+  <si>
+    <t>Jaime invitó Mariscos</t>
+  </si>
 </sst>
 </file>
 
@@ -1787,8 +1796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="J54" workbookViewId="0">
+      <selection activeCell="V73" sqref="V73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,7 +2065,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>35203.729999999996</v>
+        <v>35629.229999999996</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -2104,7 +2113,7 @@
       </c>
       <c r="BA4" s="60">
         <f>(SUM((AP3:AP519)))-(SUM((AT3:AT519)))</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="BB4" s="60"/>
     </row>
@@ -2201,7 +2210,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>22.5</v>
+        <v>248</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -2277,12 +2286,12 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>2122.5</v>
+        <v>2548</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
         <f>(SUM(R11:R499))-(SUM(E11:E500))</f>
-        <v>2100</v>
+        <v>2300</v>
       </c>
       <c r="Q7" s="58"/>
       <c r="R7" s="58"/>
@@ -5801,11 +5810,19 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="N42" s="37"/>
-      <c r="O42" s="37"/>
+      <c r="N42" s="38">
+        <v>43025</v>
+      </c>
+      <c r="O42" s="37" t="s">
+        <v>170</v>
+      </c>
       <c r="P42" s="37"/>
-      <c r="Q42" s="39"/>
-      <c r="R42" s="39"/>
+      <c r="Q42" s="39">
+        <v>300</v>
+      </c>
+      <c r="R42" s="39">
+        <v>200</v>
+      </c>
       <c r="T42" s="49">
         <v>42994</v>
       </c>
@@ -8645,19 +8662,32 @@
       <c r="U72" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="V72" s="51"/>
+      <c r="V72" s="51" t="s">
+        <v>318</v>
+      </c>
       <c r="W72" s="43">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X72" s="52"/>
+        <v>51.5</v>
+      </c>
+      <c r="X72" s="52">
+        <v>120</v>
+      </c>
       <c r="Y72" s="52"/>
       <c r="AA72" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>68.5</v>
+      </c>
+      <c r="AB72">
+        <v>0</v>
+      </c>
+      <c r="AC72" t="s">
+        <v>320</v>
+      </c>
+      <c r="AD72" t="s">
+        <v>256</v>
       </c>
       <c r="AE72">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AF72">
         <v>0</v>
@@ -8688,15 +8718,24 @@
       </c>
       <c r="AO72">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>62.5</v>
+      </c>
+      <c r="AP72">
+        <v>50</v>
+      </c>
+      <c r="AS72">
+        <v>1</v>
       </c>
       <c r="AT72">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AV72">
         <f t="shared" si="11"/>
         <v>0</v>
+      </c>
+      <c r="AW72">
+        <v>12.5</v>
       </c>
     </row>
     <row r="73" spans="3:49" x14ac:dyDescent="0.25">
@@ -8723,16 +8762,20 @@
       <c r="U73" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="V73" s="51"/>
+      <c r="V73" s="51" t="s">
+        <v>319</v>
+      </c>
       <c r="W73" s="43">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X73" s="52"/>
+        <v>74</v>
+      </c>
+      <c r="X73" s="52">
+        <v>80</v>
+      </c>
       <c r="Y73" s="52"/>
       <c r="AA73" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AE73">
         <v>0</v>
@@ -8766,15 +8809,24 @@
       </c>
       <c r="AO73">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="AQ73">
+        <v>4</v>
+      </c>
+      <c r="AS73">
+        <v>4</v>
       </c>
       <c r="AT73">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="AV73">
         <f t="shared" si="11"/>
         <v>0</v>
+      </c>
+      <c r="AW73">
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="3:49" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Gastos de transporte en martes
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1796,8 +1796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J54" workbookViewId="0">
-      <selection activeCell="V73" sqref="V73"/>
+    <sheetView tabSelected="1" topLeftCell="P39" workbookViewId="0">
+      <selection activeCell="X74" sqref="X74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>35629.229999999996</v>
+        <v>35695.729999999996</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -2210,7 +2210,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>248</v>
+        <v>314.5</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -2286,7 +2286,7 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>2548</v>
+        <v>2614.5</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
@@ -8856,13 +8856,15 @@
       <c r="V74" s="51"/>
       <c r="W74" s="43">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X74" s="52"/>
+        <v>66.5</v>
+      </c>
+      <c r="X74" s="52">
+        <v>80</v>
+      </c>
       <c r="Y74" s="52"/>
       <c r="AA74" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>13.5</v>
       </c>
       <c r="AE74">
         <v>0</v>
@@ -8896,7 +8898,7 @@
       </c>
       <c r="AO74">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>13.5</v>
       </c>
       <c r="AT74">
         <f t="shared" si="6"/>
@@ -8905,6 +8907,9 @@
       <c r="AV74">
         <f t="shared" si="11"/>
         <v>0</v>
+      </c>
+      <c r="AW74">
+        <v>13.5</v>
       </c>
     </row>
     <row r="75" spans="3:49" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Gastos del miercoles al lunes
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="335">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -917,9 +917,6 @@
     <t>Netflix  (Sept,2016-Oct,2017)</t>
   </si>
   <si>
-    <t>Oct,2017</t>
-  </si>
-  <si>
     <t>BladeRunner Original</t>
   </si>
   <si>
@@ -987,6 +984,51 @@
   </si>
   <si>
     <t>Jaime invitó Mariscos</t>
+  </si>
+  <si>
+    <t>Jaime invitó IHOP</t>
+  </si>
+  <si>
+    <t>Sushi Buffete</t>
+  </si>
+  <si>
+    <t>Café con Pan de Muerto</t>
+  </si>
+  <si>
+    <t>Café con Ale</t>
+  </si>
+  <si>
+    <t>Seminario Python</t>
+  </si>
+  <si>
+    <t>Ale Consejos de Celular 1</t>
+  </si>
+  <si>
+    <t>Tía de Jaime</t>
+  </si>
+  <si>
+    <t>Buscando Juego en la FrikiPlaza</t>
+  </si>
+  <si>
+    <t>PERDI EL CELULAR :C</t>
+  </si>
+  <si>
+    <t>Cervezas</t>
+  </si>
+  <si>
+    <t>China yo pagué; Maíz</t>
+  </si>
+  <si>
+    <t>Comida Tia Ivonne</t>
+  </si>
+  <si>
+    <t>Cooperacha Café</t>
+  </si>
+  <si>
+    <t>Revision Jaime Tesis</t>
+  </si>
+  <si>
+    <t>Oct, 2017</t>
   </si>
 </sst>
 </file>
@@ -1796,14 +1838,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P39" workbookViewId="0">
-      <selection activeCell="X74" sqref="X74"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="4" width="11.42578125" customWidth="1"/>
     <col min="9" max="9" width="25.28515625" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -2065,7 +2107,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>35695.729999999996</v>
+        <v>35583.229999999996</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -2113,7 +2155,7 @@
       </c>
       <c r="BA4" s="60">
         <f>(SUM((AP3:AP519)))-(SUM((AT3:AT519)))</f>
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="BB4" s="60"/>
     </row>
@@ -2210,7 +2252,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>314.5</v>
+        <v>202</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -2286,7 +2328,7 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>2614.5</v>
+        <v>2502</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
@@ -4246,7 +4288,7 @@
         <v>43022</v>
       </c>
       <c r="B28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="12">
@@ -5366,10 +5408,10 @@
         <v>43016</v>
       </c>
       <c r="O38" s="37" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P38" s="37" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="Q38" s="39">
         <v>200</v>
@@ -5486,7 +5528,7 @@
         <v>278</v>
       </c>
       <c r="P39" s="37" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q39" s="39">
         <v>250</v>
@@ -5600,7 +5642,7 @@
         <v>43022</v>
       </c>
       <c r="O40" s="37" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="P40" s="37"/>
       <c r="Q40" s="39"/>
@@ -5699,7 +5741,7 @@
         <v>43022</v>
       </c>
       <c r="O41" s="37" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="P41" s="37"/>
       <c r="Q41" s="39"/>
@@ -5917,10 +5959,16 @@
         <f t="shared" si="7"/>
         <v>3200</v>
       </c>
-      <c r="N43" s="37"/>
-      <c r="O43" s="37"/>
+      <c r="N43" s="38">
+        <v>43027</v>
+      </c>
+      <c r="O43" s="37" t="s">
+        <v>278</v>
+      </c>
       <c r="P43" s="37"/>
-      <c r="Q43" s="39"/>
+      <c r="Q43" s="39">
+        <v>250</v>
+      </c>
       <c r="R43" s="39"/>
       <c r="T43" s="49">
         <v>42995</v>
@@ -6307,7 +6355,7 @@
       <c r="D47" s="12"/>
       <c r="E47" s="14"/>
       <c r="G47" s="18" t="s">
-        <v>297</v>
+        <v>334</v>
       </c>
       <c r="H47" s="18" t="s">
         <v>29</v>
@@ -6402,22 +6450,22 @@
       <c r="C48" s="13"/>
       <c r="D48" s="12"/>
       <c r="E48" s="14"/>
-      <c r="G48" s="64">
+      <c r="G48" s="59">
         <v>43016</v>
       </c>
-      <c r="H48" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="I48" s="18" t="s">
+      <c r="H48" s="60" t="s">
+        <v>301</v>
+      </c>
+      <c r="I48" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="J48" s="23">
+      <c r="J48" s="62">
         <v>200</v>
       </c>
-      <c r="K48" s="22">
+      <c r="K48" s="65">
         <v>200</v>
       </c>
-      <c r="L48" s="20">
+      <c r="L48" s="66">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -7832,7 +7880,7 @@
         <v>93</v>
       </c>
       <c r="V63" s="51" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="W63" s="43">
         <f t="shared" si="3"/>
@@ -7850,10 +7898,10 @@
         <v>100</v>
       </c>
       <c r="AC63" t="s">
+        <v>298</v>
+      </c>
+      <c r="AD63" t="s">
         <v>299</v>
-      </c>
-      <c r="AD63" t="s">
-        <v>300</v>
       </c>
       <c r="AE63">
         <v>20</v>
@@ -7923,7 +7971,7 @@
         <v>94</v>
       </c>
       <c r="V64" s="51" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="W64" s="43">
         <f t="shared" si="3"/>
@@ -8003,7 +8051,7 @@
         <v>95</v>
       </c>
       <c r="V65" s="51" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="W65" s="43">
         <f t="shared" si="3"/>
@@ -8094,7 +8142,7 @@
         <v>91</v>
       </c>
       <c r="V66" s="51" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="W66" s="43">
         <f t="shared" si="3"/>
@@ -8197,7 +8245,7 @@
         <v>96</v>
       </c>
       <c r="V67" s="51" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="W67" s="43">
         <f t="shared" si="3"/>
@@ -8218,7 +8266,7 @@
         <v>116</v>
       </c>
       <c r="AD67" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AE67">
         <v>200</v>
@@ -8294,7 +8342,7 @@
         <v>55</v>
       </c>
       <c r="V68" s="51" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="W68" s="43">
         <f t="shared" ref="W68:W131" si="10">(SUM(X68,Y68))-AA68</f>
@@ -8394,7 +8442,7 @@
         <v>92</v>
       </c>
       <c r="V69" s="51" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="W69" s="43">
         <f t="shared" si="10"/>
@@ -8412,7 +8460,7 @@
         <v>240</v>
       </c>
       <c r="AC69" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AD69" t="s">
         <v>152</v>
@@ -8491,7 +8539,7 @@
         <v>93</v>
       </c>
       <c r="V70" s="51" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="W70" s="43">
         <f t="shared" si="10"/>
@@ -8509,7 +8557,7 @@
         <v>100</v>
       </c>
       <c r="AC70" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AE70">
         <v>0</v>
@@ -8663,7 +8711,7 @@
         <v>95</v>
       </c>
       <c r="V72" s="51" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="W72" s="43">
         <f t="shared" si="10"/>
@@ -8681,7 +8729,7 @@
         <v>0</v>
       </c>
       <c r="AC72" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AD72" t="s">
         <v>256</v>
@@ -8763,7 +8811,7 @@
         <v>91</v>
       </c>
       <c r="V73" s="51" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="W73" s="43">
         <f t="shared" si="10"/>
@@ -8776,6 +8824,9 @@
       <c r="AA73" s="53">
         <f t="shared" si="8"/>
         <v>6</v>
+      </c>
+      <c r="AB73">
+        <v>0</v>
       </c>
       <c r="AE73">
         <v>0</v>
@@ -8853,10 +8904,12 @@
       <c r="U74" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="V74" s="51"/>
+      <c r="V74" s="51" t="s">
+        <v>328</v>
+      </c>
       <c r="W74" s="43">
         <f t="shared" si="10"/>
-        <v>66.5</v>
+        <v>-73.5</v>
       </c>
       <c r="X74" s="52">
         <v>80</v>
@@ -8864,10 +8917,16 @@
       <c r="Y74" s="52"/>
       <c r="AA74" s="53">
         <f t="shared" si="8"/>
-        <v>13.5</v>
+        <v>153.5</v>
+      </c>
+      <c r="AB74">
+        <v>130</v>
+      </c>
+      <c r="AC74" t="s">
+        <v>330</v>
       </c>
       <c r="AE74">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AF74">
         <v>0</v>
@@ -8900,9 +8959,12 @@
         <f t="shared" si="9"/>
         <v>13.5</v>
       </c>
+      <c r="AS74">
+        <v>1</v>
+      </c>
       <c r="AT74">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AV74">
         <f t="shared" si="11"/>
@@ -8936,19 +8998,32 @@
       <c r="U75" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="V75" s="51"/>
+      <c r="V75" s="51" t="s">
+        <v>325</v>
+      </c>
       <c r="W75" s="43">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X75" s="52"/>
+        <v>-167.5</v>
+      </c>
+      <c r="X75" s="52">
+        <v>80</v>
+      </c>
       <c r="Y75" s="52"/>
       <c r="AA75" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>247.5</v>
+      </c>
+      <c r="AB75">
+        <v>70</v>
+      </c>
+      <c r="AC75" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD75" t="s">
+        <v>323</v>
       </c>
       <c r="AE75">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="AF75">
         <v>0</v>
@@ -8979,15 +9054,27 @@
       </c>
       <c r="AO75">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>37.5</v>
+      </c>
+      <c r="AP75">
+        <v>25</v>
+      </c>
+      <c r="AQ75">
+        <v>2</v>
+      </c>
+      <c r="AS75">
+        <v>3</v>
       </c>
       <c r="AT75">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AV75">
         <f t="shared" si="11"/>
         <v>0</v>
+      </c>
+      <c r="AW75">
+        <v>12.5</v>
       </c>
     </row>
     <row r="76" spans="3:49" x14ac:dyDescent="0.25">
@@ -9014,19 +9101,32 @@
       <c r="U76" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="V76" s="51"/>
+      <c r="V76" s="51" t="s">
+        <v>324</v>
+      </c>
       <c r="W76" s="43">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X76" s="52"/>
+        <v>47.5</v>
+      </c>
+      <c r="X76" s="52">
+        <v>80</v>
+      </c>
       <c r="Y76" s="52"/>
       <c r="AA76" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>32.5</v>
+      </c>
+      <c r="AB76">
+        <v>0</v>
+      </c>
+      <c r="AC76" t="s">
+        <v>320</v>
+      </c>
+      <c r="AD76" t="s">
+        <v>329</v>
       </c>
       <c r="AE76">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AF76">
         <v>0</v>
@@ -9057,15 +9157,21 @@
       </c>
       <c r="AO76">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>12.5</v>
+      </c>
+      <c r="AS76">
+        <v>3</v>
       </c>
       <c r="AT76">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AV76">
         <f t="shared" si="11"/>
         <v>0</v>
+      </c>
+      <c r="AW76">
+        <v>12.5</v>
       </c>
     </row>
     <row r="77" spans="3:49" x14ac:dyDescent="0.25">
@@ -9092,19 +9198,32 @@
       <c r="U77" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="V77" s="51"/>
+      <c r="V77" s="51" t="s">
+        <v>327</v>
+      </c>
       <c r="W77" s="43">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X77" s="52"/>
+        <v>-50</v>
+      </c>
+      <c r="X77" s="52">
+        <v>120</v>
+      </c>
       <c r="Y77" s="52"/>
       <c r="AA77" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>170</v>
+      </c>
+      <c r="AB77">
+        <v>120</v>
+      </c>
+      <c r="AC77" t="s">
+        <v>321</v>
+      </c>
+      <c r="AD77" t="s">
+        <v>322</v>
       </c>
       <c r="AE77">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="AF77">
         <v>0</v>
@@ -9137,9 +9256,12 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AS77">
+        <v>2</v>
+      </c>
       <c r="AT77">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AV77">
         <f t="shared" si="11"/>
@@ -9170,16 +9292,21 @@
       <c r="U78" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="V78" s="51"/>
+      <c r="V78" s="51" t="s">
+        <v>326</v>
+      </c>
       <c r="W78" s="43">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>-30</v>
       </c>
       <c r="X78" s="52"/>
       <c r="Y78" s="52"/>
       <c r="AA78" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="AC78" t="s">
+        <v>331</v>
       </c>
       <c r="AE78">
         <v>0</v>
@@ -9213,11 +9340,17 @@
       </c>
       <c r="AO78">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="AP78">
+        <v>30</v>
+      </c>
+      <c r="AS78">
+        <v>1</v>
       </c>
       <c r="AT78">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AV78">
         <f t="shared" si="11"/>
@@ -9245,23 +9378,38 @@
       <c r="T79" s="49">
         <v>43031</v>
       </c>
-      <c r="U79" s="50"/>
-      <c r="V79" s="51"/>
+      <c r="U79" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="V79" s="51" t="s">
+        <v>333</v>
+      </c>
       <c r="W79" s="43">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X79" s="52"/>
+        <v>-22.5</v>
+      </c>
+      <c r="X79" s="52">
+        <v>120</v>
+      </c>
       <c r="Y79" s="52"/>
       <c r="AA79" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>142.5</v>
+      </c>
+      <c r="AB79">
+        <v>70</v>
+      </c>
+      <c r="AC79" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD79" t="s">
+        <v>332</v>
       </c>
       <c r="AE79">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="AF79">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AG79">
         <v>0</v>
@@ -9289,15 +9437,21 @@
       </c>
       <c r="AO79">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>12.5</v>
+      </c>
+      <c r="AS79">
+        <v>1</v>
       </c>
       <c r="AT79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AV79">
         <f t="shared" si="11"/>
         <v>0</v>
+      </c>
+      <c r="AW79">
+        <v>12.5</v>
       </c>
     </row>
     <row r="80" spans="3:49" x14ac:dyDescent="0.25">
@@ -9321,7 +9475,9 @@
       <c r="T80" s="49">
         <v>43032</v>
       </c>
-      <c r="U80" s="50"/>
+      <c r="U80" s="50" t="s">
+        <v>91</v>
+      </c>
       <c r="V80" s="51"/>
       <c r="W80" s="43">
         <f t="shared" si="10"/>
@@ -9397,7 +9553,9 @@
       <c r="T81" s="49">
         <v>43033</v>
       </c>
-      <c r="U81" s="50"/>
+      <c r="U81" s="50" t="s">
+        <v>96</v>
+      </c>
       <c r="V81" s="51"/>
       <c r="W81" s="43">
         <f t="shared" si="10"/>
@@ -9473,7 +9631,9 @@
       <c r="T82" s="49">
         <v>43034</v>
       </c>
-      <c r="U82" s="50"/>
+      <c r="U82" s="50" t="s">
+        <v>55</v>
+      </c>
       <c r="V82" s="51"/>
       <c r="W82" s="43">
         <f t="shared" si="10"/>
@@ -9549,7 +9709,9 @@
       <c r="T83" s="49">
         <v>43035</v>
       </c>
-      <c r="U83" s="50"/>
+      <c r="U83" s="50" t="s">
+        <v>92</v>
+      </c>
       <c r="V83" s="51"/>
       <c r="W83" s="43">
         <f t="shared" si="10"/>
@@ -9625,7 +9787,9 @@
       <c r="T84" s="49">
         <v>43036</v>
       </c>
-      <c r="U84" s="50"/>
+      <c r="U84" s="50" t="s">
+        <v>93</v>
+      </c>
       <c r="V84" s="51"/>
       <c r="W84" s="43">
         <f t="shared" si="10"/>
@@ -9701,7 +9865,9 @@
       <c r="T85" s="49">
         <v>43037</v>
       </c>
-      <c r="U85" s="50"/>
+      <c r="U85" s="50" t="s">
+        <v>94</v>
+      </c>
       <c r="V85" s="51"/>
       <c r="W85" s="43">
         <f t="shared" si="10"/>

</xml_diff>

<commit_message>
Finanzas dias de asueto Jaime
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="366">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -1103,14 +1103,32 @@
     <t>Etrian Odyssey</t>
   </si>
   <si>
-    <t>Veterinario; Taxi</t>
+    <t>Jaime Boletos</t>
+  </si>
+  <si>
+    <t>Sushi + Propina</t>
+  </si>
+  <si>
+    <t>Wingstop + Propina</t>
+  </si>
+  <si>
+    <t>Starbucks</t>
+  </si>
+  <si>
+    <t>Veterinario; Taxix2;BoletosJaime;Bubulubu</t>
+  </si>
+  <si>
+    <t>American Gods</t>
+  </si>
+  <si>
+    <t>Seminario Alejandra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1251,6 +1269,13 @@
     <font>
       <sz val="11"/>
       <color theme="7" tint="0.79998168889431442"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1450,7 +1475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1626,6 +1651,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1922,9 +1948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M73" workbookViewId="0">
-      <selection activeCell="X111" sqref="X111"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2117,7 +2141,7 @@
       </c>
       <c r="L3" s="26">
         <f>(SUM(C2,(E11:E500)))-(SUM((D11:D500),(C11:C500)))</f>
-        <v>11590.23</v>
+        <v>9790.23</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -2191,7 +2215,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>36917.729999999996</v>
+        <v>34882.729999999996</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -2239,7 +2263,7 @@
       </c>
       <c r="BA4" s="60">
         <f>(SUM((AP3:AP519)))-(SUM((AT3:AT519)))</f>
-        <v>-39</v>
+        <v>-49</v>
       </c>
       <c r="BB4" s="60"/>
     </row>
@@ -2336,7 +2360,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>527.5</v>
+        <v>292.5</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -2412,7 +2436,7 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>1527.5</v>
+        <v>1292.5</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
@@ -4839,7 +4863,15 @@
       </c>
     </row>
     <row r="32" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="C32" s="13"/>
+      <c r="A32" s="33">
+        <v>43040</v>
+      </c>
+      <c r="B32" t="s">
+        <v>359</v>
+      </c>
+      <c r="C32" s="13">
+        <v>1800</v>
+      </c>
       <c r="D32" s="12"/>
       <c r="E32" s="14"/>
       <c r="G32" s="64">
@@ -10388,7 +10420,7 @@
       </c>
       <c r="W88" s="43">
         <f t="shared" si="10"/>
-        <v>-182</v>
+        <v>-2217</v>
       </c>
       <c r="X88" s="52">
         <v>80</v>
@@ -10396,10 +10428,16 @@
       <c r="Y88" s="52"/>
       <c r="AA88" s="53">
         <f t="shared" si="8"/>
-        <v>262</v>
+        <v>2297</v>
+      </c>
+      <c r="AB88">
+        <v>230</v>
+      </c>
+      <c r="AC88" t="s">
+        <v>360</v>
       </c>
       <c r="AD88" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="AE88">
         <v>200</v>
@@ -10410,11 +10448,11 @@
       <c r="AG88">
         <v>30</v>
       </c>
-      <c r="AH88">
-        <v>0</v>
+      <c r="AH88" s="105">
+        <v>1800</v>
       </c>
       <c r="AI88">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AJ88">
         <v>0</v>
@@ -10474,19 +10512,32 @@
       <c r="U89" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="V89" s="51"/>
+      <c r="V89" s="51" t="s">
+        <v>364</v>
+      </c>
       <c r="W89" s="43">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X89" s="52"/>
+        <f>(SUM(X89,Y89))-AA89</f>
+        <v>-80</v>
+      </c>
+      <c r="X89" s="52">
+        <v>80</v>
+      </c>
       <c r="Y89" s="52"/>
       <c r="AA89" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>160</v>
+      </c>
+      <c r="AB89">
+        <v>120</v>
+      </c>
+      <c r="AC89" t="s">
+        <v>361</v>
+      </c>
+      <c r="AD89" t="s">
+        <v>362</v>
       </c>
       <c r="AE89">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AF89">
         <v>0</v>
@@ -10519,9 +10570,12 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AS89">
+        <v>2</v>
+      </c>
       <c r="AT89">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AV89">
         <f t="shared" si="11"/>
@@ -10552,12 +10606,16 @@
       <c r="U90" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="V90" s="51"/>
+      <c r="V90" s="51" t="s">
+        <v>365</v>
+      </c>
       <c r="W90" s="43">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X90" s="52"/>
+        <v>80</v>
+      </c>
+      <c r="X90" s="52">
+        <v>80</v>
+      </c>
       <c r="Y90" s="52"/>
       <c r="AA90" s="53">
         <f t="shared" si="8"/>

</xml_diff>

<commit_message>
Gastos de fin de semana
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="373">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -1123,6 +1123,27 @@
   <si>
     <t>Seminario Alejandra</t>
   </si>
+  <si>
+    <t>Celular para su mamá</t>
+  </si>
+  <si>
+    <t>Batería iPhone</t>
+  </si>
+  <si>
+    <t>Tía Emma</t>
+  </si>
+  <si>
+    <t>Pan de muerto</t>
+  </si>
+  <si>
+    <t>Palomitas y Café</t>
+  </si>
+  <si>
+    <t>Cerveza</t>
+  </si>
+  <si>
+    <t>American Gods en Ecatepec</t>
+  </si>
 </sst>
 </file>
 
@@ -1948,7 +1969,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D24" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2215,7 +2238,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>34882.729999999996</v>
+        <v>40690.229999999996</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -2360,7 +2383,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>292.5</v>
+        <v>0</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -2436,12 +2459,12 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>1292.5</v>
+        <v>1300</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
         <f>(SUM(R11:R499))-(SUM(E11:E500))</f>
-        <v>1000</v>
+        <v>1300</v>
       </c>
       <c r="Q7" s="58"/>
       <c r="R7" s="58"/>
@@ -2575,7 +2598,7 @@
       </c>
       <c r="L9" s="15">
         <f>SUM(L11:L501)</f>
-        <v>23800</v>
+        <v>29600</v>
       </c>
       <c r="N9" s="34" t="s">
         <v>51</v>
@@ -5901,13 +5924,13 @@
       </c>
       <c r="W41" s="43">
         <f t="shared" si="3"/>
-        <v>87.5</v>
+        <v>162.5</v>
       </c>
       <c r="X41" s="52">
         <v>120</v>
       </c>
       <c r="Y41" s="100">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="Z41" t="s">
         <v>151</v>
@@ -6832,19 +6855,35 @@
       <c r="D50" s="12"/>
       <c r="E50" s="14"/>
       <c r="G50" s="18"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="23"/>
+      <c r="H50" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="I50" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="J50" s="23">
+        <v>5300</v>
+      </c>
       <c r="K50" s="22"/>
       <c r="L50" s="20">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N50" s="37"/>
-      <c r="O50" s="37"/>
-      <c r="P50" s="37"/>
-      <c r="Q50" s="39"/>
-      <c r="R50" s="39"/>
+        <v>5300</v>
+      </c>
+      <c r="N50" s="38">
+        <v>43044</v>
+      </c>
+      <c r="O50" s="37" t="s">
+        <v>368</v>
+      </c>
+      <c r="P50" s="37" t="s">
+        <v>369</v>
+      </c>
+      <c r="Q50" s="39">
+        <v>150</v>
+      </c>
+      <c r="R50" s="39">
+        <v>300</v>
+      </c>
       <c r="T50" s="49">
         <v>43002</v>
       </c>
@@ -6912,13 +6951,19 @@
       <c r="D51" s="12"/>
       <c r="E51" s="14"/>
       <c r="G51" s="18"/>
-      <c r="H51" s="18"/>
-      <c r="I51" s="18"/>
-      <c r="J51" s="23"/>
+      <c r="H51" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I51" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="J51" s="23">
+        <v>500</v>
+      </c>
       <c r="K51" s="22"/>
       <c r="L51" s="20">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="N51" s="37"/>
       <c r="O51" s="37"/>
@@ -10611,7 +10656,7 @@
       </c>
       <c r="W90" s="43">
         <f t="shared" si="10"/>
-        <v>80</v>
+        <v>-127.5</v>
       </c>
       <c r="X90" s="52">
         <v>80</v>
@@ -10619,13 +10664,22 @@
       <c r="Y90" s="52"/>
       <c r="AA90" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>207.5</v>
+      </c>
+      <c r="AB90">
+        <v>100</v>
+      </c>
+      <c r="AC90" t="s">
+        <v>298</v>
+      </c>
+      <c r="AD90" t="s">
+        <v>370</v>
       </c>
       <c r="AE90">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="AF90">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AG90">
         <v>0</v>
@@ -10653,15 +10707,21 @@
       </c>
       <c r="AO90">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="AT90">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
+      <c r="AU90">
+        <v>1</v>
+      </c>
       <c r="AV90">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="AW90">
+        <v>12.5</v>
       </c>
     </row>
     <row r="91" spans="3:49" x14ac:dyDescent="0.25">
@@ -10688,19 +10748,32 @@
       <c r="U91" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="V91" s="51"/>
+      <c r="V91" s="51" t="s">
+        <v>372</v>
+      </c>
       <c r="W91" s="43">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X91" s="52"/>
+        <v>-10</v>
+      </c>
+      <c r="X91" s="52">
+        <v>120</v>
+      </c>
       <c r="Y91" s="52"/>
       <c r="AA91" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>130</v>
+      </c>
+      <c r="AB91">
+        <v>100</v>
+      </c>
+      <c r="AC91" t="s">
+        <v>275</v>
+      </c>
+      <c r="AD91" t="s">
+        <v>371</v>
       </c>
       <c r="AE91">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AF91">
         <v>0</v>
@@ -10731,15 +10804,18 @@
       </c>
       <c r="AO91">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AT91">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
+      <c r="AU91">
+        <v>2</v>
+      </c>
       <c r="AV91">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="3:49" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Practicas en R Shiny
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="375">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -1144,12 +1144,18 @@
   <si>
     <t>American Gods en Ecatepec</t>
   </si>
+  <si>
+    <t>Alejandro Celular Mamá</t>
+  </si>
+  <si>
+    <t>Ale celular</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1290,13 +1296,6 @@
     <font>
       <sz val="11"/>
       <color theme="7" tint="0.79998168889431442"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1496,7 +1495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1672,7 +1671,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1969,9 +1967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D24" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2164,7 +2160,7 @@
       </c>
       <c r="L3" s="26">
         <f>(SUM(C2,(E11:E500)))-(SUM((D11:D500),(C11:C500)))</f>
-        <v>9790.23</v>
+        <v>4490.2299999999996</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -2238,7 +2234,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>40690.229999999996</v>
+        <v>35510.229999999996</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -2383,7 +2379,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -2459,7 +2455,7 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>1300</v>
+        <v>1420</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
@@ -5004,7 +5000,15 @@
       </c>
     </row>
     <row r="33" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="C33" s="13"/>
+      <c r="A33" s="33">
+        <v>43045</v>
+      </c>
+      <c r="B33" t="s">
+        <v>373</v>
+      </c>
+      <c r="C33" s="13">
+        <v>5300</v>
+      </c>
       <c r="D33" s="12"/>
       <c r="E33" s="14"/>
       <c r="G33" s="60"/>
@@ -10493,7 +10497,7 @@
       <c r="AG88">
         <v>30</v>
       </c>
-      <c r="AH88" s="105">
+      <c r="AH88" s="13">
         <v>1800</v>
       </c>
       <c r="AI88">
@@ -10923,16 +10927,21 @@
       <c r="V93" s="51"/>
       <c r="W93" s="43">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X93" s="52"/>
+        <v>-5180</v>
+      </c>
+      <c r="X93" s="52">
+        <v>130</v>
+      </c>
       <c r="Y93" s="52"/>
       <c r="AA93" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AE93">
-        <v>0</v>
+        <v>5310</v>
+      </c>
+      <c r="AD93" t="s">
+        <v>374</v>
+      </c>
+      <c r="AE93" s="12">
+        <v>5300</v>
       </c>
       <c r="AF93">
         <v>0</v>
@@ -10963,15 +10972,18 @@
       </c>
       <c r="AO93">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AT93">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
+      <c r="AU93">
+        <v>2</v>
+      </c>
       <c r="AV93">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="3:49" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Gastos del martes brazalete nino
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="380">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -1150,6 +1150,21 @@
   <si>
     <t>Ale celular</t>
   </si>
+  <si>
+    <t>Amiguitos :D</t>
+  </si>
+  <si>
+    <t>Jaime invitó</t>
+  </si>
+  <si>
+    <t>Confirmando Palafox</t>
+  </si>
+  <si>
+    <t>Ensalada</t>
+  </si>
+  <si>
+    <t>Brazalete; Copias e Impresiones</t>
+  </si>
 </sst>
 </file>
 
@@ -1967,7 +1982,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2234,7 +2251,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>35510.229999999996</v>
+        <v>35769.229999999996</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -2282,7 +2299,7 @@
       </c>
       <c r="BA4" s="60">
         <f>(SUM((AP3:AP519)))-(SUM((AT3:AT519)))</f>
-        <v>-49</v>
+        <v>17</v>
       </c>
       <c r="BB4" s="60"/>
     </row>
@@ -2379,7 +2396,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>120</v>
+        <v>379</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -2455,7 +2472,7 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>1420</v>
+        <v>1679</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
@@ -6969,10 +6986,18 @@
         <f t="shared" si="7"/>
         <v>500</v>
       </c>
-      <c r="N51" s="37"/>
-      <c r="O51" s="37"/>
-      <c r="P51" s="37"/>
-      <c r="Q51" s="39"/>
+      <c r="N51" s="38">
+        <v>43046</v>
+      </c>
+      <c r="O51" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="P51" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q51" s="39">
+        <v>450</v>
+      </c>
       <c r="R51" s="39"/>
       <c r="T51" s="49">
         <v>43003</v>
@@ -7063,10 +7088,18 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="N52" s="37"/>
-      <c r="O52" s="37"/>
-      <c r="P52" s="37"/>
-      <c r="Q52" s="39"/>
+      <c r="N52" s="38">
+        <v>43047</v>
+      </c>
+      <c r="O52" s="37" t="s">
+        <v>278</v>
+      </c>
+      <c r="P52" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q52" s="39">
+        <v>300</v>
+      </c>
       <c r="R52" s="39"/>
       <c r="T52" s="49">
         <v>43004</v>
@@ -10378,7 +10411,7 @@
       </c>
       <c r="W87" s="43">
         <f t="shared" si="10"/>
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="X87" s="52">
         <v>120</v>
@@ -10386,7 +10419,7 @@
       <c r="Y87" s="52"/>
       <c r="AA87" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="AB87">
         <v>0</v>
@@ -10423,7 +10456,10 @@
       </c>
       <c r="AO87">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="AP87">
+        <v>50</v>
       </c>
       <c r="AQ87">
         <v>4</v>
@@ -10924,7 +10960,9 @@
       <c r="U93" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="V93" s="51"/>
+      <c r="V93" s="51" t="s">
+        <v>375</v>
+      </c>
       <c r="W93" s="43">
         <f t="shared" si="10"/>
         <v>-5180</v>
@@ -10936,6 +10974,12 @@
       <c r="AA93" s="53">
         <f t="shared" si="8"/>
         <v>5310</v>
+      </c>
+      <c r="AB93">
+        <v>0</v>
+      </c>
+      <c r="AC93" t="s">
+        <v>376</v>
       </c>
       <c r="AD93" t="s">
         <v>374</v>
@@ -11010,25 +11054,38 @@
       <c r="U94" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="V94" s="51"/>
+      <c r="V94" s="51" t="s">
+        <v>377</v>
+      </c>
       <c r="W94" s="43">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X94" s="52"/>
+        <v>-441</v>
+      </c>
+      <c r="X94" s="52">
+        <v>80</v>
+      </c>
       <c r="Y94" s="52"/>
       <c r="AA94" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>521</v>
+      </c>
+      <c r="AB94">
+        <v>50</v>
+      </c>
+      <c r="AC94" t="s">
+        <v>378</v>
+      </c>
+      <c r="AD94" t="s">
+        <v>379</v>
       </c>
       <c r="AE94">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="AF94">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AG94">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AH94">
         <v>0</v>
@@ -11053,15 +11110,27 @@
       </c>
       <c r="AO94">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="AP94">
+        <v>50</v>
+      </c>
+      <c r="AQ94">
+        <v>4</v>
+      </c>
+      <c r="AS94">
+        <v>2</v>
       </c>
       <c r="AT94">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="AU94">
+        <v>1</v>
       </c>
       <c r="AV94">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="3:49" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Gastos de mitad de semana
</commit_message>
<xml_diff>
--- a/Finanzas/4_Agosto_2017.xlsx
+++ b/Finanzas/4_Agosto_2017.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="382">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -1163,7 +1163,13 @@
     <t>Ensalada</t>
   </si>
   <si>
-    <t>Brazalete; Copias e Impresiones</t>
+    <t>Reunion Palafox</t>
+  </si>
+  <si>
+    <t>Papeles Jaime Forma 2</t>
+  </si>
+  <si>
+    <t>Brazalete; Copias e Impresiones; Coquita</t>
   </si>
 </sst>
 </file>
@@ -1983,7 +1989,7 @@
   <dimension ref="A1:BB963"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="AD95" sqref="AD95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2251,7 +2257,7 @@
       </c>
       <c r="N4" s="87">
         <f>SUM(L3,L9,N7)</f>
-        <v>35769.229999999996</v>
+        <v>35734.229999999996</v>
       </c>
       <c r="T4" s="49">
         <v>42956</v>
@@ -2299,7 +2305,7 @@
       </c>
       <c r="BA4" s="60">
         <f>(SUM((AP3:AP519)))-(SUM((AT3:AT519)))</f>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="BB4" s="60"/>
     </row>
@@ -2396,7 +2402,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q299),(W3:W500),(C11:C500)))-(SUM((R11:R499)))</f>
-        <v>379</v>
+        <v>344</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
@@ -2472,7 +2478,7 @@
       </c>
       <c r="N7" s="86">
         <f>SUM(P7,L6)</f>
-        <v>1679</v>
+        <v>1644</v>
       </c>
       <c r="O7" s="83"/>
       <c r="P7" s="82">
@@ -11059,7 +11065,7 @@
       </c>
       <c r="W94" s="43">
         <f t="shared" si="10"/>
-        <v>-441</v>
+        <v>-450</v>
       </c>
       <c r="X94" s="52">
         <v>80</v>
@@ -11067,7 +11073,7 @@
       <c r="Y94" s="52"/>
       <c r="AA94" s="53">
         <f t="shared" si="8"/>
-        <v>521</v>
+        <v>530</v>
       </c>
       <c r="AB94">
         <v>50</v>
@@ -11076,7 +11082,7 @@
         <v>378</v>
       </c>
       <c r="AD94" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="AE94">
         <v>400</v>
@@ -11088,7 +11094,7 @@
         <v>10</v>
       </c>
       <c r="AH94">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AI94">
         <v>0</v>
@@ -11157,16 +11163,26 @@
       <c r="U95" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="V95" s="51"/>
+      <c r="V95" s="51" t="s">
+        <v>379</v>
+      </c>
       <c r="W95" s="43">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X95" s="52"/>
+        <v>-70</v>
+      </c>
+      <c r="X95" s="52">
+        <v>80</v>
+      </c>
       <c r="Y95" s="52"/>
       <c r="AA95" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>150</v>
+      </c>
+      <c r="AB95">
+        <v>138</v>
+      </c>
+      <c r="AC95" t="s">
+        <v>150</v>
       </c>
       <c r="AE95">
         <v>0</v>
@@ -11200,15 +11216,21 @@
       </c>
       <c r="AO95">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="AS95">
+        <v>2</v>
       </c>
       <c r="AT95">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AV95">
         <f t="shared" si="11"/>
         <v>0</v>
+      </c>
+      <c r="AW95">
+        <v>12</v>
       </c>
     </row>
     <row r="96" spans="3:49" x14ac:dyDescent="0.25">
@@ -11235,16 +11257,20 @@
       <c r="U96" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="V96" s="51"/>
+      <c r="V96" s="51" t="s">
+        <v>380</v>
+      </c>
       <c r="W96" s="43">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X96" s="52"/>
+        <v>44</v>
+      </c>
+      <c r="X96" s="52">
+        <v>80</v>
+      </c>
       <c r="Y96" s="52"/>
       <c r="AA96" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="AE96">
         <v>0</v>
@@ -11278,15 +11304,27 @@
       </c>
       <c r="AO96">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>36</v>
+      </c>
+      <c r="AP96">
+        <v>20</v>
+      </c>
+      <c r="AQ96">
+        <v>2</v>
       </c>
       <c r="AT96">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="AU96">
+        <v>2</v>
       </c>
       <c r="AV96">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="AW96">
+        <v>6</v>
       </c>
     </row>
     <row r="97" spans="3:48" x14ac:dyDescent="0.25">

</xml_diff>